<commit_message>
tryna get a map
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myimam/Personal/15-For-50/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DE2CECE-9C3E-2441-9787-0E222BB627F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F071C76-A9B7-7446-8161-CFBA942A9DC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{A414920B-AA94-6E44-AEE3-541A17C74404}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="3" xr2:uid="{A414920B-AA94-6E44-AEE3-541A17C74404}"/>
   </bookViews>
   <sheets>
     <sheet name="Source" sheetId="1" r:id="rId1"/>
     <sheet name="Train" sheetId="2" r:id="rId2"/>
     <sheet name="Test" sheetId="4" r:id="rId3"/>
     <sheet name="Map" sheetId="5" r:id="rId4"/>
-    <sheet name="StateVT" sheetId="3" r:id="rId5"/>
+    <sheet name="latlong" sheetId="7" r:id="rId5"/>
+    <sheet name="StateVT" sheetId="3" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="164">
   <si>
     <t>E</t>
   </si>
@@ -316,15 +317,6 @@
     <t>https://transition.fec.gov/pubrec/fe2016/2016presgeresults.pdf</t>
   </si>
   <si>
-    <t> 0.00789745</t>
-  </si>
-  <si>
-    <t> 0.01236094</t>
-  </si>
-  <si>
-    <t> 0.03691014</t>
-  </si>
-  <si>
     <t>Biden v Trump: https://www.realclearpolitics.com/epolls/2020/president/us/general_election_trump_vs_biden-6247.html</t>
   </si>
   <si>
@@ -336,15 +328,244 @@
   <si>
     <t>National State Difference</t>
   </si>
+  <si>
+    <t>[0.00468663]</t>
+  </si>
+  <si>
+    <t>[-0.02185688]</t>
+  </si>
+  <si>
+    <t>[0.00159087]</t>
+  </si>
+  <si>
+    <t>[-0.03416853]</t>
+  </si>
+  <si>
+    <t>[0.07939428]</t>
+  </si>
+  <si>
+    <t>[-0.06415205]</t>
+  </si>
+  <si>
+    <t>[0.07269401]</t>
+  </si>
+  <si>
+    <t>[0.00644235]</t>
+  </si>
+  <si>
+    <t>[0.04646545]</t>
+  </si>
+  <si>
+    <t>[-0.02753968]</t>
+  </si>
+  <si>
+    <t>[-0.00280925]</t>
+  </si>
+  <si>
+    <t>[0.00619881]</t>
+  </si>
+  <si>
+    <t>Final Results</t>
+  </si>
+  <si>
+    <t>pulled from results.txt</t>
+  </si>
+  <si>
+    <t>Final Dem Electoral</t>
+  </si>
+  <si>
+    <t>Final Rep Electoral</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/public-data/docs/canonical/states_csv</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="170" formatCode="0.00000"/>
+    <numFmt numFmtId="173" formatCode="0.00000000000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -397,6 +618,18 @@
       <name val="Andale Mono"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -419,7 +652,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -435,11 +668,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -14276,7 +14519,7 @@
   <dimension ref="A1:BB97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J97"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34821,7 +35064,7 @@
   <dimension ref="A1:L97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34855,7 +35098,7 @@
         <v>27</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>72</v>
@@ -38648,17 +38891,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72ED6E0E-4E9F-5F4A-8B62-0E820538F7A5}">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="12" customWidth="1"/>
-    <col min="8" max="12" width="10.83203125" style="12"/>
+    <col min="7" max="7" width="13.33203125" style="14" customWidth="1"/>
+    <col min="8" max="12" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="51" x14ac:dyDescent="0.2">
@@ -38680,20 +38923,20 @@
       <c r="F1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>90</v>
+      <c r="I1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -38716,25 +38959,25 @@
       <c r="F2" s="2">
         <v>0.14699999999999999</v>
       </c>
-      <c r="G2" s="13">
-        <v>1.6824430000000001E-2</v>
-      </c>
-      <c r="H2" s="11">
+      <c r="G2" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="13">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="13">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="13">
         <v>0.04</v>
       </c>
-      <c r="K2" s="11">
-        <f>I2-J2</f>
-        <v>1.8999999999999996E-2</v>
-      </c>
-      <c r="L2" s="12">
+      <c r="K2" s="13">
+        <f>J2-I2</f>
+        <v>-1.8999999999999996E-2</v>
+      </c>
+      <c r="L2" s="14" t="e">
         <f>G2+K2</f>
-        <v>3.5824429999999997E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>74</v>
@@ -38760,24 +39003,25 @@
       <c r="F3" s="2">
         <v>0.14699999999999999</v>
       </c>
-      <c r="G3" s="13">
-        <v>-1.442001E-2</v>
-      </c>
-      <c r="H3" s="11">
+      <c r="G3" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="13">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="13">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="13">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="K3" s="11">
-        <v>-2.8410716149803276E-2</v>
-      </c>
-      <c r="L3" s="12">
+      <c r="K3" s="13">
+        <f t="shared" ref="K3:K13" si="1">J3-I3</f>
+        <v>-2.0999999999999998E-2</v>
+      </c>
+      <c r="L3" s="14" t="e">
         <f>G3+K3</f>
-        <v>-4.283072614980328E-2</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -38800,27 +39044,28 @@
       <c r="F4" s="2">
         <v>0.14699999999999999</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="13">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="I4" s="13">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="J4" s="13">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="K4" s="13">
+        <f t="shared" si="1"/>
+        <v>-1.4999999999999999E-2</v>
+      </c>
+      <c r="L4" s="14">
+        <f>0.000789745+K4</f>
+        <v>-1.4210255E-2</v>
+      </c>
+      <c r="Q4" t="s">
         <v>84</v>
-      </c>
-      <c r="H4" s="11">
-        <v>2.0899999999999998E-2</v>
-      </c>
-      <c r="I4" s="11">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="J4" s="11">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="K4" s="11">
-        <v>-2.3253364339230961E-2</v>
-      </c>
-      <c r="L4" s="12">
-        <f>0.000789745+K4</f>
-        <v>-2.246361933923096E-2</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -38843,24 +39088,25 @@
       <c r="F5" s="2">
         <v>0.14699999999999999</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="H5" s="11">
+      <c r="G5" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="13">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="13">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="13">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="K5" s="11">
-        <v>-3.3276709455509625E-2</v>
-      </c>
-      <c r="L5" s="12">
+      <c r="K5" s="13">
+        <f t="shared" si="1"/>
+        <v>-5.4999999999999993E-2</v>
+      </c>
+      <c r="L5" s="14">
         <f>0.01236094+K5</f>
-        <v>-2.0915769455509624E-2</v>
+        <v>-4.2639059999999993E-2</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -38883,22 +39129,25 @@
       <c r="F6" s="2">
         <v>0.14699999999999999</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="H6" s="11">
+      <c r="G6" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="13">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="13">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11">
-        <v>3.2766667453648729E-2</v>
-      </c>
-      <c r="L6" s="12">
+      <c r="J6" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="K6" s="13">
+        <f t="shared" si="1"/>
+        <v>4.1000000000000009E-2</v>
+      </c>
+      <c r="L6" s="14">
         <f>0.03691014+K6</f>
-        <v>6.9676807453648737E-2</v>
+        <v>7.7910140000000017E-2</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -38921,22 +39170,25 @@
       <c r="F7" s="2">
         <v>0.14699999999999999</v>
       </c>
-      <c r="G7" s="13">
-        <v>3.9141889999999999E-2</v>
-      </c>
-      <c r="H7" s="11">
+      <c r="G7" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="13">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="13">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11">
-        <v>-0.1221709569024069</v>
-      </c>
-      <c r="L7" s="12">
+      <c r="J7" s="13">
+        <v>-4.8000000000000001E-2</v>
+      </c>
+      <c r="K7" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.107</v>
+      </c>
+      <c r="L7" s="14" t="e">
         <f>G7+K7</f>
-        <v>-8.3029066902406898E-2</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -38959,22 +39211,25 @@
       <c r="F8" s="2">
         <v>0.14699999999999999</v>
       </c>
-      <c r="G8" s="13">
-        <v>3.4339599999999998E-3</v>
-      </c>
-      <c r="H8" s="11">
+      <c r="G8" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" s="13">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="13">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11">
-        <v>-4.2628613276930946E-3</v>
-      </c>
-      <c r="L8" s="12">
+      <c r="J8" s="13">
+        <v>0.12</v>
+      </c>
+      <c r="K8" s="13">
+        <f t="shared" si="1"/>
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="L8" s="14" t="e">
         <f>G8+K8</f>
-        <v>-8.2890132769309482E-4</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -38997,22 +39252,25 @@
       <c r="F9" s="2">
         <v>0.14699999999999999</v>
       </c>
-      <c r="G9" s="13">
-        <v>1.9056179999999999E-2</v>
-      </c>
-      <c r="H9" s="11">
+      <c r="G9" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="13">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="13">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11">
-        <v>4.974188399703993E-3</v>
-      </c>
-      <c r="L9" s="12">
+      <c r="J9" s="13">
+        <v>0.04</v>
+      </c>
+      <c r="K9" s="13">
+        <f t="shared" si="1"/>
+        <v>-1.8999999999999996E-2</v>
+      </c>
+      <c r="L9" s="14" t="e">
         <f>G9+K9</f>
-        <v>2.4030368399703992E-2</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="34" x14ac:dyDescent="0.2">
@@ -39035,22 +39293,25 @@
       <c r="F10" s="2">
         <v>0.14699999999999999</v>
       </c>
-      <c r="G10" s="13">
-        <v>6.3691090000000006E-2</v>
-      </c>
-      <c r="H10" s="11">
+      <c r="G10" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="H10" s="13">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="13">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11">
-        <v>-1.6959431152385945E-2</v>
-      </c>
-      <c r="L10" s="12">
+      <c r="J10" s="13">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K10" s="13">
+        <f t="shared" si="1"/>
+        <v>-1.3999999999999999E-2</v>
+      </c>
+      <c r="L10" s="14" t="e">
         <f>G10+K10</f>
-        <v>4.6731658847614058E-2</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -39073,22 +39334,25 @@
       <c r="F11" s="2">
         <v>0.14699999999999999</v>
       </c>
-      <c r="G11" s="13">
-        <v>-1.665175E-2</v>
-      </c>
-      <c r="H11" s="11">
+      <c r="G11" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" s="13">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="13">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11">
-        <v>-5.8974916074374328E-2</v>
-      </c>
-      <c r="L11" s="12">
+      <c r="J11" s="13">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="K11" s="13">
+        <f t="shared" si="1"/>
+        <v>-2.4999999999999994E-2</v>
+      </c>
+      <c r="L11" s="14" t="e">
         <f>G11+K11</f>
-        <v>-7.5626666074374321E-2</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -39111,24 +39375,25 @@
       <c r="F12" s="2">
         <v>0.14699999999999999</v>
       </c>
-      <c r="G12" s="13">
-        <v>2.3519669999999999E-2</v>
-      </c>
-      <c r="H12" s="11">
+      <c r="G12" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="H12" s="13">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="13">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="13">
         <v>2.7E-2</v>
       </c>
-      <c r="K12" s="11">
-        <v>-2.9059780760594296E-2</v>
-      </c>
-      <c r="L12" s="12">
+      <c r="K12" s="13">
+        <f t="shared" si="1"/>
+        <v>-3.2000000000000001E-2</v>
+      </c>
+      <c r="L12" s="14" t="e">
         <f>G12+K12</f>
-        <v>-5.5401107605942967E-3</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -39151,23 +39416,62 @@
       <c r="F13" s="2">
         <v>0.14699999999999999</v>
       </c>
-      <c r="G13" s="13">
-        <v>-9.95652E-3</v>
-      </c>
-      <c r="H13" s="11">
+      <c r="G13" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="13">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="13">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11">
-        <v>3.5627525543094007E-2</v>
-      </c>
-      <c r="L13" s="12">
+      <c r="J13" s="13">
+        <v>6.3E-2</v>
+      </c>
+      <c r="K13" s="13">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="L13" s="14" t="e">
         <f>G13+K13</f>
-        <v>2.5671005543094007E-2</v>
-      </c>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I20" s="11"/>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I23" s="11"/>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I24" s="11"/>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I25" s="11"/>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I26" s="11"/>
+    </row>
+    <row r="27" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I27" s="11"/>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I28" s="11"/>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I29" s="11"/>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I30" s="11"/>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I31" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -39179,18 +39483,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A12BA6E-D220-514B-B360-4F43E4765A8F}">
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="15" width="10.83203125" style="2"/>
+    <col min="16" max="16" width="12.6640625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>79</v>
       </c>
@@ -39204,24 +39511,39 @@
         <v>77</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="K1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q1" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="str" cm="1">
-        <f t="array" ref="A2">_xlfn.IFS(ISBLANK(D2),"SwingState",D2&lt;3,"R",D2&gt;3,"D")</f>
+        <f t="array" ref="A2">_xlfn.IFS(ISBLANK(D2),"SwingState",D2 = 3, "SwingState",D2=4,"SwingState",D2&lt;3,"R",D2&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -39233,26 +39555,44 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="19">
+        <v>32.318230999999997</v>
+      </c>
+      <c r="F2" s="19">
+        <v>-86.902298000000002</v>
+      </c>
+      <c r="G2" s="2">
         <f>COUNTBLANK(D2:D51)</f>
-        <v>12</v>
-      </c>
-      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
         <f>SUMIF(A2:A52,"D",C2:C52)</f>
         <v>191</v>
       </c>
-      <c r="G2" s="2">
+      <c r="I2" s="2">
         <f>SUMIF(A2:A52,"R",C2:C52)</f>
         <v>194</v>
       </c>
-      <c r="H2" s="2">
-        <f>538-G2-F2</f>
+      <c r="J2" s="2">
+        <f>538-I2-H2</f>
         <v>153</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="K2" s="2" t="str" cm="1">
+        <f t="array" ref="K2">_xlfn.IFS(ISBLANK(D2),"SwingState",D2 = 3, "Model Rep",D2=4,"Model Dem",D2&lt;3,"R",D2&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="L2" s="2">
+        <f>SUMIF(K2:K52,"D",C2:C52)+SUMIF(K2:K52,"Model Dem",C2:C52)</f>
+        <v>267</v>
+      </c>
+      <c r="M2" s="2">
+        <f>SUMIF(K2:K52,"R",C2:C52)+SUMIF(K2:K52,"Model Rep",C2:C52)</f>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="str" cm="1">
-        <f t="array" ref="A3">_xlfn.IFS(ISBLANK(D3),"SwingState",D3&lt;3,"R",D3&gt;3,"D")</f>
+        <f t="array" ref="A3">_xlfn.IFS(ISBLANK(D3),"SwingState",D3 = 3, "SwingState",D3=4,"SwingState",D3&lt;3,"R",D3&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -39264,10 +39604,20 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="E3" s="19">
+        <v>63.588752999999997</v>
+      </c>
+      <c r="F3" s="19">
+        <v>-154.49306200000001</v>
+      </c>
+      <c r="K3" s="2" t="str" cm="1">
+        <f t="array" ref="K3">_xlfn.IFS(ISBLANK(D3),"SwingState",D3 = 3, "Model Rep",D3=4,"Model Dem",D3&lt;3,"R",D3&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="str" cm="1">
-        <f t="array" ref="A4">_xlfn.IFS(ISBLANK(D4),"SwingState",D4&lt;3,"R",D4&gt;3,"D")</f>
+        <f t="array" ref="A4">_xlfn.IFS(ISBLANK(D4),"SwingState",D4 = 3, "SwingState",D4=4,"SwingState",D4&lt;3,"R",D4&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -39279,10 +39629,24 @@
       <c r="D4" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="E4" s="19">
+        <v>34.048927999999997</v>
+      </c>
+      <c r="F4" s="19">
+        <v>-111.09373100000001</v>
+      </c>
+      <c r="K4" s="2" t="str" cm="1">
+        <f t="array" ref="K4">_xlfn.IFS(ISBLANK(D4),"SwingState",D4 = 3, "Model Rep",D4=4,"Model Dem",D4&lt;3,"R",D4&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
+    </row>
+    <row r="5" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="str" cm="1">
-        <f t="array" ref="A5">_xlfn.IFS(ISBLANK(D5),"SwingState",D5&lt;3,"R",D5&gt;3,"D")</f>
+        <f t="array" ref="A5">_xlfn.IFS(ISBLANK(D5),"SwingState",D5 = 3, "SwingState",D5=4,"SwingState",D5&lt;3,"R",D5&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -39294,10 +39658,30 @@
       <c r="D5" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="E5" s="19">
+        <v>35.201050000000002</v>
+      </c>
+      <c r="F5" s="19">
+        <v>-91.831833000000003</v>
+      </c>
+      <c r="K5" s="2" t="str" cm="1">
+        <f t="array" ref="K5">_xlfn.IFS(ISBLANK(D5),"SwingState",D5 = 3, "Model Rep",D5=4,"Model Dem",D5&lt;3,"R",D5&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+    </row>
+    <row r="6" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="str" cm="1">
-        <f t="array" ref="A6">_xlfn.IFS(ISBLANK(D6),"SwingState",D6&lt;3,"R",D6&gt;3,"D")</f>
+        <f t="array" ref="A6">_xlfn.IFS(ISBLANK(D6),"SwingState",D6 = 3, "SwingState",D6=4,"SwingState",D6&lt;3,"R",D6&gt;3,"D")</f>
         <v>D</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -39309,10 +39693,30 @@
       <c r="D6" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="E6" s="19">
+        <v>36.778261000000001</v>
+      </c>
+      <c r="F6" s="19">
+        <v>-119.41793199999999</v>
+      </c>
+      <c r="K6" s="2" t="str" cm="1">
+        <f t="array" ref="K6">_xlfn.IFS(ISBLANK(D6),"SwingState",D6 = 3, "Model Rep",D6=4,"Model Dem",D6&lt;3,"R",D6&gt;3,"D")</f>
+        <v>D</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="16">
+        <v>4.6866299999999998E-3</v>
+      </c>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+    </row>
+    <row r="7" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="str" cm="1">
-        <f t="array" ref="A7">_xlfn.IFS(ISBLANK(D7),"SwingState",D7&lt;3,"R",D7&gt;3,"D")</f>
+        <f t="array" ref="A7">_xlfn.IFS(ISBLANK(D7),"SwingState",D7 = 3, "SwingState",D7=4,"SwingState",D7&lt;3,"R",D7&gt;3,"D")</f>
         <v>SwingState</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -39321,10 +39725,33 @@
       <c r="C7" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="D7" s="2">
+        <v>4</v>
+      </c>
+      <c r="E7" s="19">
+        <v>39.550051000000003</v>
+      </c>
+      <c r="F7" s="19">
+        <v>-105.782067</v>
+      </c>
+      <c r="K7" s="2" t="str" cm="1">
+        <f t="array" ref="K7">_xlfn.IFS(ISBLANK(D7),"SwingState",D7 = 3, "Model Rep",D7=4,"Model Dem",D7&lt;3,"R",D7&gt;3,"D")</f>
+        <v>Model Dem</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q7" s="16">
+        <v>-2.1856879999999999E-2</v>
+      </c>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+    </row>
+    <row r="8" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="str" cm="1">
-        <f t="array" ref="A8">_xlfn.IFS(ISBLANK(D8),"SwingState",D8&lt;3,"R",D8&gt;3,"D")</f>
+        <f t="array" ref="A8">_xlfn.IFS(ISBLANK(D8),"SwingState",D8 = 3, "SwingState",D8=4,"SwingState",D8&lt;3,"R",D8&gt;3,"D")</f>
         <v>D</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -39336,10 +39763,30 @@
       <c r="D8" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="E8" s="19">
+        <v>41.603220999999998</v>
+      </c>
+      <c r="F8" s="19">
+        <v>-73.087749000000002</v>
+      </c>
+      <c r="K8" s="2" t="str" cm="1">
+        <f t="array" ref="K8">_xlfn.IFS(ISBLANK(D8),"SwingState",D8 = 3, "Model Rep",D8=4,"Model Dem",D8&lt;3,"R",D8&gt;3,"D")</f>
+        <v>D</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="16">
+        <v>1.5908700000000001E-3</v>
+      </c>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+    </row>
+    <row r="9" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="str" cm="1">
-        <f t="array" ref="A9">_xlfn.IFS(ISBLANK(D9),"SwingState",D9&lt;3,"R",D9&gt;3,"D")</f>
+        <f t="array" ref="A9">_xlfn.IFS(ISBLANK(D9),"SwingState",D9 = 3, "SwingState",D9=4,"SwingState",D9&lt;3,"R",D9&gt;3,"D")</f>
         <v>D</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -39351,10 +39798,32 @@
       <c r="D9" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="29" x14ac:dyDescent="0.2">
+      <c r="E9" s="19">
+        <v>38.910831999999999</v>
+      </c>
+      <c r="F9" s="19">
+        <v>-75.527670000000001</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="K9" s="2" t="str" cm="1">
+        <f t="array" ref="K9">_xlfn.IFS(ISBLANK(D9),"SwingState",D9 = 3, "Model Rep",D9=4,"Model Dem",D9&lt;3,"R",D9&gt;3,"D")</f>
+        <v>D</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q9" s="16">
+        <v>-3.4168530000000003E-2</v>
+      </c>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="17"/>
+    </row>
+    <row r="10" spans="1:24" ht="29" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="str" cm="1">
-        <f t="array" ref="A10">_xlfn.IFS(ISBLANK(D10),"SwingState",D10&lt;3,"R",D10&gt;3,"D")</f>
+        <f t="array" ref="A10">_xlfn.IFS(ISBLANK(D10),"SwingState",D10 = 3, "SwingState",D10=4,"SwingState",D10&lt;3,"R",D10&gt;3,"D")</f>
         <v>D</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -39366,10 +39835,30 @@
       <c r="D10" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="E10" s="19">
+        <v>38.905985000000001</v>
+      </c>
+      <c r="F10" s="19">
+        <v>-77.033417999999998</v>
+      </c>
+      <c r="K10" s="2" t="str" cm="1">
+        <f t="array" ref="K10">_xlfn.IFS(ISBLANK(D10),"SwingState",D10 = 3, "Model Rep",D10=4,"Model Dem",D10&lt;3,"R",D10&gt;3,"D")</f>
+        <v>D</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q10" s="16">
+        <v>7.9394279999999998E-2</v>
+      </c>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+    </row>
+    <row r="11" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="str" cm="1">
-        <f t="array" ref="A11">_xlfn.IFS(ISBLANK(D11),"SwingState",D11&lt;3,"R",D11&gt;3,"D")</f>
+        <f t="array" ref="A11">_xlfn.IFS(ISBLANK(D11),"SwingState",D11 = 3, "SwingState",D11=4,"SwingState",D11&lt;3,"R",D11&gt;3,"D")</f>
         <v>SwingState</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -39378,10 +39867,33 @@
       <c r="C11" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="19">
+        <v>27.664826999999999</v>
+      </c>
+      <c r="F11" s="19">
+        <v>-81.515754000000001</v>
+      </c>
+      <c r="K11" s="2" t="str" cm="1">
+        <f t="array" ref="K11">_xlfn.IFS(ISBLANK(D11),"SwingState",D11 = 3, "Model Rep",D11=4,"Model Dem",D11&lt;3,"R",D11&gt;3,"D")</f>
+        <v>Model Rep</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q11" s="16">
+        <v>-6.4152050000000002E-2</v>
+      </c>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+    </row>
+    <row r="12" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="str" cm="1">
-        <f t="array" ref="A12">_xlfn.IFS(ISBLANK(D12),"SwingState",D12&lt;3,"R",D12&gt;3,"D")</f>
+        <f t="array" ref="A12">_xlfn.IFS(ISBLANK(D12),"SwingState",D12 = 3, "SwingState",D12=4,"SwingState",D12&lt;3,"R",D12&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -39393,10 +39905,30 @@
       <c r="D12" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="E12" s="19">
+        <v>32.157435</v>
+      </c>
+      <c r="F12" s="19">
+        <v>-82.907122999999999</v>
+      </c>
+      <c r="K12" s="2" t="str" cm="1">
+        <f t="array" ref="K12">_xlfn.IFS(ISBLANK(D12),"SwingState",D12 = 3, "Model Rep",D12=4,"Model Dem",D12&lt;3,"R",D12&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q12" s="16">
+        <v>7.2694010000000003E-2</v>
+      </c>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
+    </row>
+    <row r="13" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="str" cm="1">
-        <f t="array" ref="A13">_xlfn.IFS(ISBLANK(D13),"SwingState",D13&lt;3,"R",D13&gt;3,"D")</f>
+        <f t="array" ref="A13">_xlfn.IFS(ISBLANK(D13),"SwingState",D13 = 3, "SwingState",D13=4,"SwingState",D13&lt;3,"R",D13&gt;3,"D")</f>
         <v>D</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -39408,10 +39940,30 @@
       <c r="D13" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="E13" s="19">
+        <v>19.898682000000001</v>
+      </c>
+      <c r="F13" s="19">
+        <v>-155.66585699999999</v>
+      </c>
+      <c r="K13" s="2" t="str" cm="1">
+        <f t="array" ref="K13">_xlfn.IFS(ISBLANK(D13),"SwingState",D13 = 3, "Model Rep",D13=4,"Model Dem",D13&lt;3,"R",D13&gt;3,"D")</f>
+        <v>D</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q13" s="16">
+        <v>6.4423500000000003E-3</v>
+      </c>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="17"/>
+    </row>
+    <row r="14" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="str" cm="1">
-        <f t="array" ref="A14">_xlfn.IFS(ISBLANK(D14),"SwingState",D14&lt;3,"R",D14&gt;3,"D")</f>
+        <f t="array" ref="A14">_xlfn.IFS(ISBLANK(D14),"SwingState",D14 = 3, "SwingState",D14=4,"SwingState",D14&lt;3,"R",D14&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -39423,10 +39975,30 @@
       <c r="D14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="E14" s="19">
+        <v>44.068201999999999</v>
+      </c>
+      <c r="F14" s="19">
+        <v>-114.742041</v>
+      </c>
+      <c r="K14" s="2" t="str" cm="1">
+        <f t="array" ref="K14">_xlfn.IFS(ISBLANK(D14),"SwingState",D14 = 3, "Model Rep",D14=4,"Model Dem",D14&lt;3,"R",D14&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q14" s="16">
+        <v>4.6465449999999998E-2</v>
+      </c>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+    </row>
+    <row r="15" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="str" cm="1">
-        <f t="array" ref="A15">_xlfn.IFS(ISBLANK(D15),"SwingState",D15&lt;3,"R",D15&gt;3,"D")</f>
+        <f t="array" ref="A15">_xlfn.IFS(ISBLANK(D15),"SwingState",D15 = 3, "SwingState",D15=4,"SwingState",D15&lt;3,"R",D15&gt;3,"D")</f>
         <v>D</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -39438,10 +40010,30 @@
       <c r="D15" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="E15" s="19">
+        <v>40.633125</v>
+      </c>
+      <c r="F15" s="19">
+        <v>-89.398527999999999</v>
+      </c>
+      <c r="K15" s="2" t="str" cm="1">
+        <f t="array" ref="K15">_xlfn.IFS(ISBLANK(D15),"SwingState",D15 = 3, "Model Rep",D15=4,"Model Dem",D15&lt;3,"R",D15&gt;3,"D")</f>
+        <v>D</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q15" s="16">
+        <v>-2.753968E-2</v>
+      </c>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+    </row>
+    <row r="16" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="str" cm="1">
-        <f t="array" ref="A16">_xlfn.IFS(ISBLANK(D16),"SwingState",D16&lt;3,"R",D16&gt;3,"D")</f>
+        <f t="array" ref="A16">_xlfn.IFS(ISBLANK(D16),"SwingState",D16 = 3, "SwingState",D16=4,"SwingState",D16&lt;3,"R",D16&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B16" s="10" t="s">
@@ -39453,10 +40045,30 @@
       <c r="D16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E16" s="19">
+        <v>40.551217000000001</v>
+      </c>
+      <c r="F16" s="19">
+        <v>-85.602363999999994</v>
+      </c>
+      <c r="K16" s="2" t="str" cm="1">
+        <f t="array" ref="K16">_xlfn.IFS(ISBLANK(D16),"SwingState",D16 = 3, "Model Rep",D16=4,"Model Dem",D16&lt;3,"R",D16&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q16" s="16">
+        <v>-2.8092500000000001E-3</v>
+      </c>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+    </row>
+    <row r="17" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="str" cm="1">
-        <f t="array" ref="A17">_xlfn.IFS(ISBLANK(D17),"SwingState",D17&lt;3,"R",D17&gt;3,"D")</f>
+        <f t="array" ref="A17">_xlfn.IFS(ISBLANK(D17),"SwingState",D17 = 3, "SwingState",D17=4,"SwingState",D17&lt;3,"R",D17&gt;3,"D")</f>
         <v>SwingState</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -39465,10 +40077,33 @@
       <c r="C17" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D17" s="2">
+        <v>3</v>
+      </c>
+      <c r="E17" s="19">
+        <v>41.878003</v>
+      </c>
+      <c r="F17" s="19">
+        <v>-93.097701999999998</v>
+      </c>
+      <c r="K17" s="2" t="str" cm="1">
+        <f t="array" ref="K17">_xlfn.IFS(ISBLANK(D17),"SwingState",D17 = 3, "Model Rep",D17=4,"Model Dem",D17&lt;3,"R",D17&gt;3,"D")</f>
+        <v>Model Rep</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q17" s="16">
+        <v>6.1988099999999999E-3</v>
+      </c>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="17"/>
+    </row>
+    <row r="18" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="str" cm="1">
-        <f t="array" ref="A18">_xlfn.IFS(ISBLANK(D18),"SwingState",D18&lt;3,"R",D18&gt;3,"D")</f>
+        <f t="array" ref="A18">_xlfn.IFS(ISBLANK(D18),"SwingState",D18 = 3, "SwingState",D18=4,"SwingState",D18&lt;3,"R",D18&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B18" s="10" t="s">
@@ -39480,10 +40115,25 @@
       <c r="D18" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E18" s="19">
+        <v>39.011901999999999</v>
+      </c>
+      <c r="F18" s="19">
+        <v>-98.484245999999999</v>
+      </c>
+      <c r="K18" s="2" t="str" cm="1">
+        <f t="array" ref="K18">_xlfn.IFS(ISBLANK(D18),"SwingState",D18 = 3, "Model Rep",D18=4,"Model Dem",D18&lt;3,"R",D18&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="Q18" s="12"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
+    </row>
+    <row r="19" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="str" cm="1">
-        <f t="array" ref="A19">_xlfn.IFS(ISBLANK(D19),"SwingState",D19&lt;3,"R",D19&gt;3,"D")</f>
+        <f t="array" ref="A19">_xlfn.IFS(ISBLANK(D19),"SwingState",D19 = 3, "SwingState",D19=4,"SwingState",D19&lt;3,"R",D19&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -39495,10 +40145,24 @@
       <c r="D19" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E19" s="19">
+        <v>37.839333000000003</v>
+      </c>
+      <c r="F19" s="19">
+        <v>-84.270017999999993</v>
+      </c>
+      <c r="K19" s="2" t="str" cm="1">
+        <f t="array" ref="K19">_xlfn.IFS(ISBLANK(D19),"SwingState",D19 = 3, "Model Rep",D19=4,"Model Dem",D19&lt;3,"R",D19&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+    </row>
+    <row r="20" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="str" cm="1">
-        <f t="array" ref="A20">_xlfn.IFS(ISBLANK(D20),"SwingState",D20&lt;3,"R",D20&gt;3,"D")</f>
+        <f t="array" ref="A20">_xlfn.IFS(ISBLANK(D20),"SwingState",D20 = 3, "SwingState",D20=4,"SwingState",D20&lt;3,"R",D20&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B20" s="10" t="s">
@@ -39510,10 +40174,24 @@
       <c r="D20" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E20" s="19">
+        <v>31.244823</v>
+      </c>
+      <c r="F20" s="19">
+        <v>-92.145024000000006</v>
+      </c>
+      <c r="K20" s="2" t="str" cm="1">
+        <f t="array" ref="K20">_xlfn.IFS(ISBLANK(D20),"SwingState",D20 = 3, "Model Rep",D20=4,"Model Dem",D20&lt;3,"R",D20&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="17"/>
+    </row>
+    <row r="21" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="str" cm="1">
-        <f t="array" ref="A21">_xlfn.IFS(ISBLANK(D21),"SwingState",D21&lt;3,"R",D21&gt;3,"D")</f>
+        <f t="array" ref="A21">_xlfn.IFS(ISBLANK(D21),"SwingState",D21 = 3, "SwingState",D21=4,"SwingState",D21&lt;3,"R",D21&gt;3,"D")</f>
         <v>D</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -39525,10 +40203,24 @@
       <c r="D21" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E21" s="19">
+        <v>45.253782999999999</v>
+      </c>
+      <c r="F21" s="19">
+        <v>-69.445469000000003</v>
+      </c>
+      <c r="K21" s="2" t="str" cm="1">
+        <f t="array" ref="K21">_xlfn.IFS(ISBLANK(D21),"SwingState",D21 = 3, "Model Rep",D21=4,"Model Dem",D21&lt;3,"R",D21&gt;3,"D")</f>
+        <v>D</v>
+      </c>
+      <c r="U21" s="17"/>
+      <c r="V21" s="17"/>
+      <c r="W21" s="17"/>
+      <c r="X21" s="17"/>
+    </row>
+    <row r="22" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="str" cm="1">
-        <f t="array" ref="A22">_xlfn.IFS(ISBLANK(D22),"SwingState",D22&lt;3,"R",D22&gt;3,"D")</f>
+        <f t="array" ref="A22">_xlfn.IFS(ISBLANK(D22),"SwingState",D22 = 3, "SwingState",D22=4,"SwingState",D22&lt;3,"R",D22&gt;3,"D")</f>
         <v>D</v>
       </c>
       <c r="B22" s="10" t="s">
@@ -39540,10 +40232,24 @@
       <c r="D22" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="E22" s="19">
+        <v>39.045755</v>
+      </c>
+      <c r="F22" s="19">
+        <v>-76.641271000000003</v>
+      </c>
+      <c r="K22" s="2" t="str" cm="1">
+        <f t="array" ref="K22">_xlfn.IFS(ISBLANK(D22),"SwingState",D22 = 3, "Model Rep",D22=4,"Model Dem",D22&lt;3,"R",D22&gt;3,"D")</f>
+        <v>D</v>
+      </c>
+      <c r="U22" s="17"/>
+      <c r="V22" s="17"/>
+      <c r="W22" s="17"/>
+      <c r="X22" s="17"/>
+    </row>
+    <row r="23" spans="1:24" ht="29" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="str" cm="1">
-        <f t="array" ref="A23">_xlfn.IFS(ISBLANK(D23),"SwingState",D23&lt;3,"R",D23&gt;3,"D")</f>
+        <f t="array" ref="A23">_xlfn.IFS(ISBLANK(D23),"SwingState",D23 = 3, "SwingState",D23=4,"SwingState",D23&lt;3,"R",D23&gt;3,"D")</f>
         <v>D</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -39555,10 +40261,24 @@
       <c r="D23" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E23" s="19">
+        <v>42.407210999999997</v>
+      </c>
+      <c r="F23" s="19">
+        <v>-71.382436999999996</v>
+      </c>
+      <c r="K23" s="2" t="str" cm="1">
+        <f t="array" ref="K23">_xlfn.IFS(ISBLANK(D23),"SwingState",D23 = 3, "Model Rep",D23=4,"Model Dem",D23&lt;3,"R",D23&gt;3,"D")</f>
+        <v>D</v>
+      </c>
+      <c r="U23" s="17"/>
+      <c r="V23" s="17"/>
+      <c r="W23" s="17"/>
+      <c r="X23" s="17"/>
+    </row>
+    <row r="24" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="str" cm="1">
-        <f t="array" ref="A24">_xlfn.IFS(ISBLANK(D24),"SwingState",D24&lt;3,"R",D24&gt;3,"D")</f>
+        <f t="array" ref="A24">_xlfn.IFS(ISBLANK(D24),"SwingState",D24 = 3, "SwingState",D24=4,"SwingState",D24&lt;3,"R",D24&gt;3,"D")</f>
         <v>SwingState</v>
       </c>
       <c r="B24" s="10" t="s">
@@ -39567,10 +40287,27 @@
       <c r="C24" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D24" s="2">
+        <v>4</v>
+      </c>
+      <c r="E24" s="19">
+        <v>44.314844000000001</v>
+      </c>
+      <c r="F24" s="19">
+        <v>-85.602363999999994</v>
+      </c>
+      <c r="K24" s="2" t="str" cm="1">
+        <f t="array" ref="K24">_xlfn.IFS(ISBLANK(D24),"SwingState",D24 = 3, "Model Rep",D24=4,"Model Dem",D24&lt;3,"R",D24&gt;3,"D")</f>
+        <v>Model Dem</v>
+      </c>
+      <c r="U24" s="17"/>
+      <c r="V24" s="17"/>
+      <c r="W24" s="17"/>
+      <c r="X24" s="17"/>
+    </row>
+    <row r="25" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="str" cm="1">
-        <f t="array" ref="A25">_xlfn.IFS(ISBLANK(D25),"SwingState",D25&lt;3,"R",D25&gt;3,"D")</f>
+        <f t="array" ref="A25">_xlfn.IFS(ISBLANK(D25),"SwingState",D25 = 3, "SwingState",D25=4,"SwingState",D25&lt;3,"R",D25&gt;3,"D")</f>
         <v>SwingState</v>
       </c>
       <c r="B25" s="10" t="s">
@@ -39579,10 +40316,27 @@
       <c r="C25" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D25" s="2">
+        <v>4</v>
+      </c>
+      <c r="E25" s="19">
+        <v>46.729553000000003</v>
+      </c>
+      <c r="F25" s="19">
+        <v>-94.685900000000004</v>
+      </c>
+      <c r="K25" s="2" t="str" cm="1">
+        <f t="array" ref="K25">_xlfn.IFS(ISBLANK(D25),"SwingState",D25 = 3, "Model Rep",D25=4,"Model Dem",D25&lt;3,"R",D25&gt;3,"D")</f>
+        <v>Model Dem</v>
+      </c>
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
+      <c r="W25" s="17"/>
+      <c r="X25" s="17"/>
+    </row>
+    <row r="26" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="str" cm="1">
-        <f t="array" ref="A26">_xlfn.IFS(ISBLANK(D26),"SwingState",D26&lt;3,"R",D26&gt;3,"D")</f>
+        <f t="array" ref="A26">_xlfn.IFS(ISBLANK(D26),"SwingState",D26 = 3, "SwingState",D26=4,"SwingState",D26&lt;3,"R",D26&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B26" s="10" t="s">
@@ -39594,10 +40348,24 @@
       <c r="D26" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E26" s="19">
+        <v>32.354667999999997</v>
+      </c>
+      <c r="F26" s="19">
+        <v>-89.398527999999999</v>
+      </c>
+      <c r="K26" s="2" t="str" cm="1">
+        <f t="array" ref="K26">_xlfn.IFS(ISBLANK(D26),"SwingState",D26 = 3, "Model Rep",D26=4,"Model Dem",D26&lt;3,"R",D26&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="U26" s="17"/>
+      <c r="V26" s="17"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="17"/>
+    </row>
+    <row r="27" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="str" cm="1">
-        <f t="array" ref="A27">_xlfn.IFS(ISBLANK(D27),"SwingState",D27&lt;3,"R",D27&gt;3,"D")</f>
+        <f t="array" ref="A27">_xlfn.IFS(ISBLANK(D27),"SwingState",D27 = 3, "SwingState",D27=4,"SwingState",D27&lt;3,"R",D27&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B27" s="10" t="s">
@@ -39609,10 +40377,24 @@
       <c r="D27" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E27" s="19">
+        <v>37.964252999999999</v>
+      </c>
+      <c r="F27" s="19">
+        <v>-91.831833000000003</v>
+      </c>
+      <c r="K27" s="2" t="str" cm="1">
+        <f t="array" ref="K27">_xlfn.IFS(ISBLANK(D27),"SwingState",D27 = 3, "Model Rep",D27=4,"Model Dem",D27&lt;3,"R",D27&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="U27" s="17"/>
+      <c r="V27" s="17"/>
+      <c r="W27" s="17"/>
+      <c r="X27" s="17"/>
+    </row>
+    <row r="28" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="str" cm="1">
-        <f t="array" ref="A28">_xlfn.IFS(ISBLANK(D28),"SwingState",D28&lt;3,"R",D28&gt;3,"D")</f>
+        <f t="array" ref="A28">_xlfn.IFS(ISBLANK(D28),"SwingState",D28 = 3, "SwingState",D28=4,"SwingState",D28&lt;3,"R",D28&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B28" s="10" t="s">
@@ -39624,10 +40406,24 @@
       <c r="D28" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E28" s="19">
+        <v>46.879682000000003</v>
+      </c>
+      <c r="F28" s="19">
+        <v>-110.362566</v>
+      </c>
+      <c r="K28" s="2" t="str" cm="1">
+        <f t="array" ref="K28">_xlfn.IFS(ISBLANK(D28),"SwingState",D28 = 3, "Model Rep",D28=4,"Model Dem",D28&lt;3,"R",D28&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+    </row>
+    <row r="29" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="str" cm="1">
-        <f t="array" ref="A29">_xlfn.IFS(ISBLANK(D29),"SwingState",D29&lt;3,"R",D29&gt;3,"D")</f>
+        <f t="array" ref="A29">_xlfn.IFS(ISBLANK(D29),"SwingState",D29 = 3, "SwingState",D29=4,"SwingState",D29&lt;3,"R",D29&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B29" s="10" t="s">
@@ -39639,10 +40435,24 @@
       <c r="D29" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E29" s="19">
+        <v>41.492536999999999</v>
+      </c>
+      <c r="F29" s="19">
+        <v>-99.901813000000004</v>
+      </c>
+      <c r="K29" s="2" t="str" cm="1">
+        <f t="array" ref="K29">_xlfn.IFS(ISBLANK(D29),"SwingState",D29 = 3, "Model Rep",D29=4,"Model Dem",D29&lt;3,"R",D29&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="U29" s="17"/>
+      <c r="V29" s="17"/>
+      <c r="W29" s="17"/>
+      <c r="X29" s="17"/>
+    </row>
+    <row r="30" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="str" cm="1">
-        <f t="array" ref="A30">_xlfn.IFS(ISBLANK(D30),"SwingState",D30&lt;3,"R",D30&gt;3,"D")</f>
+        <f t="array" ref="A30">_xlfn.IFS(ISBLANK(D30),"SwingState",D30 = 3, "SwingState",D30=4,"SwingState",D30&lt;3,"R",D30&gt;3,"D")</f>
         <v>SwingState</v>
       </c>
       <c r="B30" s="10" t="s">
@@ -39651,10 +40461,27 @@
       <c r="C30" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="D30" s="2">
+        <v>4</v>
+      </c>
+      <c r="E30" s="19">
+        <v>38.802610000000001</v>
+      </c>
+      <c r="F30" s="19">
+        <v>-116.419389</v>
+      </c>
+      <c r="K30" s="2" t="str" cm="1">
+        <f t="array" ref="K30">_xlfn.IFS(ISBLANK(D30),"SwingState",D30 = 3, "Model Rep",D30=4,"Model Dem",D30&lt;3,"R",D30&gt;3,"D")</f>
+        <v>Model Dem</v>
+      </c>
+      <c r="U30" s="17"/>
+      <c r="V30" s="17"/>
+      <c r="W30" s="17"/>
+      <c r="X30" s="17"/>
+    </row>
+    <row r="31" spans="1:24" ht="29" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="str" cm="1">
-        <f t="array" ref="A31">_xlfn.IFS(ISBLANK(D31),"SwingState",D31&lt;3,"R",D31&gt;3,"D")</f>
+        <f t="array" ref="A31">_xlfn.IFS(ISBLANK(D31),"SwingState",D31 = 3, "SwingState",D31=4,"SwingState",D31&lt;3,"R",D31&gt;3,"D")</f>
         <v>SwingState</v>
       </c>
       <c r="B31" s="10" t="s">
@@ -39663,10 +40490,27 @@
       <c r="C31" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D31" s="2">
+        <v>4</v>
+      </c>
+      <c r="E31" s="19">
+        <v>43.193852</v>
+      </c>
+      <c r="F31" s="19">
+        <v>-71.572395</v>
+      </c>
+      <c r="K31" s="2" t="str" cm="1">
+        <f t="array" ref="K31">_xlfn.IFS(ISBLANK(D31),"SwingState",D31 = 3, "Model Rep",D31=4,"Model Dem",D31&lt;3,"R",D31&gt;3,"D")</f>
+        <v>Model Dem</v>
+      </c>
+      <c r="U31" s="17"/>
+      <c r="V31" s="17"/>
+      <c r="W31" s="17"/>
+      <c r="X31" s="17"/>
+    </row>
+    <row r="32" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="str" cm="1">
-        <f t="array" ref="A32">_xlfn.IFS(ISBLANK(D32),"SwingState",D32&lt;3,"R",D32&gt;3,"D")</f>
+        <f t="array" ref="A32">_xlfn.IFS(ISBLANK(D32),"SwingState",D32 = 3, "SwingState",D32=4,"SwingState",D32&lt;3,"R",D32&gt;3,"D")</f>
         <v>D</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -39678,10 +40522,24 @@
       <c r="D32" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E32" s="19">
+        <v>40.058323999999999</v>
+      </c>
+      <c r="F32" s="19">
+        <v>-74.405660999999995</v>
+      </c>
+      <c r="K32" s="2" t="str" cm="1">
+        <f t="array" ref="K32">_xlfn.IFS(ISBLANK(D32),"SwingState",D32 = 3, "Model Rep",D32=4,"Model Dem",D32&lt;3,"R",D32&gt;3,"D")</f>
+        <v>D</v>
+      </c>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="17"/>
+    </row>
+    <row r="33" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="str" cm="1">
-        <f t="array" ref="A33">_xlfn.IFS(ISBLANK(D33),"SwingState",D33&lt;3,"R",D33&gt;3,"D")</f>
+        <f t="array" ref="A33">_xlfn.IFS(ISBLANK(D33),"SwingState",D33 = 3, "SwingState",D33=4,"SwingState",D33&lt;3,"R",D33&gt;3,"D")</f>
         <v>D</v>
       </c>
       <c r="B33" s="10" t="s">
@@ -39693,10 +40551,24 @@
       <c r="D33" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E33" s="19">
+        <v>34.972729999999999</v>
+      </c>
+      <c r="F33" s="19">
+        <v>-105.032363</v>
+      </c>
+      <c r="K33" s="2" t="str" cm="1">
+        <f t="array" ref="K33">_xlfn.IFS(ISBLANK(D33),"SwingState",D33 = 3, "Model Rep",D33=4,"Model Dem",D33&lt;3,"R",D33&gt;3,"D")</f>
+        <v>D</v>
+      </c>
+      <c r="U33" s="17"/>
+      <c r="V33" s="17"/>
+      <c r="W33" s="17"/>
+      <c r="X33" s="17"/>
+    </row>
+    <row r="34" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="str" cm="1">
-        <f t="array" ref="A34">_xlfn.IFS(ISBLANK(D34),"SwingState",D34&lt;3,"R",D34&gt;3,"D")</f>
+        <f t="array" ref="A34">_xlfn.IFS(ISBLANK(D34),"SwingState",D34 = 3, "SwingState",D34=4,"SwingState",D34&lt;3,"R",D34&gt;3,"D")</f>
         <v>D</v>
       </c>
       <c r="B34" s="10" t="s">
@@ -39708,10 +40580,24 @@
       <c r="D34" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="E34" s="19">
+        <v>43.299427999999999</v>
+      </c>
+      <c r="F34" s="19">
+        <v>-74.217933000000002</v>
+      </c>
+      <c r="K34" s="2" t="str" cm="1">
+        <f t="array" ref="K34">_xlfn.IFS(ISBLANK(D34),"SwingState",D34 = 3, "Model Rep",D34=4,"Model Dem",D34&lt;3,"R",D34&gt;3,"D")</f>
+        <v>D</v>
+      </c>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="17"/>
+    </row>
+    <row r="35" spans="1:24" ht="29" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="str" cm="1">
-        <f t="array" ref="A35">_xlfn.IFS(ISBLANK(D35),"SwingState",D35&lt;3,"R",D35&gt;3,"D")</f>
+        <f t="array" ref="A35">_xlfn.IFS(ISBLANK(D35),"SwingState",D35 = 3, "SwingState",D35=4,"SwingState",D35&lt;3,"R",D35&gt;3,"D")</f>
         <v>SwingState</v>
       </c>
       <c r="B35" s="10" t="s">
@@ -39720,10 +40606,27 @@
       <c r="C35" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="D35" s="2">
+        <v>3</v>
+      </c>
+      <c r="E35" s="19">
+        <v>35.759573000000003</v>
+      </c>
+      <c r="F35" s="19">
+        <v>-79.019300000000001</v>
+      </c>
+      <c r="K35" s="2" t="str" cm="1">
+        <f t="array" ref="K35">_xlfn.IFS(ISBLANK(D35),"SwingState",D35 = 3, "Model Rep",D35=4,"Model Dem",D35&lt;3,"R",D35&gt;3,"D")</f>
+        <v>Model Rep</v>
+      </c>
+      <c r="U35" s="17"/>
+      <c r="V35" s="17"/>
+      <c r="W35" s="17"/>
+      <c r="X35" s="17"/>
+    </row>
+    <row r="36" spans="1:24" ht="29" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="str" cm="1">
-        <f t="array" ref="A36">_xlfn.IFS(ISBLANK(D36),"SwingState",D36&lt;3,"R",D36&gt;3,"D")</f>
+        <f t="array" ref="A36">_xlfn.IFS(ISBLANK(D36),"SwingState",D36 = 3, "SwingState",D36=4,"SwingState",D36&lt;3,"R",D36&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B36" s="10" t="s">
@@ -39735,10 +40638,24 @@
       <c r="D36" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E36" s="19">
+        <v>47.551493000000001</v>
+      </c>
+      <c r="F36" s="19">
+        <v>-101.00201199999999</v>
+      </c>
+      <c r="K36" s="2" t="str" cm="1">
+        <f t="array" ref="K36">_xlfn.IFS(ISBLANK(D36),"SwingState",D36 = 3, "Model Rep",D36=4,"Model Dem",D36&lt;3,"R",D36&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="U36" s="17"/>
+      <c r="V36" s="17"/>
+      <c r="W36" s="17"/>
+      <c r="X36" s="17"/>
+    </row>
+    <row r="37" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="str" cm="1">
-        <f t="array" ref="A37">_xlfn.IFS(ISBLANK(D37),"SwingState",D37&lt;3,"R",D37&gt;3,"D")</f>
+        <f t="array" ref="A37">_xlfn.IFS(ISBLANK(D37),"SwingState",D37 = 3, "SwingState",D37=4,"SwingState",D37&lt;3,"R",D37&gt;3,"D")</f>
         <v>SwingState</v>
       </c>
       <c r="B37" s="10" t="s">
@@ -39747,10 +40664,27 @@
       <c r="C37" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D37" s="2">
+        <v>4</v>
+      </c>
+      <c r="E37" s="19">
+        <v>40.417287000000002</v>
+      </c>
+      <c r="F37" s="19">
+        <v>-82.907122999999999</v>
+      </c>
+      <c r="K37" s="2" t="str" cm="1">
+        <f t="array" ref="K37">_xlfn.IFS(ISBLANK(D37),"SwingState",D37 = 3, "Model Rep",D37=4,"Model Dem",D37&lt;3,"R",D37&gt;3,"D")</f>
+        <v>Model Dem</v>
+      </c>
+      <c r="U37" s="17"/>
+      <c r="V37" s="17"/>
+      <c r="W37" s="17"/>
+      <c r="X37" s="17"/>
+    </row>
+    <row r="38" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="str" cm="1">
-        <f t="array" ref="A38">_xlfn.IFS(ISBLANK(D38),"SwingState",D38&lt;3,"R",D38&gt;3,"D")</f>
+        <f t="array" ref="A38">_xlfn.IFS(ISBLANK(D38),"SwingState",D38 = 3, "SwingState",D38=4,"SwingState",D38&lt;3,"R",D38&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B38" s="10" t="s">
@@ -39762,10 +40696,24 @@
       <c r="D38" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E38" s="19">
+        <v>35.007752000000004</v>
+      </c>
+      <c r="F38" s="19">
+        <v>-97.092877000000001</v>
+      </c>
+      <c r="K38" s="2" t="str" cm="1">
+        <f t="array" ref="K38">_xlfn.IFS(ISBLANK(D38),"SwingState",D38 = 3, "Model Rep",D38=4,"Model Dem",D38&lt;3,"R",D38&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="U38" s="17"/>
+      <c r="V38" s="17"/>
+      <c r="W38" s="17"/>
+      <c r="X38" s="17"/>
+    </row>
+    <row r="39" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="str" cm="1">
-        <f t="array" ref="A39">_xlfn.IFS(ISBLANK(D39),"SwingState",D39&lt;3,"R",D39&gt;3,"D")</f>
+        <f t="array" ref="A39">_xlfn.IFS(ISBLANK(D39),"SwingState",D39 = 3, "SwingState",D39=4,"SwingState",D39&lt;3,"R",D39&gt;3,"D")</f>
         <v>D</v>
       </c>
       <c r="B39" s="10" t="s">
@@ -39777,10 +40725,24 @@
       <c r="D39" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="E39" s="19">
+        <v>43.804133</v>
+      </c>
+      <c r="F39" s="19">
+        <v>-120.55420100000001</v>
+      </c>
+      <c r="K39" s="2" t="str" cm="1">
+        <f t="array" ref="K39">_xlfn.IFS(ISBLANK(D39),"SwingState",D39 = 3, "Model Rep",D39=4,"Model Dem",D39&lt;3,"R",D39&gt;3,"D")</f>
+        <v>D</v>
+      </c>
+      <c r="U39" s="17"/>
+      <c r="V39" s="17"/>
+      <c r="W39" s="17"/>
+      <c r="X39" s="17"/>
+    </row>
+    <row r="40" spans="1:24" ht="29" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="str" cm="1">
-        <f t="array" ref="A40">_xlfn.IFS(ISBLANK(D40),"SwingState",D40&lt;3,"R",D40&gt;3,"D")</f>
+        <f t="array" ref="A40">_xlfn.IFS(ISBLANK(D40),"SwingState",D40 = 3, "SwingState",D40=4,"SwingState",D40&lt;3,"R",D40&gt;3,"D")</f>
         <v>SwingState</v>
       </c>
       <c r="B40" s="10" t="s">
@@ -39789,10 +40751,27 @@
       <c r="C40" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="D40" s="2">
+        <v>3</v>
+      </c>
+      <c r="E40" s="19">
+        <v>41.203322</v>
+      </c>
+      <c r="F40" s="19">
+        <v>-77.194524999999999</v>
+      </c>
+      <c r="K40" s="2" t="str" cm="1">
+        <f t="array" ref="K40">_xlfn.IFS(ISBLANK(D40),"SwingState",D40 = 3, "Model Rep",D40=4,"Model Dem",D40&lt;3,"R",D40&gt;3,"D")</f>
+        <v>Model Rep</v>
+      </c>
+      <c r="U40" s="17"/>
+      <c r="V40" s="17"/>
+      <c r="W40" s="17"/>
+      <c r="X40" s="17"/>
+    </row>
+    <row r="41" spans="1:24" ht="29" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="str" cm="1">
-        <f t="array" ref="A41">_xlfn.IFS(ISBLANK(D41),"SwingState",D41&lt;3,"R",D41&gt;3,"D")</f>
+        <f t="array" ref="A41">_xlfn.IFS(ISBLANK(D41),"SwingState",D41 = 3, "SwingState",D41=4,"SwingState",D41&lt;3,"R",D41&gt;3,"D")</f>
         <v>D</v>
       </c>
       <c r="B41" s="10" t="s">
@@ -39804,10 +40783,24 @@
       <c r="D41" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="E41" s="19">
+        <v>18.220832999999999</v>
+      </c>
+      <c r="F41" s="19">
+        <v>-66.590148999999997</v>
+      </c>
+      <c r="K41" s="2" t="str" cm="1">
+        <f t="array" ref="K41">_xlfn.IFS(ISBLANK(D41),"SwingState",D41 = 3, "Model Rep",D41=4,"Model Dem",D41&lt;3,"R",D41&gt;3,"D")</f>
+        <v>D</v>
+      </c>
+      <c r="U41" s="17"/>
+      <c r="V41" s="17"/>
+      <c r="W41" s="17"/>
+      <c r="X41" s="17"/>
+    </row>
+    <row r="42" spans="1:24" ht="29" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="str" cm="1">
-        <f t="array" ref="A42">_xlfn.IFS(ISBLANK(D42),"SwingState",D42&lt;3,"R",D42&gt;3,"D")</f>
+        <f t="array" ref="A42">_xlfn.IFS(ISBLANK(D42),"SwingState",D42 = 3, "SwingState",D42=4,"SwingState",D42&lt;3,"R",D42&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B42" s="10" t="s">
@@ -39819,10 +40812,24 @@
       <c r="D42" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="E42" s="19">
+        <v>41.580095</v>
+      </c>
+      <c r="F42" s="19">
+        <v>-71.477429000000001</v>
+      </c>
+      <c r="K42" s="2" t="str" cm="1">
+        <f t="array" ref="K42">_xlfn.IFS(ISBLANK(D42),"SwingState",D42 = 3, "Model Rep",D42=4,"Model Dem",D42&lt;3,"R",D42&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="U42" s="17"/>
+      <c r="V42" s="17"/>
+      <c r="W42" s="17"/>
+      <c r="X42" s="17"/>
+    </row>
+    <row r="43" spans="1:24" ht="29" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="str" cm="1">
-        <f t="array" ref="A43">_xlfn.IFS(ISBLANK(D43),"SwingState",D43&lt;3,"R",D43&gt;3,"D")</f>
+        <f t="array" ref="A43">_xlfn.IFS(ISBLANK(D43),"SwingState",D43 = 3, "SwingState",D43=4,"SwingState",D43&lt;3,"R",D43&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B43" s="10" t="s">
@@ -39834,10 +40841,24 @@
       <c r="D43" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E43" s="19">
+        <v>33.836081</v>
+      </c>
+      <c r="F43" s="19">
+        <v>-81.163724999999999</v>
+      </c>
+      <c r="K43" s="2" t="str" cm="1">
+        <f t="array" ref="K43">_xlfn.IFS(ISBLANK(D43),"SwingState",D43 = 3, "Model Rep",D43=4,"Model Dem",D43&lt;3,"R",D43&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="U43" s="17"/>
+      <c r="V43" s="17"/>
+      <c r="W43" s="17"/>
+      <c r="X43" s="17"/>
+    </row>
+    <row r="44" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="str" cm="1">
-        <f t="array" ref="A44">_xlfn.IFS(ISBLANK(D44),"SwingState",D44&lt;3,"R",D44&gt;3,"D")</f>
+        <f t="array" ref="A44">_xlfn.IFS(ISBLANK(D44),"SwingState",D44 = 3, "SwingState",D44=4,"SwingState",D44&lt;3,"R",D44&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B44" s="10" t="s">
@@ -39849,10 +40870,24 @@
       <c r="D44" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E44" s="19">
+        <v>43.969515000000001</v>
+      </c>
+      <c r="F44" s="19">
+        <v>-99.901813000000004</v>
+      </c>
+      <c r="K44" s="2" t="str" cm="1">
+        <f t="array" ref="K44">_xlfn.IFS(ISBLANK(D44),"SwingState",D44 = 3, "Model Rep",D44=4,"Model Dem",D44&lt;3,"R",D44&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="U44" s="17"/>
+      <c r="V44" s="17"/>
+      <c r="W44" s="17"/>
+      <c r="X44" s="17"/>
+    </row>
+    <row r="45" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="str" cm="1">
-        <f t="array" ref="A45">_xlfn.IFS(ISBLANK(D45),"SwingState",D45&lt;3,"R",D45&gt;3,"D")</f>
+        <f t="array" ref="A45">_xlfn.IFS(ISBLANK(D45),"SwingState",D45 = 3, "SwingState",D45=4,"SwingState",D45&lt;3,"R",D45&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B45" s="10" t="s">
@@ -39864,10 +40899,24 @@
       <c r="D45" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E45" s="19">
+        <v>35.517491</v>
+      </c>
+      <c r="F45" s="19">
+        <v>-86.580447000000007</v>
+      </c>
+      <c r="K45" s="2" t="str" cm="1">
+        <f t="array" ref="K45">_xlfn.IFS(ISBLANK(D45),"SwingState",D45 = 3, "Model Rep",D45=4,"Model Dem",D45&lt;3,"R",D45&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="U45" s="17"/>
+      <c r="V45" s="17"/>
+      <c r="W45" s="17"/>
+      <c r="X45" s="17"/>
+    </row>
+    <row r="46" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="str" cm="1">
-        <f t="array" ref="A46">_xlfn.IFS(ISBLANK(D46),"SwingState",D46&lt;3,"R",D46&gt;3,"D")</f>
+        <f t="array" ref="A46">_xlfn.IFS(ISBLANK(D46),"SwingState",D46 = 3, "SwingState",D46=4,"SwingState",D46&lt;3,"R",D46&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B46" s="10" t="s">
@@ -39879,10 +40928,24 @@
       <c r="D46" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E46" s="19">
+        <v>31.968599000000001</v>
+      </c>
+      <c r="F46" s="19">
+        <v>-99.901813000000004</v>
+      </c>
+      <c r="K46" s="2" t="str" cm="1">
+        <f t="array" ref="K46">_xlfn.IFS(ISBLANK(D46),"SwingState",D46 = 3, "Model Rep",D46=4,"Model Dem",D46&lt;3,"R",D46&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="U46" s="17"/>
+      <c r="V46" s="17"/>
+      <c r="W46" s="17"/>
+      <c r="X46" s="17"/>
+    </row>
+    <row r="47" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="str" cm="1">
-        <f t="array" ref="A47">_xlfn.IFS(ISBLANK(D47),"SwingState",D47&lt;3,"R",D47&gt;3,"D")</f>
+        <f t="array" ref="A47">_xlfn.IFS(ISBLANK(D47),"SwingState",D47 = 3, "SwingState",D47=4,"SwingState",D47&lt;3,"R",D47&gt;3,"D")</f>
         <v>D</v>
       </c>
       <c r="B47" s="10" t="s">
@@ -39894,10 +40957,24 @@
       <c r="D47" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E47" s="19">
+        <v>39.320979999999999</v>
+      </c>
+      <c r="F47" s="19">
+        <v>-111.09373100000001</v>
+      </c>
+      <c r="K47" s="2" t="str" cm="1">
+        <f t="array" ref="K47">_xlfn.IFS(ISBLANK(D47),"SwingState",D47 = 3, "Model Rep",D47=4,"Model Dem",D47&lt;3,"R",D47&gt;3,"D")</f>
+        <v>D</v>
+      </c>
+      <c r="U47" s="17"/>
+      <c r="V47" s="17"/>
+      <c r="W47" s="17"/>
+      <c r="X47" s="17"/>
+    </row>
+    <row r="48" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="str" cm="1">
-        <f t="array" ref="A48">_xlfn.IFS(ISBLANK(D48),"SwingState",D48&lt;3,"R",D48&gt;3,"D")</f>
+        <f t="array" ref="A48">_xlfn.IFS(ISBLANK(D48),"SwingState",D48 = 3, "SwingState",D48=4,"SwingState",D48&lt;3,"R",D48&gt;3,"D")</f>
         <v>SwingState</v>
       </c>
       <c r="B48" s="10" t="s">
@@ -39906,10 +40983,27 @@
       <c r="C48" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D48" s="2">
+        <v>4</v>
+      </c>
+      <c r="E48" s="19">
+        <v>44.558802999999997</v>
+      </c>
+      <c r="F48" s="19">
+        <v>-72.577841000000006</v>
+      </c>
+      <c r="K48" s="2" t="str" cm="1">
+        <f t="array" ref="K48">_xlfn.IFS(ISBLANK(D48),"SwingState",D48 = 3, "Model Rep",D48=4,"Model Dem",D48&lt;3,"R",D48&gt;3,"D")</f>
+        <v>Model Dem</v>
+      </c>
+      <c r="U48" s="17"/>
+      <c r="V48" s="17"/>
+      <c r="W48" s="17"/>
+      <c r="X48" s="17"/>
+    </row>
+    <row r="49" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="str" cm="1">
-        <f t="array" ref="A49">_xlfn.IFS(ISBLANK(D49),"SwingState",D49&lt;3,"R",D49&gt;3,"D")</f>
+        <f t="array" ref="A49">_xlfn.IFS(ISBLANK(D49),"SwingState",D49 = 3, "SwingState",D49=4,"SwingState",D49&lt;3,"R",D49&gt;3,"D")</f>
         <v>D</v>
       </c>
       <c r="B49" s="10" t="s">
@@ -39921,10 +41015,24 @@
       <c r="D49" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="E49" s="19">
+        <v>37.431573</v>
+      </c>
+      <c r="F49" s="19">
+        <v>-78.656893999999994</v>
+      </c>
+      <c r="K49" s="2" t="str" cm="1">
+        <f t="array" ref="K49">_xlfn.IFS(ISBLANK(D49),"SwingState",D49 = 3, "Model Rep",D49=4,"Model Dem",D49&lt;3,"R",D49&gt;3,"D")</f>
+        <v>D</v>
+      </c>
+      <c r="U49" s="17"/>
+      <c r="V49" s="17"/>
+      <c r="W49" s="17"/>
+      <c r="X49" s="17"/>
+    </row>
+    <row r="50" spans="1:24" ht="29" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="str" cm="1">
-        <f t="array" ref="A50">_xlfn.IFS(ISBLANK(D50),"SwingState",D50&lt;3,"R",D50&gt;3,"D")</f>
+        <f t="array" ref="A50">_xlfn.IFS(ISBLANK(D50),"SwingState",D50 = 3, "SwingState",D50=4,"SwingState",D50&lt;3,"R",D50&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B50" s="10" t="s">
@@ -39936,10 +41044,24 @@
       <c r="D50" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E50" s="19">
+        <v>47.751074000000003</v>
+      </c>
+      <c r="F50" s="19">
+        <v>-120.740139</v>
+      </c>
+      <c r="K50" s="2" t="str" cm="1">
+        <f t="array" ref="K50">_xlfn.IFS(ISBLANK(D50),"SwingState",D50 = 3, "Model Rep",D50=4,"Model Dem",D50&lt;3,"R",D50&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="U50" s="17"/>
+      <c r="V50" s="17"/>
+      <c r="W50" s="17"/>
+      <c r="X50" s="17"/>
+    </row>
+    <row r="51" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="str" cm="1">
-        <f t="array" ref="A51">_xlfn.IFS(ISBLANK(D51),"SwingState",D51&lt;3,"R",D51&gt;3,"D")</f>
+        <f t="array" ref="A51">_xlfn.IFS(ISBLANK(D51),"SwingState",D51 = 3, "SwingState",D51=4,"SwingState",D51&lt;3,"R",D51&gt;3,"D")</f>
         <v>SwingState</v>
       </c>
       <c r="B51" s="10" t="s">
@@ -39948,10 +41070,27 @@
       <c r="C51" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D51" s="2">
+        <v>3</v>
+      </c>
+      <c r="E51" s="19">
+        <v>38.597625999999998</v>
+      </c>
+      <c r="F51" s="19">
+        <v>-80.454903000000002</v>
+      </c>
+      <c r="K51" s="2" t="str" cm="1">
+        <f t="array" ref="K51">_xlfn.IFS(ISBLANK(D51),"SwingState",D51 = 3, "Model Rep",D51=4,"Model Dem",D51&lt;3,"R",D51&gt;3,"D")</f>
+        <v>Model Rep</v>
+      </c>
+      <c r="U51" s="17"/>
+      <c r="V51" s="17"/>
+      <c r="W51" s="17"/>
+      <c r="X51" s="17"/>
+    </row>
+    <row r="52" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="str" cm="1">
-        <f t="array" ref="A52">_xlfn.IFS(ISBLANK(D52),"SwingState",D52&lt;3,"R",D52&gt;3,"D")</f>
+        <f t="array" ref="A52">_xlfn.IFS(ISBLANK(D52),"SwingState",D52 = 3, "SwingState",D52=4,"SwingState",D52&lt;3,"R",D52&gt;3,"D")</f>
         <v>R</v>
       </c>
       <c r="B52" s="10" t="s">
@@ -39963,16 +41102,820 @@
       <c r="D52" s="2">
         <v>1</v>
       </c>
+      <c r="E52" s="19">
+        <v>43.784439999999996</v>
+      </c>
+      <c r="F52" s="19">
+        <v>-88.787868000000003</v>
+      </c>
+      <c r="K52" s="2" t="str" cm="1">
+        <f t="array" ref="K52">_xlfn.IFS(ISBLANK(D52),"SwingState",D52 = 3, "Model Rep",D52=4,"Model Dem",D52&lt;3,"R",D52&gt;3,"D")</f>
+        <v>R</v>
+      </c>
+      <c r="U52" s="17"/>
+      <c r="V52" s="17"/>
+      <c r="W52" s="17"/>
+      <c r="X52" s="17"/>
+    </row>
+    <row r="53" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="E53" s="19">
+        <v>43.075968000000003</v>
+      </c>
+      <c r="F53" s="19">
+        <v>-107.290284</v>
+      </c>
+      <c r="U53" s="17"/>
+      <c r="V53" s="17"/>
+      <c r="W53" s="17"/>
+      <c r="X53" s="17"/>
+    </row>
+    <row r="54" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="U54" s="17"/>
+      <c r="V54" s="17"/>
+      <c r="W54" s="17"/>
+      <c r="X54" s="17"/>
+    </row>
+    <row r="55" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="U55" s="17"/>
+      <c r="V55" s="17"/>
+      <c r="W55" s="17"/>
+      <c r="X55"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O1" r:id="rId1" xr:uid="{BB2978F7-FF7A-8D4E-A41C-DE1C98FC5455}"/>
+    <hyperlink ref="Q1" r:id="rId1" xr:uid="{BB2978F7-FF7A-8D4E-A41C-DE1C98FC5455}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144405A7-B4EE-6743-9EA1-4956D20FBC19}">
+  <dimension ref="A1:I53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="17">
+        <v>32.318230999999997</v>
+      </c>
+      <c r="C2" s="17">
+        <v>-86.902298000000002</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="17">
+        <v>63.588752999999997</v>
+      </c>
+      <c r="C3" s="17">
+        <v>-154.49306200000001</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="17">
+        <v>34.048927999999997</v>
+      </c>
+      <c r="C4" s="17">
+        <v>-111.09373100000001</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="17">
+        <v>35.201050000000002</v>
+      </c>
+      <c r="C5" s="17">
+        <v>-91.831833000000003</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="17">
+        <v>36.778261000000001</v>
+      </c>
+      <c r="C6" s="17">
+        <v>-119.41793199999999</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="17">
+        <v>39.550051000000003</v>
+      </c>
+      <c r="C7" s="17">
+        <v>-105.782067</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="17">
+        <v>41.603220999999998</v>
+      </c>
+      <c r="C8" s="17">
+        <v>-73.087749000000002</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="17">
+        <v>38.910831999999999</v>
+      </c>
+      <c r="C9" s="17">
+        <v>-75.527670000000001</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="17">
+        <v>38.905985000000001</v>
+      </c>
+      <c r="C10" s="17">
+        <v>-77.033417999999998</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="17">
+        <v>27.664826999999999</v>
+      </c>
+      <c r="C11" s="17">
+        <v>-81.515754000000001</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="17">
+        <v>32.157435</v>
+      </c>
+      <c r="C12" s="17">
+        <v>-82.907122999999999</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="17">
+        <v>19.898682000000001</v>
+      </c>
+      <c r="C13" s="17">
+        <v>-155.66585699999999</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="17">
+        <v>44.068201999999999</v>
+      </c>
+      <c r="C14" s="17">
+        <v>-114.742041</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="17">
+        <v>40.633125</v>
+      </c>
+      <c r="C15" s="17">
+        <v>-89.398527999999999</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="17">
+        <v>40.551217000000001</v>
+      </c>
+      <c r="C16" s="17">
+        <v>-85.602363999999994</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="17">
+        <v>41.878003</v>
+      </c>
+      <c r="C17" s="17">
+        <v>-93.097701999999998</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="17">
+        <v>39.011901999999999</v>
+      </c>
+      <c r="C18" s="17">
+        <v>-98.484245999999999</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="17">
+        <v>37.839333000000003</v>
+      </c>
+      <c r="C19" s="17">
+        <v>-84.270017999999993</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="17">
+        <v>31.244823</v>
+      </c>
+      <c r="C20" s="17">
+        <v>-92.145024000000006</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="17">
+        <v>45.253782999999999</v>
+      </c>
+      <c r="C21" s="17">
+        <v>-69.445469000000003</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="17">
+        <v>39.045755</v>
+      </c>
+      <c r="C22" s="17">
+        <v>-76.641271000000003</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="17">
+        <v>42.407210999999997</v>
+      </c>
+      <c r="C23" s="17">
+        <v>-71.382436999999996</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="17">
+        <v>44.314844000000001</v>
+      </c>
+      <c r="C24" s="17">
+        <v>-85.602363999999994</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="17">
+        <v>46.729553000000003</v>
+      </c>
+      <c r="C25" s="17">
+        <v>-94.685900000000004</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B26" s="17">
+        <v>32.354667999999997</v>
+      </c>
+      <c r="C26" s="17">
+        <v>-89.398527999999999</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B27" s="17">
+        <v>37.964252999999999</v>
+      </c>
+      <c r="C27" s="17">
+        <v>-91.831833000000003</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A28" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" s="17">
+        <v>46.879682000000003</v>
+      </c>
+      <c r="C28" s="17">
+        <v>-110.362566</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="17">
+        <v>41.492536999999999</v>
+      </c>
+      <c r="C29" s="17">
+        <v>-99.901813000000004</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30" s="17">
+        <v>38.802610000000001</v>
+      </c>
+      <c r="C30" s="17">
+        <v>-116.419389</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="17">
+        <v>43.193852</v>
+      </c>
+      <c r="C31" s="17">
+        <v>-71.572395</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" s="17">
+        <v>40.058323999999999</v>
+      </c>
+      <c r="C32" s="17">
+        <v>-74.405660999999995</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B33" s="17">
+        <v>34.972729999999999</v>
+      </c>
+      <c r="C33" s="17">
+        <v>-105.032363</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A34" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34" s="17">
+        <v>43.299427999999999</v>
+      </c>
+      <c r="C34" s="17">
+        <v>-74.217933000000002</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B35" s="17">
+        <v>35.759573000000003</v>
+      </c>
+      <c r="C35" s="17">
+        <v>-79.019300000000001</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="17">
+        <v>47.551493000000001</v>
+      </c>
+      <c r="C36" s="17">
+        <v>-101.00201199999999</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="B37" s="17">
+        <v>40.417287000000002</v>
+      </c>
+      <c r="C37" s="17">
+        <v>-82.907122999999999</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" s="17">
+        <v>35.007752000000004</v>
+      </c>
+      <c r="C38" s="17">
+        <v>-97.092877000000001</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A39" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="17">
+        <v>43.804133</v>
+      </c>
+      <c r="C39" s="17">
+        <v>-120.55420100000001</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B40" s="17">
+        <v>41.203322</v>
+      </c>
+      <c r="C40" s="17">
+        <v>-77.194524999999999</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B41" s="17">
+        <v>18.220832999999999</v>
+      </c>
+      <c r="C41" s="17">
+        <v>-66.590148999999997</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A42" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B42" s="17">
+        <v>41.580095</v>
+      </c>
+      <c r="C42" s="17">
+        <v>-71.477429000000001</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A43" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B43" s="17">
+        <v>33.836081</v>
+      </c>
+      <c r="C43" s="17">
+        <v>-81.163724999999999</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A44" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" s="17">
+        <v>43.969515000000001</v>
+      </c>
+      <c r="C44" s="17">
+        <v>-99.901813000000004</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B45" s="17">
+        <v>35.517491</v>
+      </c>
+      <c r="C45" s="17">
+        <v>-86.580447000000007</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A46" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B46" s="17">
+        <v>31.968599000000001</v>
+      </c>
+      <c r="C46" s="17">
+        <v>-99.901813000000004</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A47" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B47" s="17">
+        <v>39.320979999999999</v>
+      </c>
+      <c r="C47" s="17">
+        <v>-111.09373100000001</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A48" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B48" s="17">
+        <v>44.558802999999997</v>
+      </c>
+      <c r="C48" s="17">
+        <v>-72.577841000000006</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A49" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B49" s="17">
+        <v>37.431573</v>
+      </c>
+      <c r="C49" s="17">
+        <v>-78.656893999999994</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B50" s="17">
+        <v>47.751074000000003</v>
+      </c>
+      <c r="C50" s="17">
+        <v>-120.740139</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A51" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B51" s="17">
+        <v>38.597625999999998</v>
+      </c>
+      <c r="C51" s="17">
+        <v>-80.454903000000002</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A52" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B52" s="17">
+        <v>43.784439999999996</v>
+      </c>
+      <c r="C52" s="17">
+        <v>-88.787868000000003</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A53" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B53" s="17">
+        <v>43.075968000000003</v>
+      </c>
+      <c r="C53" s="17">
+        <v>-107.290284</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D53">
+    <sortCondition ref="D1"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="I5" r:id="rId1" xr:uid="{9AB993BB-612A-C043-946A-E73171B70CA6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9FCF36-34FD-D54B-9B0F-72A2CB9173D2}">
   <dimension ref="A1:AB261"/>
   <sheetViews>

</xml_diff>

<commit_message>
adjusting electoral votes, had wrong numbers
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myimam/Personal/15-For-50/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F071C76-A9B7-7446-8161-CFBA942A9DC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9750DCFB-725B-BE42-9637-3B8C17B2D088}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="3" xr2:uid="{A414920B-AA94-6E44-AEE3-541A17C74404}"/>
   </bookViews>
@@ -19,9 +19,10 @@
     <sheet name="Map" sheetId="5" r:id="rId4"/>
     <sheet name="latlong" sheetId="7" r:id="rId5"/>
     <sheet name="StateVT" sheetId="3" r:id="rId6"/>
+    <sheet name="Electoral Votes" sheetId="8" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="165">
   <si>
     <t>E</t>
   </si>
@@ -556,6 +557,9 @@
   <si>
     <t>https://developers.google.com/public-data/docs/canonical/states_csv</t>
   </si>
+  <si>
+    <t>Explain</t>
+  </si>
 </sst>
 </file>
 
@@ -565,7 +569,7 @@
     <numFmt numFmtId="170" formatCode="0.00000"/>
     <numFmt numFmtId="173" formatCode="0.00000000000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -630,6 +634,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF1A1A1A"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF1A1A1A"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -652,7 +669,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -683,6 +700,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -39483,21 +39502,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A12BA6E-D220-514B-B360-4F43E4765A8F}">
-  <dimension ref="A1:X55"/>
+  <dimension ref="A1:Y55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F53"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="15" width="10.83203125" style="2"/>
-    <col min="16" max="16" width="12.6640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="19.33203125" style="2" customWidth="1"/>
+    <col min="6" max="16" width="10.83203125" style="2"/>
+    <col min="17" max="17" width="12.6640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>79</v>
       </c>
@@ -39511,37 +39532,40 @@
         <v>77</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="str" cm="1">
         <f t="array" ref="A2">_xlfn.IFS(ISBLANK(D2),"SwingState",D2 = 3, "SwingState",D2=4,"SwingState",D2&lt;3,"R",D2&gt;3,"D")</f>
         <v>R</v>
@@ -39549,48 +39573,56 @@
       <c r="B2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="21">
         <v>9</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2" s="2" t="str" cm="1">
+        <f t="array" ref="E2">_xlfn.IFS(D2=1,"Confident Republican",D2=2,"Likely Republican",D2=3,"Model Republican", D2=4,"Model Democrat", D2=5,"Likely Democrat",D2=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F2" s="19">
         <v>32.318230999999997</v>
       </c>
-      <c r="F2" s="19">
+      <c r="G2" s="19">
         <v>-86.902298000000002</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <f>COUNTBLANK(D2:D51)</f>
         <v>0</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <f>SUMIF(A2:A52,"D",C2:C52)</f>
         <v>191</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <f>SUMIF(A2:A52,"R",C2:C52)</f>
-        <v>194</v>
-      </c>
-      <c r="J2" s="2">
-        <f>538-I2-H2</f>
-        <v>153</v>
-      </c>
-      <c r="K2" s="2" t="str" cm="1">
-        <f t="array" ref="K2">_xlfn.IFS(ISBLANK(D2),"SwingState",D2 = 3, "Model Rep",D2=4,"Model Dem",D2&lt;3,"R",D2&gt;3,"D")</f>
+        <v>191</v>
+      </c>
+      <c r="K2" s="2">
+        <f>538-J2-I2</f>
+        <v>156</v>
+      </c>
+      <c r="L2" s="2" t="str" cm="1">
+        <f t="array" ref="L2">_xlfn.IFS(ISBLANK(D2),"SwingState",D2 = 3, "Model Rep",D2=4,"Model Dem",D2&lt;3,"R",D2&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="L2" s="2">
-        <f>SUMIF(K2:K52,"D",C2:C52)+SUMIF(K2:K52,"Model Dem",C2:C52)</f>
+      <c r="M2" s="2">
+        <f>SUMIF(L2:L52,"D",C2:C52)+SUMIF(L2:L52,"Model Dem",C2:C52)</f>
         <v>267</v>
       </c>
-      <c r="M2" s="2">
-        <f>SUMIF(K2:K52,"R",C2:C52)+SUMIF(K2:K52,"Model Rep",C2:C52)</f>
-        <v>274</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="N2" s="2">
+        <f>SUMIF(L2:L52,"R",C2:C52)+SUMIF(L2:L52,"Model Rep",C2:C52)</f>
+        <v>271</v>
+      </c>
+      <c r="O2" s="2">
+        <f>M2+N2</f>
+        <v>538</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="str" cm="1">
         <f t="array" ref="A3">_xlfn.IFS(ISBLANK(D3),"SwingState",D3 = 3, "SwingState",D3=4,"SwingState",D3&lt;3,"R",D3&gt;3,"D")</f>
         <v>R</v>
@@ -39598,24 +39630,28 @@
       <c r="B3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="21">
         <v>3</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="2" t="str" cm="1">
+        <f t="array" ref="E3">_xlfn.IFS(D3=1,"Confident Republican",D3=2,"Likely Republican",D3=3,"Model Republican", D3=4,"Model Democrat", D3=5,"Likely Democrat",D3=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F3" s="19">
         <v>63.588752999999997</v>
       </c>
-      <c r="F3" s="19">
+      <c r="G3" s="19">
         <v>-154.49306200000001</v>
       </c>
-      <c r="K3" s="2" t="str" cm="1">
-        <f t="array" ref="K3">_xlfn.IFS(ISBLANK(D3),"SwingState",D3 = 3, "Model Rep",D3=4,"Model Dem",D3&lt;3,"R",D3&gt;3,"D")</f>
+      <c r="L3" s="2" t="str" cm="1">
+        <f t="array" ref="L3">_xlfn.IFS(ISBLANK(D3),"SwingState",D3 = 3, "Model Rep",D3=4,"Model Dem",D3&lt;3,"R",D3&gt;3,"D")</f>
         <v>R</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="str" cm="1">
         <f t="array" ref="A4">_xlfn.IFS(ISBLANK(D4),"SwingState",D4 = 3, "SwingState",D4=4,"SwingState",D4&lt;3,"R",D4&gt;3,"D")</f>
         <v>R</v>
@@ -39623,28 +39659,32 @@
       <c r="B4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="21">
         <v>11</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="2" t="str" cm="1">
+        <f t="array" ref="E4">_xlfn.IFS(D4=1,"Confident Republican",D4=2,"Likely Republican",D4=3,"Model Republican", D4=4,"Model Democrat", D4=5,"Likely Democrat",D4=6,"Confident Democrat")</f>
+        <v>Likely Republican</v>
+      </c>
+      <c r="F4" s="19">
         <v>34.048927999999997</v>
       </c>
-      <c r="F4" s="19">
+      <c r="G4" s="19">
         <v>-111.09373100000001</v>
       </c>
-      <c r="K4" s="2" t="str" cm="1">
-        <f t="array" ref="K4">_xlfn.IFS(ISBLANK(D4),"SwingState",D4 = 3, "Model Rep",D4=4,"Model Dem",D4&lt;3,"R",D4&gt;3,"D")</f>
+      <c r="L4" s="2" t="str" cm="1">
+        <f t="array" ref="L4">_xlfn.IFS(ISBLANK(D4),"SwingState",D4 = 3, "Model Rep",D4=4,"Model Dem",D4&lt;3,"R",D4&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="U4" s="18"/>
       <c r="V4" s="18"/>
       <c r="W4" s="18"/>
       <c r="X4" s="18"/>
-    </row>
-    <row r="5" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y4" s="18"/>
+    </row>
+    <row r="5" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="str" cm="1">
         <f t="array" ref="A5">_xlfn.IFS(ISBLANK(D5),"SwingState",D5 = 3, "SwingState",D5=4,"SwingState",D5&lt;3,"R",D5&gt;3,"D")</f>
         <v>R</v>
@@ -39652,34 +39692,38 @@
       <c r="B5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="21">
         <v>6</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="2" t="str" cm="1">
+        <f t="array" ref="E5">_xlfn.IFS(D5=1,"Confident Republican",D5=2,"Likely Republican",D5=3,"Model Republican", D5=4,"Model Democrat", D5=5,"Likely Democrat",D5=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F5" s="19">
         <v>35.201050000000002</v>
       </c>
-      <c r="F5" s="19">
+      <c r="G5" s="19">
         <v>-91.831833000000003</v>
       </c>
-      <c r="K5" s="2" t="str" cm="1">
-        <f t="array" ref="K5">_xlfn.IFS(ISBLANK(D5),"SwingState",D5 = 3, "Model Rep",D5=4,"Model Dem",D5&lt;3,"R",D5&gt;3,"D")</f>
+      <c r="L5" s="2" t="str" cm="1">
+        <f t="array" ref="L5">_xlfn.IFS(ISBLANK(D5),"SwingState",D5 = 3, "Model Rep",D5=4,"Model Dem",D5&lt;3,"R",D5&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="R5" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="U5" s="17"/>
       <c r="V5" s="17"/>
       <c r="W5" s="17"/>
       <c r="X5" s="17"/>
-    </row>
-    <row r="6" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y5" s="17"/>
+    </row>
+    <row r="6" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="str" cm="1">
         <f t="array" ref="A6">_xlfn.IFS(ISBLANK(D6),"SwingState",D6 = 3, "SwingState",D6=4,"SwingState",D6&lt;3,"R",D6&gt;3,"D")</f>
         <v>D</v>
@@ -39687,34 +39731,38 @@
       <c r="B6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="21">
         <v>55</v>
       </c>
       <c r="D6" s="2">
         <v>6</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="2" t="str" cm="1">
+        <f t="array" ref="E6">_xlfn.IFS(D6=1,"Confident Republican",D6=2,"Likely Republican",D6=3,"Model Republican", D6=4,"Model Democrat", D6=5,"Likely Democrat",D6=6,"Confident Democrat")</f>
+        <v>Confident Democrat</v>
+      </c>
+      <c r="F6" s="19">
         <v>36.778261000000001</v>
       </c>
-      <c r="F6" s="19">
+      <c r="G6" s="19">
         <v>-119.41793199999999</v>
       </c>
-      <c r="K6" s="2" t="str" cm="1">
-        <f t="array" ref="K6">_xlfn.IFS(ISBLANK(D6),"SwingState",D6 = 3, "Model Rep",D6=4,"Model Dem",D6&lt;3,"R",D6&gt;3,"D")</f>
+      <c r="L6" s="2" t="str" cm="1">
+        <f t="array" ref="L6">_xlfn.IFS(ISBLANK(D6),"SwingState",D6 = 3, "Model Rep",D6=4,"Model Dem",D6&lt;3,"R",D6&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Q6" s="16">
+      <c r="R6" s="16">
         <v>4.6866299999999998E-3</v>
       </c>
-      <c r="U6" s="17"/>
       <c r="V6" s="17"/>
       <c r="W6" s="17"/>
       <c r="X6" s="17"/>
-    </row>
-    <row r="7" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y6" s="17"/>
+    </row>
+    <row r="7" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="str" cm="1">
         <f t="array" ref="A7">_xlfn.IFS(ISBLANK(D7),"SwingState",D7 = 3, "SwingState",D7=4,"SwingState",D7&lt;3,"R",D7&gt;3,"D")</f>
         <v>SwingState</v>
@@ -39722,34 +39770,38 @@
       <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="21">
         <v>9</v>
       </c>
       <c r="D7" s="2">
         <v>4</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="2" t="str" cm="1">
+        <f t="array" ref="E7">_xlfn.IFS(D7=1,"Confident Republican",D7=2,"Likely Republican",D7=3,"Model Republican", D7=4,"Model Democrat", D7=5,"Likely Democrat",D7=6,"Confident Democrat")</f>
+        <v>Model Democrat</v>
+      </c>
+      <c r="F7" s="19">
         <v>39.550051000000003</v>
       </c>
-      <c r="F7" s="19">
+      <c r="G7" s="19">
         <v>-105.782067</v>
       </c>
-      <c r="K7" s="2" t="str" cm="1">
-        <f t="array" ref="K7">_xlfn.IFS(ISBLANK(D7),"SwingState",D7 = 3, "Model Rep",D7=4,"Model Dem",D7&lt;3,"R",D7&gt;3,"D")</f>
+      <c r="L7" s="2" t="str" cm="1">
+        <f t="array" ref="L7">_xlfn.IFS(ISBLANK(D7),"SwingState",D7 = 3, "Model Rep",D7=4,"Model Dem",D7&lt;3,"R",D7&gt;3,"D")</f>
         <v>Model Dem</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Q7" s="16">
+      <c r="R7" s="16">
         <v>-2.1856879999999999E-2</v>
       </c>
-      <c r="U7" s="17"/>
       <c r="V7" s="17"/>
       <c r="W7" s="17"/>
       <c r="X7" s="17"/>
-    </row>
-    <row r="8" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y7" s="17"/>
+    </row>
+    <row r="8" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="str" cm="1">
         <f t="array" ref="A8">_xlfn.IFS(ISBLANK(D8),"SwingState",D8 = 3, "SwingState",D8=4,"SwingState",D8&lt;3,"R",D8&gt;3,"D")</f>
         <v>D</v>
@@ -39757,34 +39809,38 @@
       <c r="B8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="21">
         <v>7</v>
       </c>
       <c r="D8" s="2">
         <v>6</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="2" t="str" cm="1">
+        <f t="array" ref="E8">_xlfn.IFS(D8=1,"Confident Republican",D8=2,"Likely Republican",D8=3,"Model Republican", D8=4,"Model Democrat", D8=5,"Likely Democrat",D8=6,"Confident Democrat")</f>
+        <v>Confident Democrat</v>
+      </c>
+      <c r="F8" s="19">
         <v>41.603220999999998</v>
       </c>
-      <c r="F8" s="19">
+      <c r="G8" s="19">
         <v>-73.087749000000002</v>
       </c>
-      <c r="K8" s="2" t="str" cm="1">
-        <f t="array" ref="K8">_xlfn.IFS(ISBLANK(D8),"SwingState",D8 = 3, "Model Rep",D8=4,"Model Dem",D8&lt;3,"R",D8&gt;3,"D")</f>
+      <c r="L8" s="2" t="str" cm="1">
+        <f t="array" ref="L8">_xlfn.IFS(ISBLANK(D8),"SwingState",D8 = 3, "Model Rep",D8=4,"Model Dem",D8&lt;3,"R",D8&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="Q8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="16">
+      <c r="R8" s="16">
         <v>1.5908700000000001E-3</v>
       </c>
-      <c r="U8" s="17"/>
       <c r="V8" s="17"/>
       <c r="W8" s="17"/>
       <c r="X8" s="17"/>
-    </row>
-    <row r="9" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y8" s="17"/>
+    </row>
+    <row r="9" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="str" cm="1">
         <f t="array" ref="A9">_xlfn.IFS(ISBLANK(D9),"SwingState",D9 = 3, "SwingState",D9=4,"SwingState",D9&lt;3,"R",D9&gt;3,"D")</f>
         <v>D</v>
@@ -39792,36 +39848,40 @@
       <c r="B9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="21">
         <v>3</v>
       </c>
       <c r="D9" s="2">
         <v>6</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="2" t="str" cm="1">
+        <f t="array" ref="E9">_xlfn.IFS(D9=1,"Confident Republican",D9=2,"Likely Republican",D9=3,"Model Republican", D9=4,"Model Democrat", D9=5,"Likely Democrat",D9=6,"Confident Democrat")</f>
+        <v>Confident Democrat</v>
+      </c>
+      <c r="F9" s="19">
         <v>38.910831999999999</v>
       </c>
-      <c r="F9" s="19">
+      <c r="G9" s="19">
         <v>-75.527670000000001</v>
       </c>
-      <c r="G9" s="17"/>
       <c r="H9" s="17"/>
-      <c r="K9" s="2" t="str" cm="1">
-        <f t="array" ref="K9">_xlfn.IFS(ISBLANK(D9),"SwingState",D9 = 3, "Model Rep",D9=4,"Model Dem",D9&lt;3,"R",D9&gt;3,"D")</f>
+      <c r="I9" s="17"/>
+      <c r="L9" s="2" t="str" cm="1">
+        <f t="array" ref="L9">_xlfn.IFS(ISBLANK(D9),"SwingState",D9 = 3, "Model Rep",D9=4,"Model Dem",D9&lt;3,"R",D9&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="Q9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="16">
+      <c r="R9" s="16">
         <v>-3.4168530000000003E-2</v>
       </c>
-      <c r="U9" s="17"/>
       <c r="V9" s="17"/>
       <c r="W9" s="17"/>
       <c r="X9" s="17"/>
-    </row>
-    <row r="10" spans="1:24" ht="29" x14ac:dyDescent="0.2">
+      <c r="Y9" s="17"/>
+    </row>
+    <row r="10" spans="1:25" ht="29" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="str" cm="1">
         <f t="array" ref="A10">_xlfn.IFS(ISBLANK(D10),"SwingState",D10 = 3, "SwingState",D10=4,"SwingState",D10&lt;3,"R",D10&gt;3,"D")</f>
         <v>D</v>
@@ -39829,34 +39889,38 @@
       <c r="B10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="21">
         <v>3</v>
       </c>
       <c r="D10" s="2">
         <v>6</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="2" t="str" cm="1">
+        <f t="array" ref="E10">_xlfn.IFS(D10=1,"Confident Republican",D10=2,"Likely Republican",D10=3,"Model Republican", D10=4,"Model Democrat", D10=5,"Likely Democrat",D10=6,"Confident Democrat")</f>
+        <v>Confident Democrat</v>
+      </c>
+      <c r="F10" s="19">
         <v>38.905985000000001</v>
       </c>
-      <c r="F10" s="19">
+      <c r="G10" s="19">
         <v>-77.033417999999998</v>
       </c>
-      <c r="K10" s="2" t="str" cm="1">
-        <f t="array" ref="K10">_xlfn.IFS(ISBLANK(D10),"SwingState",D10 = 3, "Model Rep",D10=4,"Model Dem",D10&lt;3,"R",D10&gt;3,"D")</f>
+      <c r="L10" s="2" t="str" cm="1">
+        <f t="array" ref="L10">_xlfn.IFS(ISBLANK(D10),"SwingState",D10 = 3, "Model Rep",D10=4,"Model Dem",D10&lt;3,"R",D10&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="Q10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q10" s="16">
+      <c r="R10" s="16">
         <v>7.9394279999999998E-2</v>
       </c>
-      <c r="U10" s="17"/>
       <c r="V10" s="17"/>
       <c r="W10" s="17"/>
       <c r="X10" s="17"/>
-    </row>
-    <row r="11" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y10" s="17"/>
+    </row>
+    <row r="11" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="str" cm="1">
         <f t="array" ref="A11">_xlfn.IFS(ISBLANK(D11),"SwingState",D11 = 3, "SwingState",D11=4,"SwingState",D11&lt;3,"R",D11&gt;3,"D")</f>
         <v>SwingState</v>
@@ -39864,34 +39928,38 @@
       <c r="B11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="21">
         <v>29</v>
       </c>
       <c r="D11" s="2">
         <v>3</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="2" t="str" cm="1">
+        <f t="array" ref="E11">_xlfn.IFS(D11=1,"Confident Republican",D11=2,"Likely Republican",D11=3,"Model Republican", D11=4,"Model Democrat", D11=5,"Likely Democrat",D11=6,"Confident Democrat")</f>
+        <v>Model Republican</v>
+      </c>
+      <c r="F11" s="19">
         <v>27.664826999999999</v>
       </c>
-      <c r="F11" s="19">
+      <c r="G11" s="19">
         <v>-81.515754000000001</v>
       </c>
-      <c r="K11" s="2" t="str" cm="1">
-        <f t="array" ref="K11">_xlfn.IFS(ISBLANK(D11),"SwingState",D11 = 3, "Model Rep",D11=4,"Model Dem",D11&lt;3,"R",D11&gt;3,"D")</f>
+      <c r="L11" s="2" t="str" cm="1">
+        <f t="array" ref="L11">_xlfn.IFS(ISBLANK(D11),"SwingState",D11 = 3, "Model Rep",D11=4,"Model Dem",D11&lt;3,"R",D11&gt;3,"D")</f>
         <v>Model Rep</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="Q11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q11" s="16">
+      <c r="R11" s="16">
         <v>-6.4152050000000002E-2</v>
       </c>
-      <c r="U11" s="17"/>
       <c r="V11" s="17"/>
       <c r="W11" s="17"/>
       <c r="X11" s="17"/>
-    </row>
-    <row r="12" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y11" s="17"/>
+    </row>
+    <row r="12" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="str" cm="1">
         <f t="array" ref="A12">_xlfn.IFS(ISBLANK(D12),"SwingState",D12 = 3, "SwingState",D12=4,"SwingState",D12&lt;3,"R",D12&gt;3,"D")</f>
         <v>R</v>
@@ -39899,34 +39967,38 @@
       <c r="B12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="21">
         <v>16</v>
       </c>
       <c r="D12" s="2">
         <v>2</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="2" t="str" cm="1">
+        <f t="array" ref="E12">_xlfn.IFS(D12=1,"Confident Republican",D12=2,"Likely Republican",D12=3,"Model Republican", D12=4,"Model Democrat", D12=5,"Likely Democrat",D12=6,"Confident Democrat")</f>
+        <v>Likely Republican</v>
+      </c>
+      <c r="F12" s="19">
         <v>32.157435</v>
       </c>
-      <c r="F12" s="19">
+      <c r="G12" s="19">
         <v>-82.907122999999999</v>
       </c>
-      <c r="K12" s="2" t="str" cm="1">
-        <f t="array" ref="K12">_xlfn.IFS(ISBLANK(D12),"SwingState",D12 = 3, "Model Rep",D12=4,"Model Dem",D12&lt;3,"R",D12&gt;3,"D")</f>
+      <c r="L12" s="2" t="str" cm="1">
+        <f t="array" ref="L12">_xlfn.IFS(ISBLANK(D12),"SwingState",D12 = 3, "Model Rep",D12=4,"Model Dem",D12&lt;3,"R",D12&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="Q12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q12" s="16">
+      <c r="R12" s="16">
         <v>7.2694010000000003E-2</v>
       </c>
-      <c r="U12" s="17"/>
       <c r="V12" s="17"/>
       <c r="W12" s="17"/>
       <c r="X12" s="17"/>
-    </row>
-    <row r="13" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y12" s="17"/>
+    </row>
+    <row r="13" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="str" cm="1">
         <f t="array" ref="A13">_xlfn.IFS(ISBLANK(D13),"SwingState",D13 = 3, "SwingState",D13=4,"SwingState",D13&lt;3,"R",D13&gt;3,"D")</f>
         <v>D</v>
@@ -39934,34 +40006,38 @@
       <c r="B13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="21">
         <v>4</v>
       </c>
       <c r="D13" s="2">
         <v>6</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="2" t="str" cm="1">
+        <f t="array" ref="E13">_xlfn.IFS(D13=1,"Confident Republican",D13=2,"Likely Republican",D13=3,"Model Republican", D13=4,"Model Democrat", D13=5,"Likely Democrat",D13=6,"Confident Democrat")</f>
+        <v>Confident Democrat</v>
+      </c>
+      <c r="F13" s="19">
         <v>19.898682000000001</v>
       </c>
-      <c r="F13" s="19">
+      <c r="G13" s="19">
         <v>-155.66585699999999</v>
       </c>
-      <c r="K13" s="2" t="str" cm="1">
-        <f t="array" ref="K13">_xlfn.IFS(ISBLANK(D13),"SwingState",D13 = 3, "Model Rep",D13=4,"Model Dem",D13&lt;3,"R",D13&gt;3,"D")</f>
+      <c r="L13" s="2" t="str" cm="1">
+        <f t="array" ref="L13">_xlfn.IFS(ISBLANK(D13),"SwingState",D13 = 3, "Model Rep",D13=4,"Model Dem",D13&lt;3,"R",D13&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="Q13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q13" s="16">
+      <c r="R13" s="16">
         <v>6.4423500000000003E-3</v>
       </c>
-      <c r="U13" s="17"/>
       <c r="V13" s="17"/>
       <c r="W13" s="17"/>
       <c r="X13" s="17"/>
-    </row>
-    <row r="14" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y13" s="17"/>
+    </row>
+    <row r="14" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="str" cm="1">
         <f t="array" ref="A14">_xlfn.IFS(ISBLANK(D14),"SwingState",D14 = 3, "SwingState",D14=4,"SwingState",D14&lt;3,"R",D14&gt;3,"D")</f>
         <v>R</v>
@@ -39969,34 +40045,38 @@
       <c r="B14" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="21">
         <v>4</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="2" t="str" cm="1">
+        <f t="array" ref="E14">_xlfn.IFS(D14=1,"Confident Republican",D14=2,"Likely Republican",D14=3,"Model Republican", D14=4,"Model Democrat", D14=5,"Likely Democrat",D14=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F14" s="19">
         <v>44.068201999999999</v>
       </c>
-      <c r="F14" s="19">
+      <c r="G14" s="19">
         <v>-114.742041</v>
       </c>
-      <c r="K14" s="2" t="str" cm="1">
-        <f t="array" ref="K14">_xlfn.IFS(ISBLANK(D14),"SwingState",D14 = 3, "Model Rep",D14=4,"Model Dem",D14&lt;3,"R",D14&gt;3,"D")</f>
+      <c r="L14" s="2" t="str" cm="1">
+        <f t="array" ref="L14">_xlfn.IFS(ISBLANK(D14),"SwingState",D14 = 3, "Model Rep",D14=4,"Model Dem",D14&lt;3,"R",D14&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="Q14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Q14" s="16">
+      <c r="R14" s="16">
         <v>4.6465449999999998E-2</v>
       </c>
-      <c r="U14" s="17"/>
       <c r="V14" s="17"/>
       <c r="W14" s="17"/>
       <c r="X14" s="17"/>
-    </row>
-    <row r="15" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y14" s="17"/>
+    </row>
+    <row r="15" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="str" cm="1">
         <f t="array" ref="A15">_xlfn.IFS(ISBLANK(D15),"SwingState",D15 = 3, "SwingState",D15=4,"SwingState",D15&lt;3,"R",D15&gt;3,"D")</f>
         <v>D</v>
@@ -40004,34 +40084,38 @@
       <c r="B15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="21">
         <v>20</v>
       </c>
       <c r="D15" s="2">
         <v>6</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="2" t="str" cm="1">
+        <f t="array" ref="E15">_xlfn.IFS(D15=1,"Confident Republican",D15=2,"Likely Republican",D15=3,"Model Republican", D15=4,"Model Democrat", D15=5,"Likely Democrat",D15=6,"Confident Democrat")</f>
+        <v>Confident Democrat</v>
+      </c>
+      <c r="F15" s="19">
         <v>40.633125</v>
       </c>
-      <c r="F15" s="19">
+      <c r="G15" s="19">
         <v>-89.398527999999999</v>
       </c>
-      <c r="K15" s="2" t="str" cm="1">
-        <f t="array" ref="K15">_xlfn.IFS(ISBLANK(D15),"SwingState",D15 = 3, "Model Rep",D15=4,"Model Dem",D15&lt;3,"R",D15&gt;3,"D")</f>
+      <c r="L15" s="2" t="str" cm="1">
+        <f t="array" ref="L15">_xlfn.IFS(ISBLANK(D15),"SwingState",D15 = 3, "Model Rep",D15=4,"Model Dem",D15&lt;3,"R",D15&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="P15" s="2" t="s">
+      <c r="Q15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="16">
+      <c r="R15" s="16">
         <v>-2.753968E-2</v>
       </c>
-      <c r="U15" s="17"/>
       <c r="V15" s="17"/>
       <c r="W15" s="17"/>
       <c r="X15" s="17"/>
-    </row>
-    <row r="16" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y15" s="17"/>
+    </row>
+    <row r="16" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="str" cm="1">
         <f t="array" ref="A16">_xlfn.IFS(ISBLANK(D16),"SwingState",D16 = 3, "SwingState",D16=4,"SwingState",D16&lt;3,"R",D16&gt;3,"D")</f>
         <v>R</v>
@@ -40039,34 +40123,38 @@
       <c r="B16" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="21">
         <v>11</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="2" t="str" cm="1">
+        <f t="array" ref="E16">_xlfn.IFS(D16=1,"Confident Republican",D16=2,"Likely Republican",D16=3,"Model Republican", D16=4,"Model Democrat", D16=5,"Likely Democrat",D16=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F16" s="19">
         <v>40.551217000000001</v>
       </c>
-      <c r="F16" s="19">
+      <c r="G16" s="19">
         <v>-85.602363999999994</v>
       </c>
-      <c r="K16" s="2" t="str" cm="1">
-        <f t="array" ref="K16">_xlfn.IFS(ISBLANK(D16),"SwingState",D16 = 3, "Model Rep",D16=4,"Model Dem",D16&lt;3,"R",D16&gt;3,"D")</f>
+      <c r="L16" s="2" t="str" cm="1">
+        <f t="array" ref="L16">_xlfn.IFS(ISBLANK(D16),"SwingState",D16 = 3, "Model Rep",D16=4,"Model Dem",D16&lt;3,"R",D16&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="Q16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q16" s="16">
+      <c r="R16" s="16">
         <v>-2.8092500000000001E-3</v>
       </c>
-      <c r="U16" s="17"/>
       <c r="V16" s="17"/>
       <c r="W16" s="17"/>
       <c r="X16" s="17"/>
-    </row>
-    <row r="17" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y16" s="17"/>
+    </row>
+    <row r="17" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="str" cm="1">
         <f t="array" ref="A17">_xlfn.IFS(ISBLANK(D17),"SwingState",D17 = 3, "SwingState",D17=4,"SwingState",D17&lt;3,"R",D17&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40074,34 +40162,38 @@
       <c r="B17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="21">
         <v>6</v>
       </c>
       <c r="D17" s="2">
         <v>3</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="2" t="str" cm="1">
+        <f t="array" ref="E17">_xlfn.IFS(D17=1,"Confident Republican",D17=2,"Likely Republican",D17=3,"Model Republican", D17=4,"Model Democrat", D17=5,"Likely Democrat",D17=6,"Confident Democrat")</f>
+        <v>Model Republican</v>
+      </c>
+      <c r="F17" s="19">
         <v>41.878003</v>
       </c>
-      <c r="F17" s="19">
+      <c r="G17" s="19">
         <v>-93.097701999999998</v>
       </c>
-      <c r="K17" s="2" t="str" cm="1">
-        <f t="array" ref="K17">_xlfn.IFS(ISBLANK(D17),"SwingState",D17 = 3, "Model Rep",D17=4,"Model Dem",D17&lt;3,"R",D17&gt;3,"D")</f>
+      <c r="L17" s="2" t="str" cm="1">
+        <f t="array" ref="L17">_xlfn.IFS(ISBLANK(D17),"SwingState",D17 = 3, "Model Rep",D17=4,"Model Dem",D17&lt;3,"R",D17&gt;3,"D")</f>
         <v>Model Rep</v>
       </c>
-      <c r="P17" s="2" t="s">
+      <c r="Q17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q17" s="16">
+      <c r="R17" s="16">
         <v>6.1988099999999999E-3</v>
       </c>
-      <c r="U17" s="17"/>
       <c r="V17" s="17"/>
       <c r="W17" s="17"/>
       <c r="X17" s="17"/>
-    </row>
-    <row r="18" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y17" s="17"/>
+    </row>
+    <row r="18" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="str" cm="1">
         <f t="array" ref="A18">_xlfn.IFS(ISBLANK(D18),"SwingState",D18 = 3, "SwingState",D18=4,"SwingState",D18&lt;3,"R",D18&gt;3,"D")</f>
         <v>R</v>
@@ -40109,29 +40201,33 @@
       <c r="B18" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="21">
         <v>6</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="2" t="str" cm="1">
+        <f t="array" ref="E18">_xlfn.IFS(D18=1,"Confident Republican",D18=2,"Likely Republican",D18=3,"Model Republican", D18=4,"Model Democrat", D18=5,"Likely Democrat",D18=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F18" s="19">
         <v>39.011901999999999</v>
       </c>
-      <c r="F18" s="19">
+      <c r="G18" s="19">
         <v>-98.484245999999999</v>
       </c>
-      <c r="K18" s="2" t="str" cm="1">
-        <f t="array" ref="K18">_xlfn.IFS(ISBLANK(D18),"SwingState",D18 = 3, "Model Rep",D18=4,"Model Dem",D18&lt;3,"R",D18&gt;3,"D")</f>
+      <c r="L18" s="2" t="str" cm="1">
+        <f t="array" ref="L18">_xlfn.IFS(ISBLANK(D18),"SwingState",D18 = 3, "Model Rep",D18=4,"Model Dem",D18&lt;3,"R",D18&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="Q18" s="12"/>
-      <c r="U18" s="17"/>
+      <c r="R18" s="12"/>
       <c r="V18" s="17"/>
       <c r="W18" s="17"/>
       <c r="X18" s="17"/>
-    </row>
-    <row r="19" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y18" s="17"/>
+    </row>
+    <row r="19" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="str" cm="1">
         <f t="array" ref="A19">_xlfn.IFS(ISBLANK(D19),"SwingState",D19 = 3, "SwingState",D19=4,"SwingState",D19&lt;3,"R",D19&gt;3,"D")</f>
         <v>R</v>
@@ -40139,28 +40235,32 @@
       <c r="B19" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="21">
         <v>8</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="2" t="str" cm="1">
+        <f t="array" ref="E19">_xlfn.IFS(D19=1,"Confident Republican",D19=2,"Likely Republican",D19=3,"Model Republican", D19=4,"Model Democrat", D19=5,"Likely Democrat",D19=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F19" s="19">
         <v>37.839333000000003</v>
       </c>
-      <c r="F19" s="19">
+      <c r="G19" s="19">
         <v>-84.270017999999993</v>
       </c>
-      <c r="K19" s="2" t="str" cm="1">
-        <f t="array" ref="K19">_xlfn.IFS(ISBLANK(D19),"SwingState",D19 = 3, "Model Rep",D19=4,"Model Dem",D19&lt;3,"R",D19&gt;3,"D")</f>
+      <c r="L19" s="2" t="str" cm="1">
+        <f t="array" ref="L19">_xlfn.IFS(ISBLANK(D19),"SwingState",D19 = 3, "Model Rep",D19=4,"Model Dem",D19&lt;3,"R",D19&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="U19" s="17"/>
       <c r="V19" s="17"/>
       <c r="W19" s="17"/>
       <c r="X19" s="17"/>
-    </row>
-    <row r="20" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y19" s="17"/>
+    </row>
+    <row r="20" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="str" cm="1">
         <f t="array" ref="A20">_xlfn.IFS(ISBLANK(D20),"SwingState",D20 = 3, "SwingState",D20=4,"SwingState",D20&lt;3,"R",D20&gt;3,"D")</f>
         <v>R</v>
@@ -40168,28 +40268,32 @@
       <c r="B20" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="21">
         <v>8</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="2" t="str" cm="1">
+        <f t="array" ref="E20">_xlfn.IFS(D20=1,"Confident Republican",D20=2,"Likely Republican",D20=3,"Model Republican", D20=4,"Model Democrat", D20=5,"Likely Democrat",D20=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F20" s="19">
         <v>31.244823</v>
       </c>
-      <c r="F20" s="19">
+      <c r="G20" s="19">
         <v>-92.145024000000006</v>
       </c>
-      <c r="K20" s="2" t="str" cm="1">
-        <f t="array" ref="K20">_xlfn.IFS(ISBLANK(D20),"SwingState",D20 = 3, "Model Rep",D20=4,"Model Dem",D20&lt;3,"R",D20&gt;3,"D")</f>
+      <c r="L20" s="2" t="str" cm="1">
+        <f t="array" ref="L20">_xlfn.IFS(ISBLANK(D20),"SwingState",D20 = 3, "Model Rep",D20=4,"Model Dem",D20&lt;3,"R",D20&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="U20" s="17"/>
       <c r="V20" s="17"/>
       <c r="W20" s="17"/>
       <c r="X20" s="17"/>
-    </row>
-    <row r="21" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y20" s="17"/>
+    </row>
+    <row r="21" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="str" cm="1">
         <f t="array" ref="A21">_xlfn.IFS(ISBLANK(D21),"SwingState",D21 = 3, "SwingState",D21=4,"SwingState",D21&lt;3,"R",D21&gt;3,"D")</f>
         <v>D</v>
@@ -40197,28 +40301,32 @@
       <c r="B21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="21">
         <v>4</v>
       </c>
       <c r="D21" s="2">
         <v>5</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="2" t="str" cm="1">
+        <f t="array" ref="E21">_xlfn.IFS(D21=1,"Confident Republican",D21=2,"Likely Republican",D21=3,"Model Republican", D21=4,"Model Democrat", D21=5,"Likely Democrat",D21=6,"Confident Democrat")</f>
+        <v>Likely Democrat</v>
+      </c>
+      <c r="F21" s="19">
         <v>45.253782999999999</v>
       </c>
-      <c r="F21" s="19">
+      <c r="G21" s="19">
         <v>-69.445469000000003</v>
       </c>
-      <c r="K21" s="2" t="str" cm="1">
-        <f t="array" ref="K21">_xlfn.IFS(ISBLANK(D21),"SwingState",D21 = 3, "Model Rep",D21=4,"Model Dem",D21&lt;3,"R",D21&gt;3,"D")</f>
+      <c r="L21" s="2" t="str" cm="1">
+        <f t="array" ref="L21">_xlfn.IFS(ISBLANK(D21),"SwingState",D21 = 3, "Model Rep",D21=4,"Model Dem",D21&lt;3,"R",D21&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="U21" s="17"/>
       <c r="V21" s="17"/>
       <c r="W21" s="17"/>
       <c r="X21" s="17"/>
-    </row>
-    <row r="22" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y21" s="17"/>
+    </row>
+    <row r="22" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="str" cm="1">
         <f t="array" ref="A22">_xlfn.IFS(ISBLANK(D22),"SwingState",D22 = 3, "SwingState",D22=4,"SwingState",D22&lt;3,"R",D22&gt;3,"D")</f>
         <v>D</v>
@@ -40226,28 +40334,32 @@
       <c r="B22" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="21">
         <v>10</v>
       </c>
       <c r="D22" s="2">
         <v>6</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="2" t="str" cm="1">
+        <f t="array" ref="E22">_xlfn.IFS(D22=1,"Confident Republican",D22=2,"Likely Republican",D22=3,"Model Republican", D22=4,"Model Democrat", D22=5,"Likely Democrat",D22=6,"Confident Democrat")</f>
+        <v>Confident Democrat</v>
+      </c>
+      <c r="F22" s="19">
         <v>39.045755</v>
       </c>
-      <c r="F22" s="19">
+      <c r="G22" s="19">
         <v>-76.641271000000003</v>
       </c>
-      <c r="K22" s="2" t="str" cm="1">
-        <f t="array" ref="K22">_xlfn.IFS(ISBLANK(D22),"SwingState",D22 = 3, "Model Rep",D22=4,"Model Dem",D22&lt;3,"R",D22&gt;3,"D")</f>
+      <c r="L22" s="2" t="str" cm="1">
+        <f t="array" ref="L22">_xlfn.IFS(ISBLANK(D22),"SwingState",D22 = 3, "Model Rep",D22=4,"Model Dem",D22&lt;3,"R",D22&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="U22" s="17"/>
       <c r="V22" s="17"/>
       <c r="W22" s="17"/>
       <c r="X22" s="17"/>
-    </row>
-    <row r="23" spans="1:24" ht="29" x14ac:dyDescent="0.2">
+      <c r="Y22" s="17"/>
+    </row>
+    <row r="23" spans="1:25" ht="29" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="str" cm="1">
         <f t="array" ref="A23">_xlfn.IFS(ISBLANK(D23),"SwingState",D23 = 3, "SwingState",D23=4,"SwingState",D23&lt;3,"R",D23&gt;3,"D")</f>
         <v>D</v>
@@ -40255,28 +40367,32 @@
       <c r="B23" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="21">
         <v>11</v>
       </c>
       <c r="D23" s="2">
         <v>6</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="2" t="str" cm="1">
+        <f t="array" ref="E23">_xlfn.IFS(D23=1,"Confident Republican",D23=2,"Likely Republican",D23=3,"Model Republican", D23=4,"Model Democrat", D23=5,"Likely Democrat",D23=6,"Confident Democrat")</f>
+        <v>Confident Democrat</v>
+      </c>
+      <c r="F23" s="19">
         <v>42.407210999999997</v>
       </c>
-      <c r="F23" s="19">
+      <c r="G23" s="19">
         <v>-71.382436999999996</v>
       </c>
-      <c r="K23" s="2" t="str" cm="1">
-        <f t="array" ref="K23">_xlfn.IFS(ISBLANK(D23),"SwingState",D23 = 3, "Model Rep",D23=4,"Model Dem",D23&lt;3,"R",D23&gt;3,"D")</f>
+      <c r="L23" s="2" t="str" cm="1">
+        <f t="array" ref="L23">_xlfn.IFS(ISBLANK(D23),"SwingState",D23 = 3, "Model Rep",D23=4,"Model Dem",D23&lt;3,"R",D23&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="U23" s="17"/>
       <c r="V23" s="17"/>
       <c r="W23" s="17"/>
       <c r="X23" s="17"/>
-    </row>
-    <row r="24" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y23" s="17"/>
+    </row>
+    <row r="24" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="str" cm="1">
         <f t="array" ref="A24">_xlfn.IFS(ISBLANK(D24),"SwingState",D24 = 3, "SwingState",D24=4,"SwingState",D24&lt;3,"R",D24&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40284,28 +40400,32 @@
       <c r="B24" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="21">
         <v>16</v>
       </c>
       <c r="D24" s="2">
         <v>4</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="2" t="str" cm="1">
+        <f t="array" ref="E24">_xlfn.IFS(D24=1,"Confident Republican",D24=2,"Likely Republican",D24=3,"Model Republican", D24=4,"Model Democrat", D24=5,"Likely Democrat",D24=6,"Confident Democrat")</f>
+        <v>Model Democrat</v>
+      </c>
+      <c r="F24" s="19">
         <v>44.314844000000001</v>
       </c>
-      <c r="F24" s="19">
+      <c r="G24" s="19">
         <v>-85.602363999999994</v>
       </c>
-      <c r="K24" s="2" t="str" cm="1">
-        <f t="array" ref="K24">_xlfn.IFS(ISBLANK(D24),"SwingState",D24 = 3, "Model Rep",D24=4,"Model Dem",D24&lt;3,"R",D24&gt;3,"D")</f>
+      <c r="L24" s="2" t="str" cm="1">
+        <f t="array" ref="L24">_xlfn.IFS(ISBLANK(D24),"SwingState",D24 = 3, "Model Rep",D24=4,"Model Dem",D24&lt;3,"R",D24&gt;3,"D")</f>
         <v>Model Dem</v>
       </c>
-      <c r="U24" s="17"/>
       <c r="V24" s="17"/>
       <c r="W24" s="17"/>
       <c r="X24" s="17"/>
-    </row>
-    <row r="25" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y24" s="17"/>
+    </row>
+    <row r="25" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="str" cm="1">
         <f t="array" ref="A25">_xlfn.IFS(ISBLANK(D25),"SwingState",D25 = 3, "SwingState",D25=4,"SwingState",D25&lt;3,"R",D25&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40313,28 +40433,32 @@
       <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="21">
         <v>10</v>
       </c>
       <c r="D25" s="2">
         <v>4</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="2" t="str" cm="1">
+        <f t="array" ref="E25">_xlfn.IFS(D25=1,"Confident Republican",D25=2,"Likely Republican",D25=3,"Model Republican", D25=4,"Model Democrat", D25=5,"Likely Democrat",D25=6,"Confident Democrat")</f>
+        <v>Model Democrat</v>
+      </c>
+      <c r="F25" s="19">
         <v>46.729553000000003</v>
       </c>
-      <c r="F25" s="19">
+      <c r="G25" s="19">
         <v>-94.685900000000004</v>
       </c>
-      <c r="K25" s="2" t="str" cm="1">
-        <f t="array" ref="K25">_xlfn.IFS(ISBLANK(D25),"SwingState",D25 = 3, "Model Rep",D25=4,"Model Dem",D25&lt;3,"R",D25&gt;3,"D")</f>
+      <c r="L25" s="2" t="str" cm="1">
+        <f t="array" ref="L25">_xlfn.IFS(ISBLANK(D25),"SwingState",D25 = 3, "Model Rep",D25=4,"Model Dem",D25&lt;3,"R",D25&gt;3,"D")</f>
         <v>Model Dem</v>
       </c>
-      <c r="U25" s="17"/>
       <c r="V25" s="17"/>
       <c r="W25" s="17"/>
       <c r="X25" s="17"/>
-    </row>
-    <row r="26" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y25" s="17"/>
+    </row>
+    <row r="26" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="str" cm="1">
         <f t="array" ref="A26">_xlfn.IFS(ISBLANK(D26),"SwingState",D26 = 3, "SwingState",D26=4,"SwingState",D26&lt;3,"R",D26&gt;3,"D")</f>
         <v>R</v>
@@ -40342,28 +40466,32 @@
       <c r="B26" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="21">
         <v>6</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
       </c>
-      <c r="E26" s="19">
+      <c r="E26" s="2" t="str" cm="1">
+        <f t="array" ref="E26">_xlfn.IFS(D26=1,"Confident Republican",D26=2,"Likely Republican",D26=3,"Model Republican", D26=4,"Model Democrat", D26=5,"Likely Democrat",D26=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F26" s="19">
         <v>32.354667999999997</v>
       </c>
-      <c r="F26" s="19">
+      <c r="G26" s="19">
         <v>-89.398527999999999</v>
       </c>
-      <c r="K26" s="2" t="str" cm="1">
-        <f t="array" ref="K26">_xlfn.IFS(ISBLANK(D26),"SwingState",D26 = 3, "Model Rep",D26=4,"Model Dem",D26&lt;3,"R",D26&gt;3,"D")</f>
+      <c r="L26" s="2" t="str" cm="1">
+        <f t="array" ref="L26">_xlfn.IFS(ISBLANK(D26),"SwingState",D26 = 3, "Model Rep",D26=4,"Model Dem",D26&lt;3,"R",D26&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="U26" s="17"/>
       <c r="V26" s="17"/>
       <c r="W26" s="17"/>
       <c r="X26" s="17"/>
-    </row>
-    <row r="27" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y26" s="17"/>
+    </row>
+    <row r="27" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="str" cm="1">
         <f t="array" ref="A27">_xlfn.IFS(ISBLANK(D27),"SwingState",D27 = 3, "SwingState",D27=4,"SwingState",D27&lt;3,"R",D27&gt;3,"D")</f>
         <v>R</v>
@@ -40371,28 +40499,32 @@
       <c r="B27" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="2">
-        <v>6</v>
+      <c r="C27" s="21">
+        <v>10</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E27" s="2" t="str" cm="1">
+        <f t="array" ref="E27">_xlfn.IFS(D27=1,"Confident Republican",D27=2,"Likely Republican",D27=3,"Model Republican", D27=4,"Model Democrat", D27=5,"Likely Democrat",D27=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F27" s="19">
         <v>37.964252999999999</v>
       </c>
-      <c r="F27" s="19">
+      <c r="G27" s="19">
         <v>-91.831833000000003</v>
       </c>
-      <c r="K27" s="2" t="str" cm="1">
-        <f t="array" ref="K27">_xlfn.IFS(ISBLANK(D27),"SwingState",D27 = 3, "Model Rep",D27=4,"Model Dem",D27&lt;3,"R",D27&gt;3,"D")</f>
+      <c r="L27" s="2" t="str" cm="1">
+        <f t="array" ref="L27">_xlfn.IFS(ISBLANK(D27),"SwingState",D27 = 3, "Model Rep",D27=4,"Model Dem",D27&lt;3,"R",D27&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="U27" s="17"/>
       <c r="V27" s="17"/>
       <c r="W27" s="17"/>
       <c r="X27" s="17"/>
-    </row>
-    <row r="28" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y27" s="17"/>
+    </row>
+    <row r="28" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="str" cm="1">
         <f t="array" ref="A28">_xlfn.IFS(ISBLANK(D28),"SwingState",D28 = 3, "SwingState",D28=4,"SwingState",D28&lt;3,"R",D28&gt;3,"D")</f>
         <v>R</v>
@@ -40400,28 +40532,32 @@
       <c r="B28" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="2">
-        <v>10</v>
+      <c r="C28" s="21">
+        <v>3</v>
       </c>
       <c r="D28" s="2">
         <v>1</v>
       </c>
-      <c r="E28" s="19">
+      <c r="E28" s="2" t="str" cm="1">
+        <f t="array" ref="E28">_xlfn.IFS(D28=1,"Confident Republican",D28=2,"Likely Republican",D28=3,"Model Republican", D28=4,"Model Democrat", D28=5,"Likely Democrat",D28=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F28" s="19">
         <v>46.879682000000003</v>
       </c>
-      <c r="F28" s="19">
+      <c r="G28" s="19">
         <v>-110.362566</v>
       </c>
-      <c r="K28" s="2" t="str" cm="1">
-        <f t="array" ref="K28">_xlfn.IFS(ISBLANK(D28),"SwingState",D28 = 3, "Model Rep",D28=4,"Model Dem",D28&lt;3,"R",D28&gt;3,"D")</f>
+      <c r="L28" s="2" t="str" cm="1">
+        <f t="array" ref="L28">_xlfn.IFS(ISBLANK(D28),"SwingState",D28 = 3, "Model Rep",D28=4,"Model Dem",D28&lt;3,"R",D28&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="U28" s="17"/>
       <c r="V28" s="17"/>
       <c r="W28" s="17"/>
       <c r="X28" s="17"/>
-    </row>
-    <row r="29" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y28" s="17"/>
+    </row>
+    <row r="29" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="str" cm="1">
         <f t="array" ref="A29">_xlfn.IFS(ISBLANK(D29),"SwingState",D29 = 3, "SwingState",D29=4,"SwingState",D29&lt;3,"R",D29&gt;3,"D")</f>
         <v>R</v>
@@ -40429,28 +40565,32 @@
       <c r="B29" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="21">
         <v>5</v>
       </c>
       <c r="D29" s="2">
         <v>1</v>
       </c>
-      <c r="E29" s="19">
+      <c r="E29" s="2" t="str" cm="1">
+        <f t="array" ref="E29">_xlfn.IFS(D29=1,"Confident Republican",D29=2,"Likely Republican",D29=3,"Model Republican", D29=4,"Model Democrat", D29=5,"Likely Democrat",D29=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F29" s="19">
         <v>41.492536999999999</v>
       </c>
-      <c r="F29" s="19">
+      <c r="G29" s="19">
         <v>-99.901813000000004</v>
       </c>
-      <c r="K29" s="2" t="str" cm="1">
-        <f t="array" ref="K29">_xlfn.IFS(ISBLANK(D29),"SwingState",D29 = 3, "Model Rep",D29=4,"Model Dem",D29&lt;3,"R",D29&gt;3,"D")</f>
+      <c r="L29" s="2" t="str" cm="1">
+        <f t="array" ref="L29">_xlfn.IFS(ISBLANK(D29),"SwingState",D29 = 3, "Model Rep",D29=4,"Model Dem",D29&lt;3,"R",D29&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="U29" s="17"/>
       <c r="V29" s="17"/>
       <c r="W29" s="17"/>
       <c r="X29" s="17"/>
-    </row>
-    <row r="30" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y29" s="17"/>
+    </row>
+    <row r="30" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="str" cm="1">
         <f t="array" ref="A30">_xlfn.IFS(ISBLANK(D30),"SwingState",D30 = 3, "SwingState",D30=4,"SwingState",D30&lt;3,"R",D30&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40458,28 +40598,32 @@
       <c r="B30" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="21">
         <v>6</v>
       </c>
       <c r="D30" s="2">
         <v>4</v>
       </c>
-      <c r="E30" s="19">
+      <c r="E30" s="2" t="str" cm="1">
+        <f t="array" ref="E30">_xlfn.IFS(D30=1,"Confident Republican",D30=2,"Likely Republican",D30=3,"Model Republican", D30=4,"Model Democrat", D30=5,"Likely Democrat",D30=6,"Confident Democrat")</f>
+        <v>Model Democrat</v>
+      </c>
+      <c r="F30" s="19">
         <v>38.802610000000001</v>
       </c>
-      <c r="F30" s="19">
+      <c r="G30" s="19">
         <v>-116.419389</v>
       </c>
-      <c r="K30" s="2" t="str" cm="1">
-        <f t="array" ref="K30">_xlfn.IFS(ISBLANK(D30),"SwingState",D30 = 3, "Model Rep",D30=4,"Model Dem",D30&lt;3,"R",D30&gt;3,"D")</f>
+      <c r="L30" s="2" t="str" cm="1">
+        <f t="array" ref="L30">_xlfn.IFS(ISBLANK(D30),"SwingState",D30 = 3, "Model Rep",D30=4,"Model Dem",D30&lt;3,"R",D30&gt;3,"D")</f>
         <v>Model Dem</v>
       </c>
-      <c r="U30" s="17"/>
       <c r="V30" s="17"/>
       <c r="W30" s="17"/>
       <c r="X30" s="17"/>
-    </row>
-    <row r="31" spans="1:24" ht="29" x14ac:dyDescent="0.2">
+      <c r="Y30" s="17"/>
+    </row>
+    <row r="31" spans="1:25" ht="29" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="str" cm="1">
         <f t="array" ref="A31">_xlfn.IFS(ISBLANK(D31),"SwingState",D31 = 3, "SwingState",D31=4,"SwingState",D31&lt;3,"R",D31&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40487,28 +40631,32 @@
       <c r="B31" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="21">
         <v>4</v>
       </c>
       <c r="D31" s="2">
         <v>4</v>
       </c>
-      <c r="E31" s="19">
+      <c r="E31" s="2" t="str" cm="1">
+        <f t="array" ref="E31">_xlfn.IFS(D31=1,"Confident Republican",D31=2,"Likely Republican",D31=3,"Model Republican", D31=4,"Model Democrat", D31=5,"Likely Democrat",D31=6,"Confident Democrat")</f>
+        <v>Model Democrat</v>
+      </c>
+      <c r="F31" s="19">
         <v>43.193852</v>
       </c>
-      <c r="F31" s="19">
+      <c r="G31" s="19">
         <v>-71.572395</v>
       </c>
-      <c r="K31" s="2" t="str" cm="1">
-        <f t="array" ref="K31">_xlfn.IFS(ISBLANK(D31),"SwingState",D31 = 3, "Model Rep",D31=4,"Model Dem",D31&lt;3,"R",D31&gt;3,"D")</f>
+      <c r="L31" s="2" t="str" cm="1">
+        <f t="array" ref="L31">_xlfn.IFS(ISBLANK(D31),"SwingState",D31 = 3, "Model Rep",D31=4,"Model Dem",D31&lt;3,"R",D31&gt;3,"D")</f>
         <v>Model Dem</v>
       </c>
-      <c r="U31" s="17"/>
       <c r="V31" s="17"/>
       <c r="W31" s="17"/>
       <c r="X31" s="17"/>
-    </row>
-    <row r="32" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y31" s="17"/>
+    </row>
+    <row r="32" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="str" cm="1">
         <f t="array" ref="A32">_xlfn.IFS(ISBLANK(D32),"SwingState",D32 = 3, "SwingState",D32=4,"SwingState",D32&lt;3,"R",D32&gt;3,"D")</f>
         <v>D</v>
@@ -40516,28 +40664,32 @@
       <c r="B32" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="21">
         <v>14</v>
       </c>
       <c r="D32" s="2">
         <v>6</v>
       </c>
-      <c r="E32" s="19">
+      <c r="E32" s="2" t="str" cm="1">
+        <f t="array" ref="E32">_xlfn.IFS(D32=1,"Confident Republican",D32=2,"Likely Republican",D32=3,"Model Republican", D32=4,"Model Democrat", D32=5,"Likely Democrat",D32=6,"Confident Democrat")</f>
+        <v>Confident Democrat</v>
+      </c>
+      <c r="F32" s="19">
         <v>40.058323999999999</v>
       </c>
-      <c r="F32" s="19">
+      <c r="G32" s="19">
         <v>-74.405660999999995</v>
       </c>
-      <c r="K32" s="2" t="str" cm="1">
-        <f t="array" ref="K32">_xlfn.IFS(ISBLANK(D32),"SwingState",D32 = 3, "Model Rep",D32=4,"Model Dem",D32&lt;3,"R",D32&gt;3,"D")</f>
+      <c r="L32" s="2" t="str" cm="1">
+        <f t="array" ref="L32">_xlfn.IFS(ISBLANK(D32),"SwingState",D32 = 3, "Model Rep",D32=4,"Model Dem",D32&lt;3,"R",D32&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="U32" s="17"/>
       <c r="V32" s="17"/>
       <c r="W32" s="17"/>
       <c r="X32" s="17"/>
-    </row>
-    <row r="33" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y32" s="17"/>
+    </row>
+    <row r="33" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="str" cm="1">
         <f t="array" ref="A33">_xlfn.IFS(ISBLANK(D33),"SwingState",D33 = 3, "SwingState",D33=4,"SwingState",D33&lt;3,"R",D33&gt;3,"D")</f>
         <v>D</v>
@@ -40545,28 +40697,32 @@
       <c r="B33" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="21">
         <v>5</v>
       </c>
       <c r="D33" s="2">
         <v>6</v>
       </c>
-      <c r="E33" s="19">
+      <c r="E33" s="2" t="str" cm="1">
+        <f t="array" ref="E33">_xlfn.IFS(D33=1,"Confident Republican",D33=2,"Likely Republican",D33=3,"Model Republican", D33=4,"Model Democrat", D33=5,"Likely Democrat",D33=6,"Confident Democrat")</f>
+        <v>Confident Democrat</v>
+      </c>
+      <c r="F33" s="19">
         <v>34.972729999999999</v>
       </c>
-      <c r="F33" s="19">
+      <c r="G33" s="19">
         <v>-105.032363</v>
       </c>
-      <c r="K33" s="2" t="str" cm="1">
-        <f t="array" ref="K33">_xlfn.IFS(ISBLANK(D33),"SwingState",D33 = 3, "Model Rep",D33=4,"Model Dem",D33&lt;3,"R",D33&gt;3,"D")</f>
+      <c r="L33" s="2" t="str" cm="1">
+        <f t="array" ref="L33">_xlfn.IFS(ISBLANK(D33),"SwingState",D33 = 3, "Model Rep",D33=4,"Model Dem",D33&lt;3,"R",D33&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="U33" s="17"/>
       <c r="V33" s="17"/>
       <c r="W33" s="17"/>
       <c r="X33" s="17"/>
-    </row>
-    <row r="34" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y33" s="17"/>
+    </row>
+    <row r="34" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="str" cm="1">
         <f t="array" ref="A34">_xlfn.IFS(ISBLANK(D34),"SwingState",D34 = 3, "SwingState",D34=4,"SwingState",D34&lt;3,"R",D34&gt;3,"D")</f>
         <v>D</v>
@@ -40574,28 +40730,32 @@
       <c r="B34" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="21">
         <v>29</v>
       </c>
       <c r="D34" s="2">
         <v>6</v>
       </c>
-      <c r="E34" s="19">
+      <c r="E34" s="2" t="str" cm="1">
+        <f t="array" ref="E34">_xlfn.IFS(D34=1,"Confident Republican",D34=2,"Likely Republican",D34=3,"Model Republican", D34=4,"Model Democrat", D34=5,"Likely Democrat",D34=6,"Confident Democrat")</f>
+        <v>Confident Democrat</v>
+      </c>
+      <c r="F34" s="19">
         <v>43.299427999999999</v>
       </c>
-      <c r="F34" s="19">
+      <c r="G34" s="19">
         <v>-74.217933000000002</v>
       </c>
-      <c r="K34" s="2" t="str" cm="1">
-        <f t="array" ref="K34">_xlfn.IFS(ISBLANK(D34),"SwingState",D34 = 3, "Model Rep",D34=4,"Model Dem",D34&lt;3,"R",D34&gt;3,"D")</f>
+      <c r="L34" s="2" t="str" cm="1">
+        <f t="array" ref="L34">_xlfn.IFS(ISBLANK(D34),"SwingState",D34 = 3, "Model Rep",D34=4,"Model Dem",D34&lt;3,"R",D34&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="U34" s="17"/>
       <c r="V34" s="17"/>
       <c r="W34" s="17"/>
       <c r="X34" s="17"/>
-    </row>
-    <row r="35" spans="1:24" ht="29" x14ac:dyDescent="0.2">
+      <c r="Y34" s="17"/>
+    </row>
+    <row r="35" spans="1:25" ht="29" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="str" cm="1">
         <f t="array" ref="A35">_xlfn.IFS(ISBLANK(D35),"SwingState",D35 = 3, "SwingState",D35=4,"SwingState",D35&lt;3,"R",D35&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40603,28 +40763,32 @@
       <c r="B35" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="21">
         <v>15</v>
       </c>
       <c r="D35" s="2">
         <v>3</v>
       </c>
-      <c r="E35" s="19">
+      <c r="E35" s="2" t="str" cm="1">
+        <f t="array" ref="E35">_xlfn.IFS(D35=1,"Confident Republican",D35=2,"Likely Republican",D35=3,"Model Republican", D35=4,"Model Democrat", D35=5,"Likely Democrat",D35=6,"Confident Democrat")</f>
+        <v>Model Republican</v>
+      </c>
+      <c r="F35" s="19">
         <v>35.759573000000003</v>
       </c>
-      <c r="F35" s="19">
+      <c r="G35" s="19">
         <v>-79.019300000000001</v>
       </c>
-      <c r="K35" s="2" t="str" cm="1">
-        <f t="array" ref="K35">_xlfn.IFS(ISBLANK(D35),"SwingState",D35 = 3, "Model Rep",D35=4,"Model Dem",D35&lt;3,"R",D35&gt;3,"D")</f>
+      <c r="L35" s="2" t="str" cm="1">
+        <f t="array" ref="L35">_xlfn.IFS(ISBLANK(D35),"SwingState",D35 = 3, "Model Rep",D35=4,"Model Dem",D35&lt;3,"R",D35&gt;3,"D")</f>
         <v>Model Rep</v>
       </c>
-      <c r="U35" s="17"/>
       <c r="V35" s="17"/>
       <c r="W35" s="17"/>
       <c r="X35" s="17"/>
-    </row>
-    <row r="36" spans="1:24" ht="29" x14ac:dyDescent="0.2">
+      <c r="Y35" s="17"/>
+    </row>
+    <row r="36" spans="1:25" ht="29" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="str" cm="1">
         <f t="array" ref="A36">_xlfn.IFS(ISBLANK(D36),"SwingState",D36 = 3, "SwingState",D36=4,"SwingState",D36&lt;3,"R",D36&gt;3,"D")</f>
         <v>R</v>
@@ -40632,28 +40796,32 @@
       <c r="B36" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="21">
         <v>3</v>
       </c>
       <c r="D36" s="2">
         <v>1</v>
       </c>
-      <c r="E36" s="19">
+      <c r="E36" s="2" t="str" cm="1">
+        <f t="array" ref="E36">_xlfn.IFS(D36=1,"Confident Republican",D36=2,"Likely Republican",D36=3,"Model Republican", D36=4,"Model Democrat", D36=5,"Likely Democrat",D36=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F36" s="19">
         <v>47.551493000000001</v>
       </c>
-      <c r="F36" s="19">
+      <c r="G36" s="19">
         <v>-101.00201199999999</v>
       </c>
-      <c r="K36" s="2" t="str" cm="1">
-        <f t="array" ref="K36">_xlfn.IFS(ISBLANK(D36),"SwingState",D36 = 3, "Model Rep",D36=4,"Model Dem",D36&lt;3,"R",D36&gt;3,"D")</f>
+      <c r="L36" s="2" t="str" cm="1">
+        <f t="array" ref="L36">_xlfn.IFS(ISBLANK(D36),"SwingState",D36 = 3, "Model Rep",D36=4,"Model Dem",D36&lt;3,"R",D36&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="U36" s="17"/>
       <c r="V36" s="17"/>
       <c r="W36" s="17"/>
       <c r="X36" s="17"/>
-    </row>
-    <row r="37" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y36" s="17"/>
+    </row>
+    <row r="37" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="str" cm="1">
         <f t="array" ref="A37">_xlfn.IFS(ISBLANK(D37),"SwingState",D37 = 3, "SwingState",D37=4,"SwingState",D37&lt;3,"R",D37&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40661,28 +40829,32 @@
       <c r="B37" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="21">
         <v>18</v>
       </c>
       <c r="D37" s="2">
         <v>4</v>
       </c>
-      <c r="E37" s="19">
+      <c r="E37" s="2" t="str" cm="1">
+        <f t="array" ref="E37">_xlfn.IFS(D37=1,"Confident Republican",D37=2,"Likely Republican",D37=3,"Model Republican", D37=4,"Model Democrat", D37=5,"Likely Democrat",D37=6,"Confident Democrat")</f>
+        <v>Model Democrat</v>
+      </c>
+      <c r="F37" s="19">
         <v>40.417287000000002</v>
       </c>
-      <c r="F37" s="19">
+      <c r="G37" s="19">
         <v>-82.907122999999999</v>
       </c>
-      <c r="K37" s="2" t="str" cm="1">
-        <f t="array" ref="K37">_xlfn.IFS(ISBLANK(D37),"SwingState",D37 = 3, "Model Rep",D37=4,"Model Dem",D37&lt;3,"R",D37&gt;3,"D")</f>
+      <c r="L37" s="2" t="str" cm="1">
+        <f t="array" ref="L37">_xlfn.IFS(ISBLANK(D37),"SwingState",D37 = 3, "Model Rep",D37=4,"Model Dem",D37&lt;3,"R",D37&gt;3,"D")</f>
         <v>Model Dem</v>
       </c>
-      <c r="U37" s="17"/>
       <c r="V37" s="17"/>
       <c r="W37" s="17"/>
       <c r="X37" s="17"/>
-    </row>
-    <row r="38" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y37" s="17"/>
+    </row>
+    <row r="38" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="str" cm="1">
         <f t="array" ref="A38">_xlfn.IFS(ISBLANK(D38),"SwingState",D38 = 3, "SwingState",D38=4,"SwingState",D38&lt;3,"R",D38&gt;3,"D")</f>
         <v>R</v>
@@ -40690,28 +40862,32 @@
       <c r="B38" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="21">
         <v>7</v>
       </c>
       <c r="D38" s="2">
         <v>1</v>
       </c>
-      <c r="E38" s="19">
+      <c r="E38" s="2" t="str" cm="1">
+        <f t="array" ref="E38">_xlfn.IFS(D38=1,"Confident Republican",D38=2,"Likely Republican",D38=3,"Model Republican", D38=4,"Model Democrat", D38=5,"Likely Democrat",D38=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F38" s="19">
         <v>35.007752000000004</v>
       </c>
-      <c r="F38" s="19">
+      <c r="G38" s="19">
         <v>-97.092877000000001</v>
       </c>
-      <c r="K38" s="2" t="str" cm="1">
-        <f t="array" ref="K38">_xlfn.IFS(ISBLANK(D38),"SwingState",D38 = 3, "Model Rep",D38=4,"Model Dem",D38&lt;3,"R",D38&gt;3,"D")</f>
+      <c r="L38" s="2" t="str" cm="1">
+        <f t="array" ref="L38">_xlfn.IFS(ISBLANK(D38),"SwingState",D38 = 3, "Model Rep",D38=4,"Model Dem",D38&lt;3,"R",D38&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="U38" s="17"/>
       <c r="V38" s="17"/>
       <c r="W38" s="17"/>
       <c r="X38" s="17"/>
-    </row>
-    <row r="39" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y38" s="17"/>
+    </row>
+    <row r="39" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="str" cm="1">
         <f t="array" ref="A39">_xlfn.IFS(ISBLANK(D39),"SwingState",D39 = 3, "SwingState",D39=4,"SwingState",D39&lt;3,"R",D39&gt;3,"D")</f>
         <v>D</v>
@@ -40719,28 +40895,32 @@
       <c r="B39" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="21">
         <v>7</v>
       </c>
       <c r="D39" s="2">
         <v>6</v>
       </c>
-      <c r="E39" s="19">
+      <c r="E39" s="2" t="str" cm="1">
+        <f t="array" ref="E39">_xlfn.IFS(D39=1,"Confident Republican",D39=2,"Likely Republican",D39=3,"Model Republican", D39=4,"Model Democrat", D39=5,"Likely Democrat",D39=6,"Confident Democrat")</f>
+        <v>Confident Democrat</v>
+      </c>
+      <c r="F39" s="19">
         <v>43.804133</v>
       </c>
-      <c r="F39" s="19">
+      <c r="G39" s="19">
         <v>-120.55420100000001</v>
       </c>
-      <c r="K39" s="2" t="str" cm="1">
-        <f t="array" ref="K39">_xlfn.IFS(ISBLANK(D39),"SwingState",D39 = 3, "Model Rep",D39=4,"Model Dem",D39&lt;3,"R",D39&gt;3,"D")</f>
+      <c r="L39" s="2" t="str" cm="1">
+        <f t="array" ref="L39">_xlfn.IFS(ISBLANK(D39),"SwingState",D39 = 3, "Model Rep",D39=4,"Model Dem",D39&lt;3,"R",D39&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="U39" s="17"/>
       <c r="V39" s="17"/>
       <c r="W39" s="17"/>
       <c r="X39" s="17"/>
-    </row>
-    <row r="40" spans="1:24" ht="29" x14ac:dyDescent="0.2">
+      <c r="Y39" s="17"/>
+    </row>
+    <row r="40" spans="1:25" ht="29" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="str" cm="1">
         <f t="array" ref="A40">_xlfn.IFS(ISBLANK(D40),"SwingState",D40 = 3, "SwingState",D40=4,"SwingState",D40&lt;3,"R",D40&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40748,28 +40928,32 @@
       <c r="B40" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="21">
         <v>20</v>
       </c>
       <c r="D40" s="2">
         <v>3</v>
       </c>
-      <c r="E40" s="19">
+      <c r="E40" s="2" t="str" cm="1">
+        <f t="array" ref="E40">_xlfn.IFS(D40=1,"Confident Republican",D40=2,"Likely Republican",D40=3,"Model Republican", D40=4,"Model Democrat", D40=5,"Likely Democrat",D40=6,"Confident Democrat")</f>
+        <v>Model Republican</v>
+      </c>
+      <c r="F40" s="19">
         <v>41.203322</v>
       </c>
-      <c r="F40" s="19">
+      <c r="G40" s="19">
         <v>-77.194524999999999</v>
       </c>
-      <c r="K40" s="2" t="str" cm="1">
-        <f t="array" ref="K40">_xlfn.IFS(ISBLANK(D40),"SwingState",D40 = 3, "Model Rep",D40=4,"Model Dem",D40&lt;3,"R",D40&gt;3,"D")</f>
+      <c r="L40" s="2" t="str" cm="1">
+        <f t="array" ref="L40">_xlfn.IFS(ISBLANK(D40),"SwingState",D40 = 3, "Model Rep",D40=4,"Model Dem",D40&lt;3,"R",D40&gt;3,"D")</f>
         <v>Model Rep</v>
       </c>
-      <c r="U40" s="17"/>
       <c r="V40" s="17"/>
       <c r="W40" s="17"/>
       <c r="X40" s="17"/>
-    </row>
-    <row r="41" spans="1:24" ht="29" x14ac:dyDescent="0.2">
+      <c r="Y40" s="17"/>
+    </row>
+    <row r="41" spans="1:25" ht="29" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="str" cm="1">
         <f t="array" ref="A41">_xlfn.IFS(ISBLANK(D41),"SwingState",D41 = 3, "SwingState",D41=4,"SwingState",D41&lt;3,"R",D41&gt;3,"D")</f>
         <v>D</v>
@@ -40777,28 +40961,32 @@
       <c r="B41" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="21">
         <v>4</v>
       </c>
       <c r="D41" s="2">
         <v>6</v>
       </c>
-      <c r="E41" s="19">
+      <c r="E41" s="2" t="str" cm="1">
+        <f t="array" ref="E41">_xlfn.IFS(D41=1,"Confident Republican",D41=2,"Likely Republican",D41=3,"Model Republican", D41=4,"Model Democrat", D41=5,"Likely Democrat",D41=6,"Confident Democrat")</f>
+        <v>Confident Democrat</v>
+      </c>
+      <c r="F41" s="19">
         <v>18.220832999999999</v>
       </c>
-      <c r="F41" s="19">
+      <c r="G41" s="19">
         <v>-66.590148999999997</v>
       </c>
-      <c r="K41" s="2" t="str" cm="1">
-        <f t="array" ref="K41">_xlfn.IFS(ISBLANK(D41),"SwingState",D41 = 3, "Model Rep",D41=4,"Model Dem",D41&lt;3,"R",D41&gt;3,"D")</f>
+      <c r="L41" s="2" t="str" cm="1">
+        <f t="array" ref="L41">_xlfn.IFS(ISBLANK(D41),"SwingState",D41 = 3, "Model Rep",D41=4,"Model Dem",D41&lt;3,"R",D41&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="U41" s="17"/>
       <c r="V41" s="17"/>
       <c r="W41" s="17"/>
       <c r="X41" s="17"/>
-    </row>
-    <row r="42" spans="1:24" ht="29" x14ac:dyDescent="0.2">
+      <c r="Y41" s="17"/>
+    </row>
+    <row r="42" spans="1:25" ht="29" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="str" cm="1">
         <f t="array" ref="A42">_xlfn.IFS(ISBLANK(D42),"SwingState",D42 = 3, "SwingState",D42=4,"SwingState",D42&lt;3,"R",D42&gt;3,"D")</f>
         <v>R</v>
@@ -40806,28 +40994,32 @@
       <c r="B42" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="21">
         <v>9</v>
       </c>
       <c r="D42" s="2">
         <v>1</v>
       </c>
-      <c r="E42" s="19">
+      <c r="E42" s="2" t="str" cm="1">
+        <f t="array" ref="E42">_xlfn.IFS(D42=1,"Confident Republican",D42=2,"Likely Republican",D42=3,"Model Republican", D42=4,"Model Democrat", D42=5,"Likely Democrat",D42=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F42" s="19">
         <v>41.580095</v>
       </c>
-      <c r="F42" s="19">
+      <c r="G42" s="19">
         <v>-71.477429000000001</v>
       </c>
-      <c r="K42" s="2" t="str" cm="1">
-        <f t="array" ref="K42">_xlfn.IFS(ISBLANK(D42),"SwingState",D42 = 3, "Model Rep",D42=4,"Model Dem",D42&lt;3,"R",D42&gt;3,"D")</f>
+      <c r="L42" s="2" t="str" cm="1">
+        <f t="array" ref="L42">_xlfn.IFS(ISBLANK(D42),"SwingState",D42 = 3, "Model Rep",D42=4,"Model Dem",D42&lt;3,"R",D42&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="U42" s="17"/>
       <c r="V42" s="17"/>
       <c r="W42" s="17"/>
       <c r="X42" s="17"/>
-    </row>
-    <row r="43" spans="1:24" ht="29" x14ac:dyDescent="0.2">
+      <c r="Y42" s="17"/>
+    </row>
+    <row r="43" spans="1:25" ht="29" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="str" cm="1">
         <f t="array" ref="A43">_xlfn.IFS(ISBLANK(D43),"SwingState",D43 = 3, "SwingState",D43=4,"SwingState",D43&lt;3,"R",D43&gt;3,"D")</f>
         <v>R</v>
@@ -40835,28 +41027,32 @@
       <c r="B43" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="21">
         <v>3</v>
       </c>
       <c r="D43" s="2">
         <v>1</v>
       </c>
-      <c r="E43" s="19">
+      <c r="E43" s="2" t="str" cm="1">
+        <f t="array" ref="E43">_xlfn.IFS(D43=1,"Confident Republican",D43=2,"Likely Republican",D43=3,"Model Republican", D43=4,"Model Democrat", D43=5,"Likely Democrat",D43=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F43" s="19">
         <v>33.836081</v>
       </c>
-      <c r="F43" s="19">
+      <c r="G43" s="19">
         <v>-81.163724999999999</v>
       </c>
-      <c r="K43" s="2" t="str" cm="1">
-        <f t="array" ref="K43">_xlfn.IFS(ISBLANK(D43),"SwingState",D43 = 3, "Model Rep",D43=4,"Model Dem",D43&lt;3,"R",D43&gt;3,"D")</f>
+      <c r="L43" s="2" t="str" cm="1">
+        <f t="array" ref="L43">_xlfn.IFS(ISBLANK(D43),"SwingState",D43 = 3, "Model Rep",D43=4,"Model Dem",D43&lt;3,"R",D43&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="U43" s="17"/>
       <c r="V43" s="17"/>
       <c r="W43" s="17"/>
       <c r="X43" s="17"/>
-    </row>
-    <row r="44" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y43" s="17"/>
+    </row>
+    <row r="44" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="str" cm="1">
         <f t="array" ref="A44">_xlfn.IFS(ISBLANK(D44),"SwingState",D44 = 3, "SwingState",D44=4,"SwingState",D44&lt;3,"R",D44&gt;3,"D")</f>
         <v>R</v>
@@ -40864,28 +41060,32 @@
       <c r="B44" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="21">
         <v>11</v>
       </c>
       <c r="D44" s="2">
         <v>1</v>
       </c>
-      <c r="E44" s="19">
+      <c r="E44" s="2" t="str" cm="1">
+        <f t="array" ref="E44">_xlfn.IFS(D44=1,"Confident Republican",D44=2,"Likely Republican",D44=3,"Model Republican", D44=4,"Model Democrat", D44=5,"Likely Democrat",D44=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F44" s="19">
         <v>43.969515000000001</v>
       </c>
-      <c r="F44" s="19">
+      <c r="G44" s="19">
         <v>-99.901813000000004</v>
       </c>
-      <c r="K44" s="2" t="str" cm="1">
-        <f t="array" ref="K44">_xlfn.IFS(ISBLANK(D44),"SwingState",D44 = 3, "Model Rep",D44=4,"Model Dem",D44&lt;3,"R",D44&gt;3,"D")</f>
+      <c r="L44" s="2" t="str" cm="1">
+        <f t="array" ref="L44">_xlfn.IFS(ISBLANK(D44),"SwingState",D44 = 3, "Model Rep",D44=4,"Model Dem",D44&lt;3,"R",D44&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="U44" s="17"/>
       <c r="V44" s="17"/>
       <c r="W44" s="17"/>
       <c r="X44" s="17"/>
-    </row>
-    <row r="45" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y44" s="17"/>
+    </row>
+    <row r="45" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="str" cm="1">
         <f t="array" ref="A45">_xlfn.IFS(ISBLANK(D45),"SwingState",D45 = 3, "SwingState",D45=4,"SwingState",D45&lt;3,"R",D45&gt;3,"D")</f>
         <v>R</v>
@@ -40893,28 +41093,32 @@
       <c r="B45" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="21">
         <v>38</v>
       </c>
       <c r="D45" s="2">
         <v>1</v>
       </c>
-      <c r="E45" s="19">
+      <c r="E45" s="2" t="str" cm="1">
+        <f t="array" ref="E45">_xlfn.IFS(D45=1,"Confident Republican",D45=2,"Likely Republican",D45=3,"Model Republican", D45=4,"Model Democrat", D45=5,"Likely Democrat",D45=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F45" s="19">
         <v>35.517491</v>
       </c>
-      <c r="F45" s="19">
+      <c r="G45" s="19">
         <v>-86.580447000000007</v>
       </c>
-      <c r="K45" s="2" t="str" cm="1">
-        <f t="array" ref="K45">_xlfn.IFS(ISBLANK(D45),"SwingState",D45 = 3, "Model Rep",D45=4,"Model Dem",D45&lt;3,"R",D45&gt;3,"D")</f>
+      <c r="L45" s="2" t="str" cm="1">
+        <f t="array" ref="L45">_xlfn.IFS(ISBLANK(D45),"SwingState",D45 = 3, "Model Rep",D45=4,"Model Dem",D45&lt;3,"R",D45&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="U45" s="17"/>
       <c r="V45" s="17"/>
       <c r="W45" s="17"/>
       <c r="X45" s="17"/>
-    </row>
-    <row r="46" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y45" s="17"/>
+    </row>
+    <row r="46" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="str" cm="1">
         <f t="array" ref="A46">_xlfn.IFS(ISBLANK(D46),"SwingState",D46 = 3, "SwingState",D46=4,"SwingState",D46&lt;3,"R",D46&gt;3,"D")</f>
         <v>R</v>
@@ -40922,28 +41126,32 @@
       <c r="B46" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="21">
         <v>6</v>
       </c>
       <c r="D46" s="2">
         <v>1</v>
       </c>
-      <c r="E46" s="19">
+      <c r="E46" s="2" t="str" cm="1">
+        <f t="array" ref="E46">_xlfn.IFS(D46=1,"Confident Republican",D46=2,"Likely Republican",D46=3,"Model Republican", D46=4,"Model Democrat", D46=5,"Likely Democrat",D46=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F46" s="19">
         <v>31.968599000000001</v>
       </c>
-      <c r="F46" s="19">
+      <c r="G46" s="19">
         <v>-99.901813000000004</v>
       </c>
-      <c r="K46" s="2" t="str" cm="1">
-        <f t="array" ref="K46">_xlfn.IFS(ISBLANK(D46),"SwingState",D46 = 3, "Model Rep",D46=4,"Model Dem",D46&lt;3,"R",D46&gt;3,"D")</f>
+      <c r="L46" s="2" t="str" cm="1">
+        <f t="array" ref="L46">_xlfn.IFS(ISBLANK(D46),"SwingState",D46 = 3, "Model Rep",D46=4,"Model Dem",D46&lt;3,"R",D46&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="U46" s="17"/>
       <c r="V46" s="17"/>
       <c r="W46" s="17"/>
       <c r="X46" s="17"/>
-    </row>
-    <row r="47" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y46" s="17"/>
+    </row>
+    <row r="47" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="str" cm="1">
         <f t="array" ref="A47">_xlfn.IFS(ISBLANK(D47),"SwingState",D47 = 3, "SwingState",D47=4,"SwingState",D47&lt;3,"R",D47&gt;3,"D")</f>
         <v>D</v>
@@ -40951,28 +41159,32 @@
       <c r="B47" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="21">
         <v>3</v>
       </c>
       <c r="D47" s="2">
         <v>6</v>
       </c>
-      <c r="E47" s="19">
+      <c r="E47" s="2" t="str" cm="1">
+        <f t="array" ref="E47">_xlfn.IFS(D47=1,"Confident Republican",D47=2,"Likely Republican",D47=3,"Model Republican", D47=4,"Model Democrat", D47=5,"Likely Democrat",D47=6,"Confident Democrat")</f>
+        <v>Confident Democrat</v>
+      </c>
+      <c r="F47" s="19">
         <v>39.320979999999999</v>
       </c>
-      <c r="F47" s="19">
+      <c r="G47" s="19">
         <v>-111.09373100000001</v>
       </c>
-      <c r="K47" s="2" t="str" cm="1">
-        <f t="array" ref="K47">_xlfn.IFS(ISBLANK(D47),"SwingState",D47 = 3, "Model Rep",D47=4,"Model Dem",D47&lt;3,"R",D47&gt;3,"D")</f>
+      <c r="L47" s="2" t="str" cm="1">
+        <f t="array" ref="L47">_xlfn.IFS(ISBLANK(D47),"SwingState",D47 = 3, "Model Rep",D47=4,"Model Dem",D47&lt;3,"R",D47&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="U47" s="17"/>
       <c r="V47" s="17"/>
       <c r="W47" s="17"/>
       <c r="X47" s="17"/>
-    </row>
-    <row r="48" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y47" s="17"/>
+    </row>
+    <row r="48" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="str" cm="1">
         <f t="array" ref="A48">_xlfn.IFS(ISBLANK(D48),"SwingState",D48 = 3, "SwingState",D48=4,"SwingState",D48&lt;3,"R",D48&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40980,28 +41192,32 @@
       <c r="B48" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="21">
         <v>13</v>
       </c>
       <c r="D48" s="2">
         <v>4</v>
       </c>
-      <c r="E48" s="19">
+      <c r="E48" s="2" t="str" cm="1">
+        <f t="array" ref="E48">_xlfn.IFS(D48=1,"Confident Republican",D48=2,"Likely Republican",D48=3,"Model Republican", D48=4,"Model Democrat", D48=5,"Likely Democrat",D48=6,"Confident Democrat")</f>
+        <v>Model Democrat</v>
+      </c>
+      <c r="F48" s="19">
         <v>44.558802999999997</v>
       </c>
-      <c r="F48" s="19">
+      <c r="G48" s="19">
         <v>-72.577841000000006</v>
       </c>
-      <c r="K48" s="2" t="str" cm="1">
-        <f t="array" ref="K48">_xlfn.IFS(ISBLANK(D48),"SwingState",D48 = 3, "Model Rep",D48=4,"Model Dem",D48&lt;3,"R",D48&gt;3,"D")</f>
+      <c r="L48" s="2" t="str" cm="1">
+        <f t="array" ref="L48">_xlfn.IFS(ISBLANK(D48),"SwingState",D48 = 3, "Model Rep",D48=4,"Model Dem",D48&lt;3,"R",D48&gt;3,"D")</f>
         <v>Model Dem</v>
       </c>
-      <c r="U48" s="17"/>
       <c r="V48" s="17"/>
       <c r="W48" s="17"/>
       <c r="X48" s="17"/>
-    </row>
-    <row r="49" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y48" s="17"/>
+    </row>
+    <row r="49" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="str" cm="1">
         <f t="array" ref="A49">_xlfn.IFS(ISBLANK(D49),"SwingState",D49 = 3, "SwingState",D49=4,"SwingState",D49&lt;3,"R",D49&gt;3,"D")</f>
         <v>D</v>
@@ -41009,28 +41225,32 @@
       <c r="B49" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="21">
         <v>12</v>
       </c>
       <c r="D49" s="2">
         <v>6</v>
       </c>
-      <c r="E49" s="19">
+      <c r="E49" s="2" t="str" cm="1">
+        <f t="array" ref="E49">_xlfn.IFS(D49=1,"Confident Republican",D49=2,"Likely Republican",D49=3,"Model Republican", D49=4,"Model Democrat", D49=5,"Likely Democrat",D49=6,"Confident Democrat")</f>
+        <v>Confident Democrat</v>
+      </c>
+      <c r="F49" s="19">
         <v>37.431573</v>
       </c>
-      <c r="F49" s="19">
+      <c r="G49" s="19">
         <v>-78.656893999999994</v>
       </c>
-      <c r="K49" s="2" t="str" cm="1">
-        <f t="array" ref="K49">_xlfn.IFS(ISBLANK(D49),"SwingState",D49 = 3, "Model Rep",D49=4,"Model Dem",D49&lt;3,"R",D49&gt;3,"D")</f>
+      <c r="L49" s="2" t="str" cm="1">
+        <f t="array" ref="L49">_xlfn.IFS(ISBLANK(D49),"SwingState",D49 = 3, "Model Rep",D49=4,"Model Dem",D49&lt;3,"R",D49&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="U49" s="17"/>
       <c r="V49" s="17"/>
       <c r="W49" s="17"/>
       <c r="X49" s="17"/>
-    </row>
-    <row r="50" spans="1:24" ht="29" x14ac:dyDescent="0.2">
+      <c r="Y49" s="17"/>
+    </row>
+    <row r="50" spans="1:25" ht="29" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="str" cm="1">
         <f t="array" ref="A50">_xlfn.IFS(ISBLANK(D50),"SwingState",D50 = 3, "SwingState",D50=4,"SwingState",D50&lt;3,"R",D50&gt;3,"D")</f>
         <v>R</v>
@@ -41038,28 +41258,32 @@
       <c r="B50" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="21">
         <v>5</v>
       </c>
       <c r="D50" s="2">
         <v>1</v>
       </c>
-      <c r="E50" s="19">
+      <c r="E50" s="2" t="str" cm="1">
+        <f t="array" ref="E50">_xlfn.IFS(D50=1,"Confident Republican",D50=2,"Likely Republican",D50=3,"Model Republican", D50=4,"Model Democrat", D50=5,"Likely Democrat",D50=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F50" s="19">
         <v>47.751074000000003</v>
       </c>
-      <c r="F50" s="19">
+      <c r="G50" s="19">
         <v>-120.740139</v>
       </c>
-      <c r="K50" s="2" t="str" cm="1">
-        <f t="array" ref="K50">_xlfn.IFS(ISBLANK(D50),"SwingState",D50 = 3, "Model Rep",D50=4,"Model Dem",D50&lt;3,"R",D50&gt;3,"D")</f>
+      <c r="L50" s="2" t="str" cm="1">
+        <f t="array" ref="L50">_xlfn.IFS(ISBLANK(D50),"SwingState",D50 = 3, "Model Rep",D50=4,"Model Dem",D50&lt;3,"R",D50&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="U50" s="17"/>
       <c r="V50" s="17"/>
       <c r="W50" s="17"/>
       <c r="X50" s="17"/>
-    </row>
-    <row r="51" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y50" s="17"/>
+    </row>
+    <row r="51" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="str" cm="1">
         <f t="array" ref="A51">_xlfn.IFS(ISBLANK(D51),"SwingState",D51 = 3, "SwingState",D51=4,"SwingState",D51&lt;3,"R",D51&gt;3,"D")</f>
         <v>SwingState</v>
@@ -41067,28 +41291,32 @@
       <c r="B51" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="21">
         <v>10</v>
       </c>
       <c r="D51" s="2">
         <v>3</v>
       </c>
-      <c r="E51" s="19">
+      <c r="E51" s="2" t="str" cm="1">
+        <f t="array" ref="E51">_xlfn.IFS(D51=1,"Confident Republican",D51=2,"Likely Republican",D51=3,"Model Republican", D51=4,"Model Democrat", D51=5,"Likely Democrat",D51=6,"Confident Democrat")</f>
+        <v>Model Republican</v>
+      </c>
+      <c r="F51" s="19">
         <v>38.597625999999998</v>
       </c>
-      <c r="F51" s="19">
+      <c r="G51" s="19">
         <v>-80.454903000000002</v>
       </c>
-      <c r="K51" s="2" t="str" cm="1">
-        <f t="array" ref="K51">_xlfn.IFS(ISBLANK(D51),"SwingState",D51 = 3, "Model Rep",D51=4,"Model Dem",D51&lt;3,"R",D51&gt;3,"D")</f>
+      <c r="L51" s="2" t="str" cm="1">
+        <f t="array" ref="L51">_xlfn.IFS(ISBLANK(D51),"SwingState",D51 = 3, "Model Rep",D51=4,"Model Dem",D51&lt;3,"R",D51&gt;3,"D")</f>
         <v>Model Rep</v>
       </c>
-      <c r="U51" s="17"/>
       <c r="V51" s="17"/>
       <c r="W51" s="17"/>
       <c r="X51" s="17"/>
-    </row>
-    <row r="52" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="Y51" s="17"/>
+    </row>
+    <row r="52" spans="1:25" ht="20" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="str" cm="1">
         <f t="array" ref="A52">_xlfn.IFS(ISBLANK(D52),"SwingState",D52 = 3, "SwingState",D52=4,"SwingState",D52&lt;3,"R",D52&gt;3,"D")</f>
         <v>R</v>
@@ -41096,54 +41324,58 @@
       <c r="B52" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="21">
         <v>3</v>
       </c>
       <c r="D52" s="2">
         <v>1</v>
       </c>
-      <c r="E52" s="19">
+      <c r="E52" s="2" t="str" cm="1">
+        <f t="array" ref="E52">_xlfn.IFS(D52=1,"Confident Republican",D52=2,"Likely Republican",D52=3,"Model Republican", D52=4,"Model Democrat", D52=5,"Likely Democrat",D52=6,"Confident Democrat")</f>
+        <v>Confident Republican</v>
+      </c>
+      <c r="F52" s="19">
         <v>43.784439999999996</v>
       </c>
-      <c r="F52" s="19">
+      <c r="G52" s="19">
         <v>-88.787868000000003</v>
       </c>
-      <c r="K52" s="2" t="str" cm="1">
-        <f t="array" ref="K52">_xlfn.IFS(ISBLANK(D52),"SwingState",D52 = 3, "Model Rep",D52=4,"Model Dem",D52&lt;3,"R",D52&gt;3,"D")</f>
+      <c r="L52" s="2" t="str" cm="1">
+        <f t="array" ref="L52">_xlfn.IFS(ISBLANK(D52),"SwingState",D52 = 3, "Model Rep",D52=4,"Model Dem",D52&lt;3,"R",D52&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="U52" s="17"/>
       <c r="V52" s="17"/>
       <c r="W52" s="17"/>
       <c r="X52" s="17"/>
-    </row>
-    <row r="53" spans="1:24" ht="18" x14ac:dyDescent="0.2">
-      <c r="E53" s="19">
+      <c r="Y52" s="17"/>
+    </row>
+    <row r="53" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+      <c r="F53" s="19">
         <v>43.075968000000003</v>
       </c>
-      <c r="F53" s="19">
+      <c r="G53" s="19">
         <v>-107.290284</v>
       </c>
-      <c r="U53" s="17"/>
       <c r="V53" s="17"/>
       <c r="W53" s="17"/>
       <c r="X53" s="17"/>
-    </row>
-    <row r="54" spans="1:24" ht="18" x14ac:dyDescent="0.2">
-      <c r="U54" s="17"/>
+      <c r="Y53" s="17"/>
+    </row>
+    <row r="54" spans="1:25" ht="18" x14ac:dyDescent="0.2">
       <c r="V54" s="17"/>
       <c r="W54" s="17"/>
       <c r="X54" s="17"/>
-    </row>
-    <row r="55" spans="1:24" ht="18" x14ac:dyDescent="0.2">
-      <c r="U55" s="17"/>
+      <c r="Y54" s="17"/>
+    </row>
+    <row r="55" spans="1:25" ht="18" x14ac:dyDescent="0.2">
       <c r="V55" s="17"/>
       <c r="W55" s="17"/>
-      <c r="X55"/>
+      <c r="X55" s="17"/>
+      <c r="Y55"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q1" r:id="rId1" xr:uid="{BB2978F7-FF7A-8D4E-A41C-DE1C98FC5455}"/>
+    <hyperlink ref="R1" r:id="rId1" xr:uid="{BB2978F7-FF7A-8D4E-A41C-DE1C98FC5455}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -47255,4 +47487,430 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE63A017-C247-4F4B-8EAA-3B88279B2419}">
+  <dimension ref="A2:B52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="21">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="21">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A21" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A22" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A23" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A25" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A26" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A28" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A29" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A30" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A31" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A32" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A33" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A34" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="21">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A35" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A36" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A37" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="21">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A38" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A39" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A40" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A41" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A42" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A43" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A44" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A45" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="21">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A46" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A47" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A48" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="21">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A49" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" s="21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A50" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A51" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A52" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="21">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B52">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
comments and renaming .py
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myimam/Personal/15-For-50/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9750DCFB-725B-BE42-9637-3B8C17B2D088}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC3A0E2-0639-FC44-BAF7-7795F1015CE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="3" xr2:uid="{A414920B-AA94-6E44-AEE3-541A17C74404}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="166">
   <si>
     <t>E</t>
   </si>
@@ -364,6 +364,9 @@
   </si>
   <si>
     <t>[0.00619881]</t>
+  </si>
+  <si>
+    <t>Results</t>
   </si>
   <si>
     <t>Final Results</t>
@@ -35083,7 +35086,7 @@
   <dimension ref="A1:L97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B2" sqref="B2:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -39502,23 +39505,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A12BA6E-D220-514B-B360-4F43E4765A8F}">
-  <dimension ref="A1:Y55"/>
+  <dimension ref="A1:Z55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="10.83203125" style="2"/>
     <col min="5" max="5" width="19.33203125" style="2" customWidth="1"/>
-    <col min="6" max="16" width="10.83203125" style="2"/>
-    <col min="17" max="17" width="12.6640625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="2"/>
+    <col min="6" max="17" width="10.83203125" style="2"/>
+    <col min="18" max="18" width="12.6640625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>79</v>
       </c>
@@ -39532,13 +39535,13 @@
         <v>77</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>78</v>
@@ -39553,19 +39556,22 @@
         <v>82</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="O1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="S1" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="str" cm="1">
         <f t="array" ref="A2">_xlfn.IFS(ISBLANK(D2),"SwingState",D2 = 3, "SwingState",D2=4,"SwingState",D2&lt;3,"R",D2&gt;3,"D")</f>
         <v>R</v>
@@ -39609,20 +39615,24 @@
         <f t="array" ref="L2">_xlfn.IFS(ISBLANK(D2),"SwingState",D2 = 3, "Model Rep",D2=4,"Model Dem",D2&lt;3,"R",D2&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="2" t="str" cm="1">
+        <f t="array" ref="M2">_xlfn.IFS(D2&lt;4,"Republican",D2&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
+      <c r="N2" s="2">
         <f>SUMIF(L2:L52,"D",C2:C52)+SUMIF(L2:L52,"Model Dem",C2:C52)</f>
         <v>267</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <f>SUMIF(L2:L52,"R",C2:C52)+SUMIF(L2:L52,"Model Rep",C2:C52)</f>
         <v>271</v>
       </c>
-      <c r="O2" s="2">
-        <f>M2+N2</f>
+      <c r="P2" s="2">
+        <f>N2+O2</f>
         <v>538</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="str" cm="1">
         <f t="array" ref="A3">_xlfn.IFS(ISBLANK(D3),"SwingState",D3 = 3, "SwingState",D3=4,"SwingState",D3&lt;3,"R",D3&gt;3,"D")</f>
         <v>R</v>
@@ -39650,8 +39660,12 @@
         <f t="array" ref="L3">_xlfn.IFS(ISBLANK(D3),"SwingState",D3 = 3, "Model Rep",D3=4,"Model Dem",D3&lt;3,"R",D3&gt;3,"D")</f>
         <v>R</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="M3" s="2" t="str" cm="1">
+        <f t="array" ref="M3">_xlfn.IFS(D3&lt;4,"Republican",D3&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="str" cm="1">
         <f t="array" ref="A4">_xlfn.IFS(ISBLANK(D4),"SwingState",D4 = 3, "SwingState",D4=4,"SwingState",D4&lt;3,"R",D4&gt;3,"D")</f>
         <v>R</v>
@@ -39679,12 +39693,16 @@
         <f t="array" ref="L4">_xlfn.IFS(ISBLANK(D4),"SwingState",D4 = 3, "Model Rep",D4=4,"Model Dem",D4&lt;3,"R",D4&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="V4" s="18"/>
+      <c r="M4" s="2" t="str" cm="1">
+        <f t="array" ref="M4">_xlfn.IFS(D4&lt;4,"Republican",D4&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W4" s="18"/>
       <c r="X4" s="18"/>
       <c r="Y4" s="18"/>
-    </row>
-    <row r="5" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+      <c r="Z4" s="18"/>
+    </row>
+    <row r="5" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="str" cm="1">
         <f t="array" ref="A5">_xlfn.IFS(ISBLANK(D5),"SwingState",D5 = 3, "SwingState",D5=4,"SwingState",D5&lt;3,"R",D5&gt;3,"D")</f>
         <v>R</v>
@@ -39712,18 +39730,22 @@
         <f t="array" ref="L5">_xlfn.IFS(ISBLANK(D5),"SwingState",D5 = 3, "Model Rep",D5=4,"Model Dem",D5&lt;3,"R",D5&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>100</v>
+      <c r="M5" s="2" t="str" cm="1">
+        <f t="array" ref="M5">_xlfn.IFS(D5&lt;4,"Republican",D5&gt;3,"Democrat")</f>
+        <v>Republican</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="V5" s="17"/>
+      <c r="T5" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="W5" s="17"/>
       <c r="X5" s="17"/>
       <c r="Y5" s="17"/>
-    </row>
-    <row r="6" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z5" s="17"/>
+    </row>
+    <row r="6" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="str" cm="1">
         <f t="array" ref="A6">_xlfn.IFS(ISBLANK(D6),"SwingState",D6 = 3, "SwingState",D6=4,"SwingState",D6&lt;3,"R",D6&gt;3,"D")</f>
         <v>D</v>
@@ -39751,18 +39773,22 @@
         <f t="array" ref="L6">_xlfn.IFS(ISBLANK(D6),"SwingState",D6 = 3, "Model Rep",D6=4,"Model Dem",D6&lt;3,"R",D6&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="M6" s="2" t="str" cm="1">
+        <f t="array" ref="M6">_xlfn.IFS(D6&lt;4,"Republican",D6&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
+      <c r="R6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="R6" s="16">
+      <c r="S6" s="16">
         <v>4.6866299999999998E-3</v>
       </c>
-      <c r="V6" s="17"/>
       <c r="W6" s="17"/>
       <c r="X6" s="17"/>
       <c r="Y6" s="17"/>
-    </row>
-    <row r="7" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z6" s="17"/>
+    </row>
+    <row r="7" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="str" cm="1">
         <f t="array" ref="A7">_xlfn.IFS(ISBLANK(D7),"SwingState",D7 = 3, "SwingState",D7=4,"SwingState",D7&lt;3,"R",D7&gt;3,"D")</f>
         <v>SwingState</v>
@@ -39790,18 +39816,22 @@
         <f t="array" ref="L7">_xlfn.IFS(ISBLANK(D7),"SwingState",D7 = 3, "Model Rep",D7=4,"Model Dem",D7&lt;3,"R",D7&gt;3,"D")</f>
         <v>Model Dem</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="M7" s="2" t="str" cm="1">
+        <f t="array" ref="M7">_xlfn.IFS(D7&lt;4,"Republican",D7&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="R7" s="16">
+      <c r="S7" s="16">
         <v>-2.1856879999999999E-2</v>
       </c>
-      <c r="V7" s="17"/>
       <c r="W7" s="17"/>
       <c r="X7" s="17"/>
       <c r="Y7" s="17"/>
-    </row>
-    <row r="8" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z7" s="17"/>
+    </row>
+    <row r="8" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="str" cm="1">
         <f t="array" ref="A8">_xlfn.IFS(ISBLANK(D8),"SwingState",D8 = 3, "SwingState",D8=4,"SwingState",D8&lt;3,"R",D8&gt;3,"D")</f>
         <v>D</v>
@@ -39829,18 +39859,22 @@
         <f t="array" ref="L8">_xlfn.IFS(ISBLANK(D8),"SwingState",D8 = 3, "Model Rep",D8=4,"Model Dem",D8&lt;3,"R",D8&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="M8" s="2" t="str" cm="1">
+        <f t="array" ref="M8">_xlfn.IFS(D8&lt;4,"Republican",D8&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="R8" s="16">
+      <c r="S8" s="16">
         <v>1.5908700000000001E-3</v>
       </c>
-      <c r="V8" s="17"/>
       <c r="W8" s="17"/>
       <c r="X8" s="17"/>
       <c r="Y8" s="17"/>
-    </row>
-    <row r="9" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z8" s="17"/>
+    </row>
+    <row r="9" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="str" cm="1">
         <f t="array" ref="A9">_xlfn.IFS(ISBLANK(D9),"SwingState",D9 = 3, "SwingState",D9=4,"SwingState",D9&lt;3,"R",D9&gt;3,"D")</f>
         <v>D</v>
@@ -39870,18 +39904,22 @@
         <f t="array" ref="L9">_xlfn.IFS(ISBLANK(D9),"SwingState",D9 = 3, "Model Rep",D9=4,"Model Dem",D9&lt;3,"R",D9&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="M9" s="2" t="str" cm="1">
+        <f t="array" ref="M9">_xlfn.IFS(D9&lt;4,"Republican",D9&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
+      <c r="R9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R9" s="16">
+      <c r="S9" s="16">
         <v>-3.4168530000000003E-2</v>
       </c>
-      <c r="V9" s="17"/>
       <c r="W9" s="17"/>
       <c r="X9" s="17"/>
       <c r="Y9" s="17"/>
-    </row>
-    <row r="10" spans="1:25" ht="29" x14ac:dyDescent="0.2">
+      <c r="Z9" s="17"/>
+    </row>
+    <row r="10" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="str" cm="1">
         <f t="array" ref="A10">_xlfn.IFS(ISBLANK(D10),"SwingState",D10 = 3, "SwingState",D10=4,"SwingState",D10&lt;3,"R",D10&gt;3,"D")</f>
         <v>D</v>
@@ -39909,18 +39947,22 @@
         <f t="array" ref="L10">_xlfn.IFS(ISBLANK(D10),"SwingState",D10 = 3, "Model Rep",D10=4,"Model Dem",D10&lt;3,"R",D10&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="M10" s="2" t="str" cm="1">
+        <f t="array" ref="M10">_xlfn.IFS(D10&lt;4,"Republican",D10&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
+      <c r="R10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R10" s="16">
+      <c r="S10" s="16">
         <v>7.9394279999999998E-2</v>
       </c>
-      <c r="V10" s="17"/>
       <c r="W10" s="17"/>
       <c r="X10" s="17"/>
       <c r="Y10" s="17"/>
-    </row>
-    <row r="11" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z10" s="17"/>
+    </row>
+    <row r="11" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="str" cm="1">
         <f t="array" ref="A11">_xlfn.IFS(ISBLANK(D11),"SwingState",D11 = 3, "SwingState",D11=4,"SwingState",D11&lt;3,"R",D11&gt;3,"D")</f>
         <v>SwingState</v>
@@ -39948,18 +39990,22 @@
         <f t="array" ref="L11">_xlfn.IFS(ISBLANK(D11),"SwingState",D11 = 3, "Model Rep",D11=4,"Model Dem",D11&lt;3,"R",D11&gt;3,"D")</f>
         <v>Model Rep</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="M11" s="2" t="str" cm="1">
+        <f t="array" ref="M11">_xlfn.IFS(D11&lt;4,"Republican",D11&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
+      <c r="R11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R11" s="16">
+      <c r="S11" s="16">
         <v>-6.4152050000000002E-2</v>
       </c>
-      <c r="V11" s="17"/>
       <c r="W11" s="17"/>
       <c r="X11" s="17"/>
       <c r="Y11" s="17"/>
-    </row>
-    <row r="12" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z11" s="17"/>
+    </row>
+    <row r="12" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="str" cm="1">
         <f t="array" ref="A12">_xlfn.IFS(ISBLANK(D12),"SwingState",D12 = 3, "SwingState",D12=4,"SwingState",D12&lt;3,"R",D12&gt;3,"D")</f>
         <v>R</v>
@@ -39987,18 +40033,22 @@
         <f t="array" ref="L12">_xlfn.IFS(ISBLANK(D12),"SwingState",D12 = 3, "Model Rep",D12=4,"Model Dem",D12&lt;3,"R",D12&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="M12" s="2" t="str" cm="1">
+        <f t="array" ref="M12">_xlfn.IFS(D12&lt;4,"Republican",D12&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
+      <c r="R12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R12" s="16">
+      <c r="S12" s="16">
         <v>7.2694010000000003E-2</v>
       </c>
-      <c r="V12" s="17"/>
       <c r="W12" s="17"/>
       <c r="X12" s="17"/>
       <c r="Y12" s="17"/>
-    </row>
-    <row r="13" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z12" s="17"/>
+    </row>
+    <row r="13" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="str" cm="1">
         <f t="array" ref="A13">_xlfn.IFS(ISBLANK(D13),"SwingState",D13 = 3, "SwingState",D13=4,"SwingState",D13&lt;3,"R",D13&gt;3,"D")</f>
         <v>D</v>
@@ -40026,18 +40076,22 @@
         <f t="array" ref="L13">_xlfn.IFS(ISBLANK(D13),"SwingState",D13 = 3, "Model Rep",D13=4,"Model Dem",D13&lt;3,"R",D13&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="M13" s="2" t="str" cm="1">
+        <f t="array" ref="M13">_xlfn.IFS(D13&lt;4,"Republican",D13&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
+      <c r="R13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R13" s="16">
+      <c r="S13" s="16">
         <v>6.4423500000000003E-3</v>
       </c>
-      <c r="V13" s="17"/>
       <c r="W13" s="17"/>
       <c r="X13" s="17"/>
       <c r="Y13" s="17"/>
-    </row>
-    <row r="14" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+      <c r="Z13" s="17"/>
+    </row>
+    <row r="14" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="str" cm="1">
         <f t="array" ref="A14">_xlfn.IFS(ISBLANK(D14),"SwingState",D14 = 3, "SwingState",D14=4,"SwingState",D14&lt;3,"R",D14&gt;3,"D")</f>
         <v>R</v>
@@ -40065,18 +40119,22 @@
         <f t="array" ref="L14">_xlfn.IFS(ISBLANK(D14),"SwingState",D14 = 3, "Model Rep",D14=4,"Model Dem",D14&lt;3,"R",D14&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="M14" s="2" t="str" cm="1">
+        <f t="array" ref="M14">_xlfn.IFS(D14&lt;4,"Republican",D14&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
+      <c r="R14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R14" s="16">
+      <c r="S14" s="16">
         <v>4.6465449999999998E-2</v>
       </c>
-      <c r="V14" s="17"/>
       <c r="W14" s="17"/>
       <c r="X14" s="17"/>
       <c r="Y14" s="17"/>
-    </row>
-    <row r="15" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+      <c r="Z14" s="17"/>
+    </row>
+    <row r="15" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="str" cm="1">
         <f t="array" ref="A15">_xlfn.IFS(ISBLANK(D15),"SwingState",D15 = 3, "SwingState",D15=4,"SwingState",D15&lt;3,"R",D15&gt;3,"D")</f>
         <v>D</v>
@@ -40104,18 +40162,22 @@
         <f t="array" ref="L15">_xlfn.IFS(ISBLANK(D15),"SwingState",D15 = 3, "Model Rep",D15=4,"Model Dem",D15&lt;3,"R",D15&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="M15" s="2" t="str" cm="1">
+        <f t="array" ref="M15">_xlfn.IFS(D15&lt;4,"Republican",D15&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
+      <c r="R15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R15" s="16">
+      <c r="S15" s="16">
         <v>-2.753968E-2</v>
       </c>
-      <c r="V15" s="17"/>
       <c r="W15" s="17"/>
       <c r="X15" s="17"/>
       <c r="Y15" s="17"/>
-    </row>
-    <row r="16" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z15" s="17"/>
+    </row>
+    <row r="16" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="str" cm="1">
         <f t="array" ref="A16">_xlfn.IFS(ISBLANK(D16),"SwingState",D16 = 3, "SwingState",D16=4,"SwingState",D16&lt;3,"R",D16&gt;3,"D")</f>
         <v>R</v>
@@ -40143,18 +40205,22 @@
         <f t="array" ref="L16">_xlfn.IFS(ISBLANK(D16),"SwingState",D16 = 3, "Model Rep",D16=4,"Model Dem",D16&lt;3,"R",D16&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="Q16" s="2" t="s">
+      <c r="M16" s="2" t="str" cm="1">
+        <f t="array" ref="M16">_xlfn.IFS(D16&lt;4,"Republican",D16&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
+      <c r="R16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="R16" s="16">
+      <c r="S16" s="16">
         <v>-2.8092500000000001E-3</v>
       </c>
-      <c r="V16" s="17"/>
       <c r="W16" s="17"/>
       <c r="X16" s="17"/>
       <c r="Y16" s="17"/>
-    </row>
-    <row r="17" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z16" s="17"/>
+    </row>
+    <row r="17" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="str" cm="1">
         <f t="array" ref="A17">_xlfn.IFS(ISBLANK(D17),"SwingState",D17 = 3, "SwingState",D17=4,"SwingState",D17&lt;3,"R",D17&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40182,18 +40248,22 @@
         <f t="array" ref="L17">_xlfn.IFS(ISBLANK(D17),"SwingState",D17 = 3, "Model Rep",D17=4,"Model Dem",D17&lt;3,"R",D17&gt;3,"D")</f>
         <v>Model Rep</v>
       </c>
-      <c r="Q17" s="2" t="s">
+      <c r="M17" s="2" t="str" cm="1">
+        <f t="array" ref="M17">_xlfn.IFS(D17&lt;4,"Republican",D17&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
+      <c r="R17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R17" s="16">
+      <c r="S17" s="16">
         <v>6.1988099999999999E-3</v>
       </c>
-      <c r="V17" s="17"/>
       <c r="W17" s="17"/>
       <c r="X17" s="17"/>
       <c r="Y17" s="17"/>
-    </row>
-    <row r="18" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z17" s="17"/>
+    </row>
+    <row r="18" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="str" cm="1">
         <f t="array" ref="A18">_xlfn.IFS(ISBLANK(D18),"SwingState",D18 = 3, "SwingState",D18=4,"SwingState",D18&lt;3,"R",D18&gt;3,"D")</f>
         <v>R</v>
@@ -40221,13 +40291,17 @@
         <f t="array" ref="L18">_xlfn.IFS(ISBLANK(D18),"SwingState",D18 = 3, "Model Rep",D18=4,"Model Dem",D18&lt;3,"R",D18&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="R18" s="12"/>
-      <c r="V18" s="17"/>
+      <c r="M18" s="2" t="str" cm="1">
+        <f t="array" ref="M18">_xlfn.IFS(D18&lt;4,"Republican",D18&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
+      <c r="S18" s="12"/>
       <c r="W18" s="17"/>
       <c r="X18" s="17"/>
       <c r="Y18" s="17"/>
-    </row>
-    <row r="19" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z18" s="17"/>
+    </row>
+    <row r="19" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="str" cm="1">
         <f t="array" ref="A19">_xlfn.IFS(ISBLANK(D19),"SwingState",D19 = 3, "SwingState",D19=4,"SwingState",D19&lt;3,"R",D19&gt;3,"D")</f>
         <v>R</v>
@@ -40255,12 +40329,16 @@
         <f t="array" ref="L19">_xlfn.IFS(ISBLANK(D19),"SwingState",D19 = 3, "Model Rep",D19=4,"Model Dem",D19&lt;3,"R",D19&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="V19" s="17"/>
+      <c r="M19" s="2" t="str" cm="1">
+        <f t="array" ref="M19">_xlfn.IFS(D19&lt;4,"Republican",D19&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W19" s="17"/>
       <c r="X19" s="17"/>
       <c r="Y19" s="17"/>
-    </row>
-    <row r="20" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z19" s="17"/>
+    </row>
+    <row r="20" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="str" cm="1">
         <f t="array" ref="A20">_xlfn.IFS(ISBLANK(D20),"SwingState",D20 = 3, "SwingState",D20=4,"SwingState",D20&lt;3,"R",D20&gt;3,"D")</f>
         <v>R</v>
@@ -40288,12 +40366,16 @@
         <f t="array" ref="L20">_xlfn.IFS(ISBLANK(D20),"SwingState",D20 = 3, "Model Rep",D20=4,"Model Dem",D20&lt;3,"R",D20&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="V20" s="17"/>
+      <c r="M20" s="2" t="str" cm="1">
+        <f t="array" ref="M20">_xlfn.IFS(D20&lt;4,"Republican",D20&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W20" s="17"/>
       <c r="X20" s="17"/>
       <c r="Y20" s="17"/>
-    </row>
-    <row r="21" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z20" s="17"/>
+    </row>
+    <row r="21" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="str" cm="1">
         <f t="array" ref="A21">_xlfn.IFS(ISBLANK(D21),"SwingState",D21 = 3, "SwingState",D21=4,"SwingState",D21&lt;3,"R",D21&gt;3,"D")</f>
         <v>D</v>
@@ -40321,12 +40403,16 @@
         <f t="array" ref="L21">_xlfn.IFS(ISBLANK(D21),"SwingState",D21 = 3, "Model Rep",D21=4,"Model Dem",D21&lt;3,"R",D21&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="V21" s="17"/>
+      <c r="M21" s="2" t="str" cm="1">
+        <f t="array" ref="M21">_xlfn.IFS(D21&lt;4,"Republican",D21&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
       <c r="W21" s="17"/>
       <c r="X21" s="17"/>
       <c r="Y21" s="17"/>
-    </row>
-    <row r="22" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z21" s="17"/>
+    </row>
+    <row r="22" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="str" cm="1">
         <f t="array" ref="A22">_xlfn.IFS(ISBLANK(D22),"SwingState",D22 = 3, "SwingState",D22=4,"SwingState",D22&lt;3,"R",D22&gt;3,"D")</f>
         <v>D</v>
@@ -40354,12 +40440,16 @@
         <f t="array" ref="L22">_xlfn.IFS(ISBLANK(D22),"SwingState",D22 = 3, "Model Rep",D22=4,"Model Dem",D22&lt;3,"R",D22&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="V22" s="17"/>
+      <c r="M22" s="2" t="str" cm="1">
+        <f t="array" ref="M22">_xlfn.IFS(D22&lt;4,"Republican",D22&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
       <c r="W22" s="17"/>
       <c r="X22" s="17"/>
       <c r="Y22" s="17"/>
-    </row>
-    <row r="23" spans="1:25" ht="29" x14ac:dyDescent="0.2">
+      <c r="Z22" s="17"/>
+    </row>
+    <row r="23" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="str" cm="1">
         <f t="array" ref="A23">_xlfn.IFS(ISBLANK(D23),"SwingState",D23 = 3, "SwingState",D23=4,"SwingState",D23&lt;3,"R",D23&gt;3,"D")</f>
         <v>D</v>
@@ -40387,12 +40477,16 @@
         <f t="array" ref="L23">_xlfn.IFS(ISBLANK(D23),"SwingState",D23 = 3, "Model Rep",D23=4,"Model Dem",D23&lt;3,"R",D23&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="V23" s="17"/>
+      <c r="M23" s="2" t="str" cm="1">
+        <f t="array" ref="M23">_xlfn.IFS(D23&lt;4,"Republican",D23&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
       <c r="W23" s="17"/>
       <c r="X23" s="17"/>
       <c r="Y23" s="17"/>
-    </row>
-    <row r="24" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z23" s="17"/>
+    </row>
+    <row r="24" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="str" cm="1">
         <f t="array" ref="A24">_xlfn.IFS(ISBLANK(D24),"SwingState",D24 = 3, "SwingState",D24=4,"SwingState",D24&lt;3,"R",D24&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40420,12 +40514,16 @@
         <f t="array" ref="L24">_xlfn.IFS(ISBLANK(D24),"SwingState",D24 = 3, "Model Rep",D24=4,"Model Dem",D24&lt;3,"R",D24&gt;3,"D")</f>
         <v>Model Dem</v>
       </c>
-      <c r="V24" s="17"/>
+      <c r="M24" s="2" t="str" cm="1">
+        <f t="array" ref="M24">_xlfn.IFS(D24&lt;4,"Republican",D24&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
       <c r="W24" s="17"/>
       <c r="X24" s="17"/>
       <c r="Y24" s="17"/>
-    </row>
-    <row r="25" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z24" s="17"/>
+    </row>
+    <row r="25" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="str" cm="1">
         <f t="array" ref="A25">_xlfn.IFS(ISBLANK(D25),"SwingState",D25 = 3, "SwingState",D25=4,"SwingState",D25&lt;3,"R",D25&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40453,12 +40551,16 @@
         <f t="array" ref="L25">_xlfn.IFS(ISBLANK(D25),"SwingState",D25 = 3, "Model Rep",D25=4,"Model Dem",D25&lt;3,"R",D25&gt;3,"D")</f>
         <v>Model Dem</v>
       </c>
-      <c r="V25" s="17"/>
+      <c r="M25" s="2" t="str" cm="1">
+        <f t="array" ref="M25">_xlfn.IFS(D25&lt;4,"Republican",D25&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
       <c r="W25" s="17"/>
       <c r="X25" s="17"/>
       <c r="Y25" s="17"/>
-    </row>
-    <row r="26" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z25" s="17"/>
+    </row>
+    <row r="26" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="str" cm="1">
         <f t="array" ref="A26">_xlfn.IFS(ISBLANK(D26),"SwingState",D26 = 3, "SwingState",D26=4,"SwingState",D26&lt;3,"R",D26&gt;3,"D")</f>
         <v>R</v>
@@ -40486,12 +40588,16 @@
         <f t="array" ref="L26">_xlfn.IFS(ISBLANK(D26),"SwingState",D26 = 3, "Model Rep",D26=4,"Model Dem",D26&lt;3,"R",D26&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="V26" s="17"/>
+      <c r="M26" s="2" t="str" cm="1">
+        <f t="array" ref="M26">_xlfn.IFS(D26&lt;4,"Republican",D26&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W26" s="17"/>
       <c r="X26" s="17"/>
       <c r="Y26" s="17"/>
-    </row>
-    <row r="27" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z26" s="17"/>
+    </row>
+    <row r="27" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="str" cm="1">
         <f t="array" ref="A27">_xlfn.IFS(ISBLANK(D27),"SwingState",D27 = 3, "SwingState",D27=4,"SwingState",D27&lt;3,"R",D27&gt;3,"D")</f>
         <v>R</v>
@@ -40519,12 +40625,16 @@
         <f t="array" ref="L27">_xlfn.IFS(ISBLANK(D27),"SwingState",D27 = 3, "Model Rep",D27=4,"Model Dem",D27&lt;3,"R",D27&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="V27" s="17"/>
+      <c r="M27" s="2" t="str" cm="1">
+        <f t="array" ref="M27">_xlfn.IFS(D27&lt;4,"Republican",D27&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W27" s="17"/>
       <c r="X27" s="17"/>
       <c r="Y27" s="17"/>
-    </row>
-    <row r="28" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z27" s="17"/>
+    </row>
+    <row r="28" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="str" cm="1">
         <f t="array" ref="A28">_xlfn.IFS(ISBLANK(D28),"SwingState",D28 = 3, "SwingState",D28=4,"SwingState",D28&lt;3,"R",D28&gt;3,"D")</f>
         <v>R</v>
@@ -40552,12 +40662,16 @@
         <f t="array" ref="L28">_xlfn.IFS(ISBLANK(D28),"SwingState",D28 = 3, "Model Rep",D28=4,"Model Dem",D28&lt;3,"R",D28&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="V28" s="17"/>
+      <c r="M28" s="2" t="str" cm="1">
+        <f t="array" ref="M28">_xlfn.IFS(D28&lt;4,"Republican",D28&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W28" s="17"/>
       <c r="X28" s="17"/>
       <c r="Y28" s="17"/>
-    </row>
-    <row r="29" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z28" s="17"/>
+    </row>
+    <row r="29" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="str" cm="1">
         <f t="array" ref="A29">_xlfn.IFS(ISBLANK(D29),"SwingState",D29 = 3, "SwingState",D29=4,"SwingState",D29&lt;3,"R",D29&gt;3,"D")</f>
         <v>R</v>
@@ -40585,12 +40699,16 @@
         <f t="array" ref="L29">_xlfn.IFS(ISBLANK(D29),"SwingState",D29 = 3, "Model Rep",D29=4,"Model Dem",D29&lt;3,"R",D29&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="V29" s="17"/>
+      <c r="M29" s="2" t="str" cm="1">
+        <f t="array" ref="M29">_xlfn.IFS(D29&lt;4,"Republican",D29&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W29" s="17"/>
       <c r="X29" s="17"/>
       <c r="Y29" s="17"/>
-    </row>
-    <row r="30" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z29" s="17"/>
+    </row>
+    <row r="30" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="str" cm="1">
         <f t="array" ref="A30">_xlfn.IFS(ISBLANK(D30),"SwingState",D30 = 3, "SwingState",D30=4,"SwingState",D30&lt;3,"R",D30&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40618,12 +40736,16 @@
         <f t="array" ref="L30">_xlfn.IFS(ISBLANK(D30),"SwingState",D30 = 3, "Model Rep",D30=4,"Model Dem",D30&lt;3,"R",D30&gt;3,"D")</f>
         <v>Model Dem</v>
       </c>
-      <c r="V30" s="17"/>
+      <c r="M30" s="2" t="str" cm="1">
+        <f t="array" ref="M30">_xlfn.IFS(D30&lt;4,"Republican",D30&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
       <c r="W30" s="17"/>
       <c r="X30" s="17"/>
       <c r="Y30" s="17"/>
-    </row>
-    <row r="31" spans="1:25" ht="29" x14ac:dyDescent="0.2">
+      <c r="Z30" s="17"/>
+    </row>
+    <row r="31" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="str" cm="1">
         <f t="array" ref="A31">_xlfn.IFS(ISBLANK(D31),"SwingState",D31 = 3, "SwingState",D31=4,"SwingState",D31&lt;3,"R",D31&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40651,12 +40773,16 @@
         <f t="array" ref="L31">_xlfn.IFS(ISBLANK(D31),"SwingState",D31 = 3, "Model Rep",D31=4,"Model Dem",D31&lt;3,"R",D31&gt;3,"D")</f>
         <v>Model Dem</v>
       </c>
-      <c r="V31" s="17"/>
+      <c r="M31" s="2" t="str" cm="1">
+        <f t="array" ref="M31">_xlfn.IFS(D31&lt;4,"Republican",D31&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
       <c r="W31" s="17"/>
       <c r="X31" s="17"/>
       <c r="Y31" s="17"/>
-    </row>
-    <row r="32" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z31" s="17"/>
+    </row>
+    <row r="32" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="str" cm="1">
         <f t="array" ref="A32">_xlfn.IFS(ISBLANK(D32),"SwingState",D32 = 3, "SwingState",D32=4,"SwingState",D32&lt;3,"R",D32&gt;3,"D")</f>
         <v>D</v>
@@ -40684,12 +40810,16 @@
         <f t="array" ref="L32">_xlfn.IFS(ISBLANK(D32),"SwingState",D32 = 3, "Model Rep",D32=4,"Model Dem",D32&lt;3,"R",D32&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="V32" s="17"/>
+      <c r="M32" s="2" t="str" cm="1">
+        <f t="array" ref="M32">_xlfn.IFS(D32&lt;4,"Republican",D32&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
       <c r="W32" s="17"/>
       <c r="X32" s="17"/>
       <c r="Y32" s="17"/>
-    </row>
-    <row r="33" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z32" s="17"/>
+    </row>
+    <row r="33" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="str" cm="1">
         <f t="array" ref="A33">_xlfn.IFS(ISBLANK(D33),"SwingState",D33 = 3, "SwingState",D33=4,"SwingState",D33&lt;3,"R",D33&gt;3,"D")</f>
         <v>D</v>
@@ -40717,12 +40847,16 @@
         <f t="array" ref="L33">_xlfn.IFS(ISBLANK(D33),"SwingState",D33 = 3, "Model Rep",D33=4,"Model Dem",D33&lt;3,"R",D33&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="V33" s="17"/>
+      <c r="M33" s="2" t="str" cm="1">
+        <f t="array" ref="M33">_xlfn.IFS(D33&lt;4,"Republican",D33&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
       <c r="W33" s="17"/>
       <c r="X33" s="17"/>
       <c r="Y33" s="17"/>
-    </row>
-    <row r="34" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z33" s="17"/>
+    </row>
+    <row r="34" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="str" cm="1">
         <f t="array" ref="A34">_xlfn.IFS(ISBLANK(D34),"SwingState",D34 = 3, "SwingState",D34=4,"SwingState",D34&lt;3,"R",D34&gt;3,"D")</f>
         <v>D</v>
@@ -40750,12 +40884,16 @@
         <f t="array" ref="L34">_xlfn.IFS(ISBLANK(D34),"SwingState",D34 = 3, "Model Rep",D34=4,"Model Dem",D34&lt;3,"R",D34&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="V34" s="17"/>
+      <c r="M34" s="2" t="str" cm="1">
+        <f t="array" ref="M34">_xlfn.IFS(D34&lt;4,"Republican",D34&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
       <c r="W34" s="17"/>
       <c r="X34" s="17"/>
       <c r="Y34" s="17"/>
-    </row>
-    <row r="35" spans="1:25" ht="29" x14ac:dyDescent="0.2">
+      <c r="Z34" s="17"/>
+    </row>
+    <row r="35" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="str" cm="1">
         <f t="array" ref="A35">_xlfn.IFS(ISBLANK(D35),"SwingState",D35 = 3, "SwingState",D35=4,"SwingState",D35&lt;3,"R",D35&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40783,12 +40921,16 @@
         <f t="array" ref="L35">_xlfn.IFS(ISBLANK(D35),"SwingState",D35 = 3, "Model Rep",D35=4,"Model Dem",D35&lt;3,"R",D35&gt;3,"D")</f>
         <v>Model Rep</v>
       </c>
-      <c r="V35" s="17"/>
+      <c r="M35" s="2" t="str" cm="1">
+        <f t="array" ref="M35">_xlfn.IFS(D35&lt;4,"Republican",D35&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W35" s="17"/>
       <c r="X35" s="17"/>
       <c r="Y35" s="17"/>
-    </row>
-    <row r="36" spans="1:25" ht="29" x14ac:dyDescent="0.2">
+      <c r="Z35" s="17"/>
+    </row>
+    <row r="36" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="str" cm="1">
         <f t="array" ref="A36">_xlfn.IFS(ISBLANK(D36),"SwingState",D36 = 3, "SwingState",D36=4,"SwingState",D36&lt;3,"R",D36&gt;3,"D")</f>
         <v>R</v>
@@ -40816,12 +40958,16 @@
         <f t="array" ref="L36">_xlfn.IFS(ISBLANK(D36),"SwingState",D36 = 3, "Model Rep",D36=4,"Model Dem",D36&lt;3,"R",D36&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="V36" s="17"/>
+      <c r="M36" s="2" t="str" cm="1">
+        <f t="array" ref="M36">_xlfn.IFS(D36&lt;4,"Republican",D36&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W36" s="17"/>
       <c r="X36" s="17"/>
       <c r="Y36" s="17"/>
-    </row>
-    <row r="37" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z36" s="17"/>
+    </row>
+    <row r="37" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="str" cm="1">
         <f t="array" ref="A37">_xlfn.IFS(ISBLANK(D37),"SwingState",D37 = 3, "SwingState",D37=4,"SwingState",D37&lt;3,"R",D37&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40849,12 +40995,16 @@
         <f t="array" ref="L37">_xlfn.IFS(ISBLANK(D37),"SwingState",D37 = 3, "Model Rep",D37=4,"Model Dem",D37&lt;3,"R",D37&gt;3,"D")</f>
         <v>Model Dem</v>
       </c>
-      <c r="V37" s="17"/>
+      <c r="M37" s="2" t="str" cm="1">
+        <f t="array" ref="M37">_xlfn.IFS(D37&lt;4,"Republican",D37&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
       <c r="W37" s="17"/>
       <c r="X37" s="17"/>
       <c r="Y37" s="17"/>
-    </row>
-    <row r="38" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z37" s="17"/>
+    </row>
+    <row r="38" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="str" cm="1">
         <f t="array" ref="A38">_xlfn.IFS(ISBLANK(D38),"SwingState",D38 = 3, "SwingState",D38=4,"SwingState",D38&lt;3,"R",D38&gt;3,"D")</f>
         <v>R</v>
@@ -40882,12 +41032,16 @@
         <f t="array" ref="L38">_xlfn.IFS(ISBLANK(D38),"SwingState",D38 = 3, "Model Rep",D38=4,"Model Dem",D38&lt;3,"R",D38&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="V38" s="17"/>
+      <c r="M38" s="2" t="str" cm="1">
+        <f t="array" ref="M38">_xlfn.IFS(D38&lt;4,"Republican",D38&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W38" s="17"/>
       <c r="X38" s="17"/>
       <c r="Y38" s="17"/>
-    </row>
-    <row r="39" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z38" s="17"/>
+    </row>
+    <row r="39" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="str" cm="1">
         <f t="array" ref="A39">_xlfn.IFS(ISBLANK(D39),"SwingState",D39 = 3, "SwingState",D39=4,"SwingState",D39&lt;3,"R",D39&gt;3,"D")</f>
         <v>D</v>
@@ -40915,12 +41069,16 @@
         <f t="array" ref="L39">_xlfn.IFS(ISBLANK(D39),"SwingState",D39 = 3, "Model Rep",D39=4,"Model Dem",D39&lt;3,"R",D39&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="V39" s="17"/>
+      <c r="M39" s="2" t="str" cm="1">
+        <f t="array" ref="M39">_xlfn.IFS(D39&lt;4,"Republican",D39&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
       <c r="W39" s="17"/>
       <c r="X39" s="17"/>
       <c r="Y39" s="17"/>
-    </row>
-    <row r="40" spans="1:25" ht="29" x14ac:dyDescent="0.2">
+      <c r="Z39" s="17"/>
+    </row>
+    <row r="40" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="str" cm="1">
         <f t="array" ref="A40">_xlfn.IFS(ISBLANK(D40),"SwingState",D40 = 3, "SwingState",D40=4,"SwingState",D40&lt;3,"R",D40&gt;3,"D")</f>
         <v>SwingState</v>
@@ -40948,12 +41106,16 @@
         <f t="array" ref="L40">_xlfn.IFS(ISBLANK(D40),"SwingState",D40 = 3, "Model Rep",D40=4,"Model Dem",D40&lt;3,"R",D40&gt;3,"D")</f>
         <v>Model Rep</v>
       </c>
-      <c r="V40" s="17"/>
+      <c r="M40" s="2" t="str" cm="1">
+        <f t="array" ref="M40">_xlfn.IFS(D40&lt;4,"Republican",D40&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W40" s="17"/>
       <c r="X40" s="17"/>
       <c r="Y40" s="17"/>
-    </row>
-    <row r="41" spans="1:25" ht="29" x14ac:dyDescent="0.2">
+      <c r="Z40" s="17"/>
+    </row>
+    <row r="41" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="str" cm="1">
         <f t="array" ref="A41">_xlfn.IFS(ISBLANK(D41),"SwingState",D41 = 3, "SwingState",D41=4,"SwingState",D41&lt;3,"R",D41&gt;3,"D")</f>
         <v>D</v>
@@ -40981,12 +41143,16 @@
         <f t="array" ref="L41">_xlfn.IFS(ISBLANK(D41),"SwingState",D41 = 3, "Model Rep",D41=4,"Model Dem",D41&lt;3,"R",D41&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="V41" s="17"/>
+      <c r="M41" s="2" t="str" cm="1">
+        <f t="array" ref="M41">_xlfn.IFS(D41&lt;4,"Republican",D41&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
       <c r="W41" s="17"/>
       <c r="X41" s="17"/>
       <c r="Y41" s="17"/>
-    </row>
-    <row r="42" spans="1:25" ht="29" x14ac:dyDescent="0.2">
+      <c r="Z41" s="17"/>
+    </row>
+    <row r="42" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="str" cm="1">
         <f t="array" ref="A42">_xlfn.IFS(ISBLANK(D42),"SwingState",D42 = 3, "SwingState",D42=4,"SwingState",D42&lt;3,"R",D42&gt;3,"D")</f>
         <v>R</v>
@@ -41014,12 +41180,16 @@
         <f t="array" ref="L42">_xlfn.IFS(ISBLANK(D42),"SwingState",D42 = 3, "Model Rep",D42=4,"Model Dem",D42&lt;3,"R",D42&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="V42" s="17"/>
+      <c r="M42" s="2" t="str" cm="1">
+        <f t="array" ref="M42">_xlfn.IFS(D42&lt;4,"Republican",D42&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W42" s="17"/>
       <c r="X42" s="17"/>
       <c r="Y42" s="17"/>
-    </row>
-    <row r="43" spans="1:25" ht="29" x14ac:dyDescent="0.2">
+      <c r="Z42" s="17"/>
+    </row>
+    <row r="43" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="str" cm="1">
         <f t="array" ref="A43">_xlfn.IFS(ISBLANK(D43),"SwingState",D43 = 3, "SwingState",D43=4,"SwingState",D43&lt;3,"R",D43&gt;3,"D")</f>
         <v>R</v>
@@ -41047,12 +41217,16 @@
         <f t="array" ref="L43">_xlfn.IFS(ISBLANK(D43),"SwingState",D43 = 3, "Model Rep",D43=4,"Model Dem",D43&lt;3,"R",D43&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="V43" s="17"/>
+      <c r="M43" s="2" t="str" cm="1">
+        <f t="array" ref="M43">_xlfn.IFS(D43&lt;4,"Republican",D43&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W43" s="17"/>
       <c r="X43" s="17"/>
       <c r="Y43" s="17"/>
-    </row>
-    <row r="44" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z43" s="17"/>
+    </row>
+    <row r="44" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="str" cm="1">
         <f t="array" ref="A44">_xlfn.IFS(ISBLANK(D44),"SwingState",D44 = 3, "SwingState",D44=4,"SwingState",D44&lt;3,"R",D44&gt;3,"D")</f>
         <v>R</v>
@@ -41080,12 +41254,16 @@
         <f t="array" ref="L44">_xlfn.IFS(ISBLANK(D44),"SwingState",D44 = 3, "Model Rep",D44=4,"Model Dem",D44&lt;3,"R",D44&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="V44" s="17"/>
+      <c r="M44" s="2" t="str" cm="1">
+        <f t="array" ref="M44">_xlfn.IFS(D44&lt;4,"Republican",D44&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W44" s="17"/>
       <c r="X44" s="17"/>
       <c r="Y44" s="17"/>
-    </row>
-    <row r="45" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z44" s="17"/>
+    </row>
+    <row r="45" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="str" cm="1">
         <f t="array" ref="A45">_xlfn.IFS(ISBLANK(D45),"SwingState",D45 = 3, "SwingState",D45=4,"SwingState",D45&lt;3,"R",D45&gt;3,"D")</f>
         <v>R</v>
@@ -41113,12 +41291,16 @@
         <f t="array" ref="L45">_xlfn.IFS(ISBLANK(D45),"SwingState",D45 = 3, "Model Rep",D45=4,"Model Dem",D45&lt;3,"R",D45&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="V45" s="17"/>
+      <c r="M45" s="2" t="str" cm="1">
+        <f t="array" ref="M45">_xlfn.IFS(D45&lt;4,"Republican",D45&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W45" s="17"/>
       <c r="X45" s="17"/>
       <c r="Y45" s="17"/>
-    </row>
-    <row r="46" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z45" s="17"/>
+    </row>
+    <row r="46" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="str" cm="1">
         <f t="array" ref="A46">_xlfn.IFS(ISBLANK(D46),"SwingState",D46 = 3, "SwingState",D46=4,"SwingState",D46&lt;3,"R",D46&gt;3,"D")</f>
         <v>R</v>
@@ -41146,12 +41328,16 @@
         <f t="array" ref="L46">_xlfn.IFS(ISBLANK(D46),"SwingState",D46 = 3, "Model Rep",D46=4,"Model Dem",D46&lt;3,"R",D46&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="V46" s="17"/>
+      <c r="M46" s="2" t="str" cm="1">
+        <f t="array" ref="M46">_xlfn.IFS(D46&lt;4,"Republican",D46&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W46" s="17"/>
       <c r="X46" s="17"/>
       <c r="Y46" s="17"/>
-    </row>
-    <row r="47" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z46" s="17"/>
+    </row>
+    <row r="47" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="str" cm="1">
         <f t="array" ref="A47">_xlfn.IFS(ISBLANK(D47),"SwingState",D47 = 3, "SwingState",D47=4,"SwingState",D47&lt;3,"R",D47&gt;3,"D")</f>
         <v>D</v>
@@ -41179,12 +41365,16 @@
         <f t="array" ref="L47">_xlfn.IFS(ISBLANK(D47),"SwingState",D47 = 3, "Model Rep",D47=4,"Model Dem",D47&lt;3,"R",D47&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="V47" s="17"/>
+      <c r="M47" s="2" t="str" cm="1">
+        <f t="array" ref="M47">_xlfn.IFS(D47&lt;4,"Republican",D47&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
       <c r="W47" s="17"/>
       <c r="X47" s="17"/>
       <c r="Y47" s="17"/>
-    </row>
-    <row r="48" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z47" s="17"/>
+    </row>
+    <row r="48" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="str" cm="1">
         <f t="array" ref="A48">_xlfn.IFS(ISBLANK(D48),"SwingState",D48 = 3, "SwingState",D48=4,"SwingState",D48&lt;3,"R",D48&gt;3,"D")</f>
         <v>SwingState</v>
@@ -41212,12 +41402,16 @@
         <f t="array" ref="L48">_xlfn.IFS(ISBLANK(D48),"SwingState",D48 = 3, "Model Rep",D48=4,"Model Dem",D48&lt;3,"R",D48&gt;3,"D")</f>
         <v>Model Dem</v>
       </c>
-      <c r="V48" s="17"/>
+      <c r="M48" s="2" t="str" cm="1">
+        <f t="array" ref="M48">_xlfn.IFS(D48&lt;4,"Republican",D48&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
       <c r="W48" s="17"/>
       <c r="X48" s="17"/>
       <c r="Y48" s="17"/>
-    </row>
-    <row r="49" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z48" s="17"/>
+    </row>
+    <row r="49" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="str" cm="1">
         <f t="array" ref="A49">_xlfn.IFS(ISBLANK(D49),"SwingState",D49 = 3, "SwingState",D49=4,"SwingState",D49&lt;3,"R",D49&gt;3,"D")</f>
         <v>D</v>
@@ -41245,12 +41439,16 @@
         <f t="array" ref="L49">_xlfn.IFS(ISBLANK(D49),"SwingState",D49 = 3, "Model Rep",D49=4,"Model Dem",D49&lt;3,"R",D49&gt;3,"D")</f>
         <v>D</v>
       </c>
-      <c r="V49" s="17"/>
+      <c r="M49" s="2" t="str" cm="1">
+        <f t="array" ref="M49">_xlfn.IFS(D49&lt;4,"Republican",D49&gt;3,"Democrat")</f>
+        <v>Democrat</v>
+      </c>
       <c r="W49" s="17"/>
       <c r="X49" s="17"/>
       <c r="Y49" s="17"/>
-    </row>
-    <row r="50" spans="1:25" ht="29" x14ac:dyDescent="0.2">
+      <c r="Z49" s="17"/>
+    </row>
+    <row r="50" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="str" cm="1">
         <f t="array" ref="A50">_xlfn.IFS(ISBLANK(D50),"SwingState",D50 = 3, "SwingState",D50=4,"SwingState",D50&lt;3,"R",D50&gt;3,"D")</f>
         <v>R</v>
@@ -41278,12 +41476,16 @@
         <f t="array" ref="L50">_xlfn.IFS(ISBLANK(D50),"SwingState",D50 = 3, "Model Rep",D50=4,"Model Dem",D50&lt;3,"R",D50&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="V50" s="17"/>
+      <c r="M50" s="2" t="str" cm="1">
+        <f t="array" ref="M50">_xlfn.IFS(D50&lt;4,"Republican",D50&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W50" s="17"/>
       <c r="X50" s="17"/>
       <c r="Y50" s="17"/>
-    </row>
-    <row r="51" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z50" s="17"/>
+    </row>
+    <row r="51" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="str" cm="1">
         <f t="array" ref="A51">_xlfn.IFS(ISBLANK(D51),"SwingState",D51 = 3, "SwingState",D51=4,"SwingState",D51&lt;3,"R",D51&gt;3,"D")</f>
         <v>SwingState</v>
@@ -41311,12 +41513,16 @@
         <f t="array" ref="L51">_xlfn.IFS(ISBLANK(D51),"SwingState",D51 = 3, "Model Rep",D51=4,"Model Dem",D51&lt;3,"R",D51&gt;3,"D")</f>
         <v>Model Rep</v>
       </c>
-      <c r="V51" s="17"/>
+      <c r="M51" s="2" t="str" cm="1">
+        <f t="array" ref="M51">_xlfn.IFS(D51&lt;4,"Republican",D51&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W51" s="17"/>
       <c r="X51" s="17"/>
       <c r="Y51" s="17"/>
-    </row>
-    <row r="52" spans="1:25" ht="20" x14ac:dyDescent="0.2">
+      <c r="Z51" s="17"/>
+    </row>
+    <row r="52" spans="1:26" ht="20" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="str" cm="1">
         <f t="array" ref="A52">_xlfn.IFS(ISBLANK(D52),"SwingState",D52 = 3, "SwingState",D52=4,"SwingState",D52&lt;3,"R",D52&gt;3,"D")</f>
         <v>R</v>
@@ -41344,38 +41550,42 @@
         <f t="array" ref="L52">_xlfn.IFS(ISBLANK(D52),"SwingState",D52 = 3, "Model Rep",D52=4,"Model Dem",D52&lt;3,"R",D52&gt;3,"D")</f>
         <v>R</v>
       </c>
-      <c r="V52" s="17"/>
+      <c r="M52" s="2" t="str" cm="1">
+        <f t="array" ref="M52">_xlfn.IFS(D52&lt;4,"Republican",D52&gt;3,"Democrat")</f>
+        <v>Republican</v>
+      </c>
       <c r="W52" s="17"/>
       <c r="X52" s="17"/>
       <c r="Y52" s="17"/>
-    </row>
-    <row r="53" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+      <c r="Z52" s="17"/>
+    </row>
+    <row r="53" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="F53" s="19">
         <v>43.075968000000003</v>
       </c>
       <c r="G53" s="19">
         <v>-107.290284</v>
       </c>
-      <c r="V53" s="17"/>
       <c r="W53" s="17"/>
       <c r="X53" s="17"/>
       <c r="Y53" s="17"/>
-    </row>
-    <row r="54" spans="1:25" ht="18" x14ac:dyDescent="0.2">
-      <c r="V54" s="17"/>
+      <c r="Z53" s="17"/>
+    </row>
+    <row r="54" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="W54" s="17"/>
       <c r="X54" s="17"/>
       <c r="Y54" s="17"/>
-    </row>
-    <row r="55" spans="1:25" ht="18" x14ac:dyDescent="0.2">
-      <c r="V55" s="17"/>
+      <c r="Z54" s="17"/>
+    </row>
+    <row r="55" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="W55" s="17"/>
       <c r="X55" s="17"/>
-      <c r="Y55"/>
+      <c r="Y55" s="17"/>
+      <c r="Z55"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R1" r:id="rId1" xr:uid="{BB2978F7-FF7A-8D4E-A41C-DE1C98FC5455}"/>
+    <hyperlink ref="S1" r:id="rId1" xr:uid="{BB2978F7-FF7A-8D4E-A41C-DE1C98FC5455}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -41393,21 +41603,21 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B2" s="17">
         <v>32.318230999999997</v>
@@ -41421,7 +41631,7 @@
     </row>
     <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B3" s="17">
         <v>63.588752999999997</v>
@@ -41435,7 +41645,7 @@
     </row>
     <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B4" s="17">
         <v>34.048927999999997</v>
@@ -41449,7 +41659,7 @@
     </row>
     <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B5" s="17">
         <v>35.201050000000002</v>
@@ -41461,12 +41671,12 @@
         <v>33</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B6" s="17">
         <v>36.778261000000001</v>
@@ -41480,7 +41690,7 @@
     </row>
     <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="17">
         <v>39.550051000000003</v>
@@ -41494,7 +41704,7 @@
     </row>
     <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B8" s="17">
         <v>41.603220999999998</v>
@@ -41508,7 +41718,7 @@
     </row>
     <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B9" s="17">
         <v>38.910831999999999</v>
@@ -41522,7 +41732,7 @@
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B10" s="17">
         <v>38.905985000000001</v>
@@ -41536,7 +41746,7 @@
     </row>
     <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B11" s="17">
         <v>27.664826999999999</v>
@@ -41550,7 +41760,7 @@
     </row>
     <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B12" s="17">
         <v>32.157435</v>
@@ -41564,7 +41774,7 @@
     </row>
     <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B13" s="17">
         <v>19.898682000000001</v>
@@ -41578,7 +41788,7 @@
     </row>
     <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B14" s="17">
         <v>44.068201999999999</v>
@@ -41592,7 +41802,7 @@
     </row>
     <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B15" s="17">
         <v>40.633125</v>
@@ -41606,7 +41816,7 @@
     </row>
     <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B16" s="17">
         <v>40.551217000000001</v>
@@ -41620,7 +41830,7 @@
     </row>
     <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B17" s="17">
         <v>41.878003</v>
@@ -41634,7 +41844,7 @@
     </row>
     <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B18" s="17">
         <v>39.011901999999999</v>
@@ -41648,7 +41858,7 @@
     </row>
     <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B19" s="17">
         <v>37.839333000000003</v>
@@ -41662,7 +41872,7 @@
     </row>
     <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B20" s="17">
         <v>31.244823</v>
@@ -41676,7 +41886,7 @@
     </row>
     <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B21" s="17">
         <v>45.253782999999999</v>
@@ -41690,7 +41900,7 @@
     </row>
     <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B22" s="17">
         <v>39.045755</v>
@@ -41704,7 +41914,7 @@
     </row>
     <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B23" s="17">
         <v>42.407210999999997</v>
@@ -41718,7 +41928,7 @@
     </row>
     <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B24" s="17">
         <v>44.314844000000001</v>
@@ -41732,7 +41942,7 @@
     </row>
     <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B25" s="17">
         <v>46.729553000000003</v>
@@ -41746,7 +41956,7 @@
     </row>
     <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B26" s="17">
         <v>32.354667999999997</v>
@@ -41760,7 +41970,7 @@
     </row>
     <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B27" s="17">
         <v>37.964252999999999</v>
@@ -41774,7 +41984,7 @@
     </row>
     <row r="28" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B28" s="17">
         <v>46.879682000000003</v>
@@ -41788,7 +41998,7 @@
     </row>
     <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B29" s="17">
         <v>41.492536999999999</v>
@@ -41802,7 +42012,7 @@
     </row>
     <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B30" s="17">
         <v>38.802610000000001</v>
@@ -41816,7 +42026,7 @@
     </row>
     <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B31" s="17">
         <v>43.193852</v>
@@ -41830,7 +42040,7 @@
     </row>
     <row r="32" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B32" s="17">
         <v>40.058323999999999</v>
@@ -41844,7 +42054,7 @@
     </row>
     <row r="33" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B33" s="17">
         <v>34.972729999999999</v>
@@ -41858,7 +42068,7 @@
     </row>
     <row r="34" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B34" s="17">
         <v>43.299427999999999</v>
@@ -41872,7 +42082,7 @@
     </row>
     <row r="35" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B35" s="17">
         <v>35.759573000000003</v>
@@ -41886,7 +42096,7 @@
     </row>
     <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B36" s="17">
         <v>47.551493000000001</v>
@@ -41900,7 +42110,7 @@
     </row>
     <row r="37" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B37" s="17">
         <v>40.417287000000002</v>
@@ -41914,7 +42124,7 @@
     </row>
     <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B38" s="17">
         <v>35.007752000000004</v>
@@ -41928,7 +42138,7 @@
     </row>
     <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B39" s="17">
         <v>43.804133</v>
@@ -41942,7 +42152,7 @@
     </row>
     <row r="40" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B40" s="17">
         <v>41.203322</v>
@@ -41956,7 +42166,7 @@
     </row>
     <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B41" s="17">
         <v>18.220832999999999</v>
@@ -41965,12 +42175,12 @@
         <v>-66.590148999999997</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B42" s="17">
         <v>41.580095</v>
@@ -41984,7 +42194,7 @@
     </row>
     <row r="43" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B43" s="17">
         <v>33.836081</v>
@@ -41998,7 +42208,7 @@
     </row>
     <row r="44" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B44" s="17">
         <v>43.969515000000001</v>
@@ -42012,7 +42222,7 @@
     </row>
     <row r="45" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B45" s="17">
         <v>35.517491</v>
@@ -42026,7 +42236,7 @@
     </row>
     <row r="46" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B46" s="17">
         <v>31.968599000000001</v>
@@ -42040,7 +42250,7 @@
     </row>
     <row r="47" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B47" s="17">
         <v>39.320979999999999</v>
@@ -42054,7 +42264,7 @@
     </row>
     <row r="48" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B48" s="17">
         <v>44.558802999999997</v>
@@ -42068,7 +42278,7 @@
     </row>
     <row r="49" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B49" s="17">
         <v>37.431573</v>
@@ -42082,7 +42292,7 @@
     </row>
     <row r="50" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B50" s="17">
         <v>47.751074000000003</v>
@@ -42096,7 +42306,7 @@
     </row>
     <row r="51" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B51" s="17">
         <v>38.597625999999998</v>
@@ -42110,7 +42320,7 @@
     </row>
     <row r="52" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B52" s="17">
         <v>43.784439999999996</v>
@@ -42124,7 +42334,7 @@
     </row>
     <row r="53" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B53" s="17">
         <v>43.075968000000003</v>

</xml_diff>